<commit_message>
Accuracy calculations after collision
</commit_message>
<xml_diff>
--- a/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
+++ b/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anderssandstrom/ecmc_bifrost_vac_tank_sat/docs/testplan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federicorojas/ecmc_bifrost_vac_tank_sat/docs/testplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38649EA-5FEF-3C46-83BB-612BD7FCF9DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE262FA3-E382-6342-878C-A941B1455E5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="520" windowWidth="27800" windowHeight="20660" activeTab="5" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="5" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="15" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="189">
   <si>
     <t>General Inspection</t>
   </si>
@@ -576,9 +576,6 @@
     <t>hardstop high</t>
   </si>
   <si>
-    <t>10.98</t>
-  </si>
-  <si>
     <t>-5,0177</t>
   </si>
   <si>
@@ -666,32 +663,53 @@
     <t>OL diff abs</t>
   </si>
   <si>
-    <t>After collision</t>
-  </si>
-  <si>
-    <t>BELOW AFTER COLLISION</t>
+    <t>-5,0111989056</t>
+  </si>
+  <si>
+    <t>-5,00433206</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -0,01192673350</t>
+  </si>
+  <si>
+    <t>0,00093083603</t>
+  </si>
+  <si>
+    <t>4,98733404692</t>
+  </si>
+  <si>
+    <t>4,973383869</t>
+  </si>
+  <si>
+    <t>9,986606220</t>
+  </si>
+  <si>
+    <t>9,97811254950</t>
+  </si>
+  <si>
+    <t>34,9829722023</t>
+  </si>
+  <si>
+    <t>34,9762915</t>
+  </si>
+  <si>
+    <t>44,9815165474</t>
+  </si>
+  <si>
+    <t>44,990913043</t>
+  </si>
+  <si>
+    <t>AFTER COLLISION</t>
   </si>
   <si>
     <t>BEFORE COLLISION</t>
-  </si>
-  <si>
-    <t>Gear ratio DIFF (before vs after collision)</t>
-  </si>
-  <si>
-    <t>Open loop</t>
-  </si>
-  <si>
-    <t>posital</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-  </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -791,31 +809,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="12"/>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -860,12 +856,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="56">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -1568,11 +1564,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1776,89 +1785,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4465,27 +4429,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CEB521-8DC8-0C48-A601-3238D1EFF0A3}">
-  <dimension ref="B2:Z62"/>
+  <dimension ref="A2:Z60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O51" sqref="O51"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="13.6640625" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>109</v>
       </c>
@@ -4493,7 +4453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>96</v>
       </c>
@@ -4504,13 +4464,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="2:26" s="146" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="150" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="158" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="158" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>124</v>
       </c>
@@ -4523,24 +4483,24 @@
       <c r="E7" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="134" t="s">
-        <v>175</v>
+      <c r="F7" s="138" t="s">
+        <v>174</v>
       </c>
       <c r="G7" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="H7" s="101" t="s">
-        <v>174</v>
-      </c>
-      <c r="I7" s="133"/>
-      <c r="J7" s="133"/>
-      <c r="K7" s="133"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="135"/>
-      <c r="N7" s="135"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="135"/>
+      <c r="H7" s="137" t="s">
+        <v>173</v>
+      </c>
+      <c r="I7" s="137"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="137"/>
+      <c r="L7" s="137"/>
+      <c r="M7" s="154"/>
+      <c r="N7" s="154"/>
+      <c r="O7" s="154"/>
+      <c r="P7" s="154"/>
+      <c r="Q7" s="154"/>
       <c r="S7" s="91" t="s">
         <v>100</v>
       </c>
@@ -4554,36 +4514,36 @@
       <c r="Y7" s="92"/>
       <c r="Z7" s="93"/>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="C8" s="128" t="s">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="C8" s="129" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="129">
+      <c r="D8" s="130">
         <v>-10.98</v>
       </c>
-      <c r="E8" s="129">
+      <c r="E8" s="130">
         <v>-10.978210375023499</v>
       </c>
-      <c r="F8" s="129">
+      <c r="F8" s="130">
         <f>ABS(D8-E8)</f>
         <v>1.7896249765012584E-3</v>
       </c>
-      <c r="G8" s="129">
+      <c r="G8" s="130">
         <v>-10.974417235955199</v>
       </c>
-      <c r="H8" s="130">
+      <c r="H8" s="137">
         <f>ABS(D8-G8)</f>
         <v>5.5827640448011806E-3</v>
       </c>
-      <c r="I8" s="133"/>
-      <c r="J8" s="133"/>
-      <c r="K8" s="133"/>
-      <c r="L8" s="133"/>
-      <c r="M8" s="133"/>
-      <c r="N8" s="133"/>
-      <c r="O8" s="133"/>
-      <c r="P8" s="133"/>
-      <c r="Q8" s="133"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="137"/>
+      <c r="K8" s="137"/>
+      <c r="L8" s="137"/>
+      <c r="M8" s="137"/>
+      <c r="N8" s="137"/>
+      <c r="O8" s="137"/>
+      <c r="P8" s="137"/>
+      <c r="Q8" s="137"/>
       <c r="S8" s="124"/>
       <c r="T8" s="125"/>
       <c r="U8" s="125"/>
@@ -4593,36 +4553,36 @@
       <c r="Y8" s="125"/>
       <c r="Z8" s="126"/>
     </row>
-    <row r="9" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="127">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="C9" s="128">
         <v>-5</v>
       </c>
-      <c r="D9" s="192" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" s="192">
+      <c r="D9" s="132" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="132">
         <v>-5.0096773753587298</v>
       </c>
-      <c r="F9" s="193">
+      <c r="F9" s="130">
         <f t="shared" ref="F9:F19" si="0">ABS(D9-E9)</f>
         <v>8.0226246412697932E-3</v>
       </c>
-      <c r="G9" s="192">
+      <c r="G9" s="132">
         <v>-5.0102009745677902</v>
       </c>
-      <c r="H9" s="197">
+      <c r="H9" s="137">
         <f t="shared" ref="H9:H19" si="1">ABS(D9-G9)</f>
         <v>7.4990254322093719E-3</v>
       </c>
-      <c r="I9" s="131"/>
-      <c r="J9" s="131"/>
-      <c r="K9" s="132"/>
-      <c r="L9" s="132"/>
-      <c r="M9" s="136"/>
-      <c r="N9" s="137"/>
-      <c r="O9" s="137"/>
-      <c r="P9" s="137"/>
-      <c r="Q9" s="137"/>
+      <c r="I9" s="133"/>
+      <c r="J9" s="133"/>
+      <c r="K9" s="134"/>
+      <c r="L9" s="134"/>
+      <c r="M9" s="155"/>
+      <c r="N9" s="156"/>
+      <c r="O9" s="156"/>
+      <c r="P9" s="156"/>
+      <c r="Q9" s="156"/>
       <c r="S9" s="95">
         <v>5</v>
       </c>
@@ -4634,42 +4594,42 @@
       <c r="Y9" s="94"/>
       <c r="Z9" s="96"/>
     </row>
-    <row r="10" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C10" s="87">
         <v>0</v>
       </c>
-      <c r="D10" s="194">
+      <c r="D10" s="53">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="E10" s="194">
+      <c r="E10" s="132">
         <v>-8.1487286875825005E-3</v>
       </c>
-      <c r="F10" s="193">
+      <c r="F10" s="130">
         <f t="shared" si="0"/>
         <v>2.7348728687582501E-2</v>
       </c>
-      <c r="G10" s="194">
+      <c r="G10" s="132">
         <v>-1.17485980349982E-2</v>
       </c>
-      <c r="H10" s="197">
+      <c r="H10" s="137">
         <f t="shared" si="1"/>
         <v>3.09485980349982E-2</v>
       </c>
-      <c r="I10" s="131"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="132"/>
-      <c r="L10" s="143"/>
-      <c r="M10" s="142" t="s">
-        <v>173</v>
-      </c>
-      <c r="N10" s="140" t="s">
-        <v>166</v>
-      </c>
-      <c r="O10" s="141" t="s">
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
+      <c r="K10" s="134"/>
+      <c r="L10" s="134"/>
+      <c r="M10" s="134" t="s">
+        <v>172</v>
+      </c>
+      <c r="N10" s="134" t="s">
+        <v>165</v>
+      </c>
+      <c r="O10" s="134" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="132"/>
-      <c r="Q10" s="132"/>
+      <c r="P10" s="134"/>
+      <c r="Q10" s="134"/>
       <c r="S10" s="95"/>
       <c r="T10" s="94"/>
       <c r="U10" s="94"/>
@@ -4679,45 +4639,45 @@
       <c r="Y10" s="94"/>
       <c r="Z10" s="96"/>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C11" s="87">
         <v>5</v>
       </c>
-      <c r="D11" s="194">
+      <c r="D11" s="53">
         <v>4.9862000000000002</v>
       </c>
-      <c r="E11" s="194">
+      <c r="E11" s="132">
         <v>4.9933787789488502</v>
       </c>
-      <c r="F11" s="193">
+      <c r="F11" s="130">
         <f t="shared" si="0"/>
         <v>7.1787789488499953E-3</v>
       </c>
-      <c r="G11" s="194">
+      <c r="G11" s="132">
         <v>4.9956060588578</v>
       </c>
-      <c r="H11" s="197">
+      <c r="H11" s="137">
         <f t="shared" si="1"/>
         <v>9.4060588577997706E-3</v>
       </c>
-      <c r="I11" s="131"/>
-      <c r="J11" s="131"/>
-      <c r="K11" s="132"/>
-      <c r="L11" s="144" t="s">
-        <v>171</v>
-      </c>
-      <c r="M11" s="103">
+      <c r="I11" s="133"/>
+      <c r="J11" s="133"/>
+      <c r="K11" s="134"/>
+      <c r="L11" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="M11" s="134">
         <v>8.1041246399999998E-5</v>
       </c>
-      <c r="N11" s="189">
+      <c r="N11" s="134">
         <v>-8.1453097600000003E-3</v>
       </c>
-      <c r="O11" s="187">
+      <c r="O11" s="134">
         <f>MAX(F9:F19)</f>
         <v>2.7348728687582501E-2</v>
       </c>
-      <c r="P11" s="132"/>
-      <c r="Q11" s="132"/>
+      <c r="P11" s="134"/>
+      <c r="Q11" s="134"/>
       <c r="S11" s="95"/>
       <c r="T11" s="94"/>
       <c r="U11" s="94"/>
@@ -4727,45 +4687,45 @@
       <c r="Y11" s="94"/>
       <c r="Z11" s="96"/>
     </row>
-    <row r="12" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C12" s="87">
         <v>10</v>
       </c>
-      <c r="D12" s="194">
+      <c r="D12" s="53">
         <v>9.9887999999999995</v>
       </c>
-      <c r="E12" s="194">
+      <c r="E12" s="132">
         <v>9.9949074254174004</v>
       </c>
-      <c r="F12" s="193">
+      <c r="F12" s="130">
         <f t="shared" si="0"/>
         <v>6.1074254174009468E-3</v>
       </c>
-      <c r="G12" s="194">
+      <c r="G12" s="132">
         <v>9.9986431097759993</v>
       </c>
-      <c r="H12" s="197">
+      <c r="H12" s="137">
         <f t="shared" si="1"/>
         <v>9.843109775999892E-3</v>
       </c>
-      <c r="I12" s="131"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="132"/>
-      <c r="L12" s="145" t="s">
-        <v>172</v>
-      </c>
-      <c r="M12" s="56">
+      <c r="I12" s="133"/>
+      <c r="J12" s="133"/>
+      <c r="K12" s="134"/>
+      <c r="L12" s="134" t="s">
+        <v>171</v>
+      </c>
+      <c r="M12" s="134">
         <v>-4.4511401799999998E-5</v>
       </c>
-      <c r="N12" s="191">
+      <c r="N12" s="134">
         <v>30.7267127</v>
       </c>
-      <c r="O12" s="188">
+      <c r="O12" s="134">
         <f>MAX(H9:H19)</f>
         <v>3.09485980349982E-2</v>
       </c>
-      <c r="P12" s="132"/>
-      <c r="Q12" s="132"/>
+      <c r="P12" s="134"/>
+      <c r="Q12" s="134"/>
       <c r="S12" s="95"/>
       <c r="T12" s="94"/>
       <c r="U12" s="94"/>
@@ -4775,36 +4735,36 @@
       <c r="Y12" s="94"/>
       <c r="Z12" s="96"/>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C13" s="87">
         <v>15</v>
       </c>
-      <c r="D13" s="194">
+      <c r="D13" s="53">
         <v>14.989699999999999</v>
       </c>
-      <c r="E13" s="194">
+      <c r="E13" s="132">
         <v>14.9964355029764</v>
       </c>
-      <c r="F13" s="193">
+      <c r="F13" s="130">
         <f t="shared" si="0"/>
         <v>6.7355029764009089E-3</v>
       </c>
-      <c r="G13" s="194">
+      <c r="G13" s="132">
         <v>15.0015911378906</v>
       </c>
-      <c r="H13" s="197">
+      <c r="H13" s="137">
         <f t="shared" si="1"/>
         <v>1.1891137890600589E-2</v>
       </c>
-      <c r="I13" s="131"/>
-      <c r="J13" s="131"/>
-      <c r="K13" s="132"/>
-      <c r="L13" s="132"/>
-      <c r="M13" s="132"/>
-      <c r="N13" s="132"/>
-      <c r="O13" s="132"/>
-      <c r="P13" s="132"/>
-      <c r="Q13" s="132"/>
+      <c r="I13" s="133"/>
+      <c r="J13" s="133"/>
+      <c r="K13" s="134"/>
+      <c r="L13" s="134"/>
+      <c r="M13" s="134"/>
+      <c r="N13" s="134"/>
+      <c r="O13" s="134"/>
+      <c r="P13" s="134"/>
+      <c r="Q13" s="134"/>
       <c r="S13" s="95"/>
       <c r="T13" s="94"/>
       <c r="U13" s="94"/>
@@ -4814,36 +4774,36 @@
       <c r="Y13" s="94"/>
       <c r="Z13" s="96"/>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C14" s="87">
         <v>20</v>
       </c>
-      <c r="D14" s="195">
+      <c r="D14" s="111">
         <v>19.995100000000001</v>
       </c>
-      <c r="E14" s="195">
+      <c r="E14" s="132">
         <v>19.997963580535298</v>
       </c>
-      <c r="F14" s="193">
+      <c r="F14" s="130">
         <f t="shared" si="0"/>
         <v>2.8635805352976718E-3</v>
       </c>
-      <c r="G14" s="195">
+      <c r="G14" s="132">
         <v>19.997906967136899</v>
       </c>
-      <c r="H14" s="197">
+      <c r="H14" s="137">
         <f t="shared" si="1"/>
         <v>2.8069671368982085E-3</v>
       </c>
-      <c r="I14" s="131"/>
-      <c r="J14" s="131"/>
-      <c r="K14" s="132"/>
-      <c r="L14" s="132"/>
-      <c r="M14" s="132"/>
-      <c r="N14" s="132"/>
-      <c r="O14" s="132"/>
-      <c r="P14" s="132"/>
-      <c r="Q14" s="132"/>
+      <c r="I14" s="133"/>
+      <c r="J14" s="133"/>
+      <c r="K14" s="134"/>
+      <c r="L14" s="134"/>
+      <c r="M14" s="134"/>
+      <c r="N14" s="134"/>
+      <c r="O14" s="134"/>
+      <c r="P14" s="134"/>
+      <c r="Q14" s="134"/>
       <c r="S14" s="95"/>
       <c r="T14" s="94"/>
       <c r="U14" s="94"/>
@@ -4853,36 +4813,36 @@
       <c r="Y14" s="94"/>
       <c r="Z14" s="96"/>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C15" s="87">
         <v>25</v>
       </c>
-      <c r="D15" s="194">
+      <c r="D15" s="53">
         <v>24.9998</v>
       </c>
-      <c r="E15" s="194">
+      <c r="E15" s="132">
         <v>24.9994916580943</v>
       </c>
-      <c r="F15" s="193">
+      <c r="F15" s="130">
         <f t="shared" si="0"/>
         <v>3.0834190570061537E-4</v>
       </c>
-      <c r="G15" s="194">
+      <c r="G15" s="132">
         <v>24.997071526098601</v>
       </c>
-      <c r="H15" s="197">
+      <c r="H15" s="137">
         <f t="shared" si="1"/>
         <v>2.7284739013992976E-3</v>
       </c>
-      <c r="I15" s="131"/>
-      <c r="J15" s="131"/>
-      <c r="K15" s="132"/>
-      <c r="L15" s="132"/>
-      <c r="M15" s="132"/>
-      <c r="N15" s="132"/>
-      <c r="O15" s="132"/>
-      <c r="P15" s="132"/>
-      <c r="Q15" s="132"/>
+      <c r="I15" s="133"/>
+      <c r="J15" s="133"/>
+      <c r="K15" s="134"/>
+      <c r="L15" s="134"/>
+      <c r="M15" s="134"/>
+      <c r="N15" s="134"/>
+      <c r="O15" s="134"/>
+      <c r="P15" s="134"/>
+      <c r="Q15" s="134"/>
       <c r="S15" s="95"/>
       <c r="T15" s="94"/>
       <c r="U15" s="94"/>
@@ -4892,36 +4852,36 @@
       <c r="Y15" s="94"/>
       <c r="Z15" s="96"/>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C16" s="87">
         <v>30</v>
       </c>
-      <c r="D16" s="194">
+      <c r="D16" s="53">
         <v>29.996500000000001</v>
       </c>
-      <c r="E16" s="194">
+      <c r="E16" s="132">
         <v>30.001019735653301</v>
       </c>
-      <c r="F16" s="193">
+      <c r="F16" s="130">
         <f t="shared" si="0"/>
         <v>4.5197356533002164E-3</v>
       </c>
-      <c r="G16" s="194">
+      <c r="G16" s="132">
         <v>29.995123300015202</v>
       </c>
-      <c r="H16" s="197">
+      <c r="H16" s="137">
         <f t="shared" si="1"/>
         <v>1.376699984799501E-3</v>
       </c>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
-      <c r="K16" s="132"/>
-      <c r="L16" s="132"/>
-      <c r="M16" s="132"/>
-      <c r="N16" s="132"/>
-      <c r="O16" s="132"/>
-      <c r="P16" s="132"/>
-      <c r="Q16" s="132"/>
+      <c r="I16" s="133"/>
+      <c r="J16" s="133"/>
+      <c r="K16" s="134"/>
+      <c r="L16" s="134"/>
+      <c r="M16" s="134"/>
+      <c r="N16" s="134"/>
+      <c r="O16" s="134"/>
+      <c r="P16" s="134"/>
+      <c r="Q16" s="134"/>
       <c r="S16" s="95"/>
       <c r="T16" s="94"/>
       <c r="U16" s="94"/>
@@ -4931,36 +4891,36 @@
       <c r="Y16" s="94"/>
       <c r="Z16" s="96"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C17" s="87">
         <v>35</v>
       </c>
-      <c r="D17" s="194">
+      <c r="D17" s="53">
         <v>35.000500000000002</v>
       </c>
-      <c r="E17" s="194">
+      <c r="E17" s="132">
         <v>35.002548380501104</v>
       </c>
-      <c r="F17" s="193">
+      <c r="F17" s="130">
         <f t="shared" si="0"/>
         <v>2.0483805011011214E-3</v>
       </c>
-      <c r="G17" s="194">
+      <c r="G17" s="132">
         <v>34.997359145700898</v>
       </c>
-      <c r="H17" s="197">
+      <c r="H17" s="137">
         <f t="shared" si="1"/>
         <v>3.1408542991044897E-3</v>
       </c>
-      <c r="I17" s="131"/>
-      <c r="J17" s="131"/>
-      <c r="K17" s="132"/>
-      <c r="L17" s="132"/>
-      <c r="M17" s="132"/>
-      <c r="N17" s="132"/>
-      <c r="O17" s="132"/>
-      <c r="P17" s="132"/>
-      <c r="Q17" s="132"/>
+      <c r="I17" s="133"/>
+      <c r="J17" s="133"/>
+      <c r="K17" s="134"/>
+      <c r="L17" s="134"/>
+      <c r="M17" s="134"/>
+      <c r="N17" s="134"/>
+      <c r="O17" s="134"/>
+      <c r="P17" s="134"/>
+      <c r="Q17" s="134"/>
       <c r="S17" s="95"/>
       <c r="T17" s="94"/>
       <c r="U17" s="94"/>
@@ -4970,35 +4930,35 @@
       <c r="Y17" s="94"/>
       <c r="Z17" s="96"/>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C18" s="90">
         <v>40</v>
       </c>
-      <c r="D18" s="196">
+      <c r="D18" s="127">
         <v>40.009500000000003</v>
       </c>
-      <c r="E18" s="196">
+      <c r="E18" s="132">
         <v>40.004076458060098</v>
       </c>
-      <c r="F18" s="193">
+      <c r="F18" s="130">
         <f t="shared" si="0"/>
         <v>5.4235419399049078E-3</v>
       </c>
-      <c r="G18" s="196">
+      <c r="G18" s="132">
         <v>40.004891848200899</v>
       </c>
-      <c r="H18" s="197">
+      <c r="H18" s="137">
         <f t="shared" si="1"/>
         <v>4.608151799104121E-3</v>
       </c>
-      <c r="I18" s="131"/>
-      <c r="J18" s="131"/>
-      <c r="L18" s="132"/>
-      <c r="M18" s="132"/>
-      <c r="N18" s="132"/>
-      <c r="O18" s="132"/>
-      <c r="P18" s="132"/>
-      <c r="Q18" s="132"/>
+      <c r="I18" s="133"/>
+      <c r="J18" s="133"/>
+      <c r="L18" s="134"/>
+      <c r="M18" s="134"/>
+      <c r="N18" s="134"/>
+      <c r="O18" s="134"/>
+      <c r="P18" s="134"/>
+      <c r="Q18" s="134"/>
       <c r="S18" s="95"/>
       <c r="T18" s="94"/>
       <c r="U18" s="94"/>
@@ -5008,36 +4968,36 @@
       <c r="Y18" s="94"/>
       <c r="Z18" s="96"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C19" s="90">
         <v>45</v>
       </c>
-      <c r="D19" s="196">
+      <c r="D19" s="127">
         <v>45.012700000000002</v>
       </c>
-      <c r="E19" s="196">
+      <c r="E19" s="132">
         <v>45.005604535619099</v>
       </c>
-      <c r="F19" s="193">
+      <c r="F19" s="130">
         <f t="shared" si="0"/>
         <v>7.0954643809031381E-3</v>
       </c>
-      <c r="G19" s="196">
+      <c r="G19" s="132">
         <v>45.0113562770578</v>
       </c>
-      <c r="H19" s="197">
+      <c r="H19" s="137">
         <f t="shared" si="1"/>
         <v>1.3437229422024188E-3</v>
       </c>
-      <c r="I19" s="131"/>
-      <c r="J19" s="131"/>
-      <c r="K19" s="132"/>
-      <c r="L19" s="132"/>
-      <c r="M19" s="132"/>
-      <c r="N19" s="132"/>
-      <c r="O19" s="132"/>
-      <c r="P19" s="132"/>
-      <c r="Q19" s="132"/>
+      <c r="I19" s="133"/>
+      <c r="J19" s="133"/>
+      <c r="K19" s="134"/>
+      <c r="L19" s="134"/>
+      <c r="M19" s="134"/>
+      <c r="N19" s="134"/>
+      <c r="O19" s="134"/>
+      <c r="P19" s="134"/>
+      <c r="Q19" s="134"/>
       <c r="S19" s="95"/>
       <c r="T19" s="94"/>
       <c r="U19" s="94"/>
@@ -5047,26 +5007,26 @@
       <c r="Y19" s="94"/>
       <c r="Z19" s="96"/>
     </row>
-    <row r="20" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="D20" s="190">
+      <c r="D20" s="56">
         <v>48.5</v>
       </c>
-      <c r="E20" s="190"/>
-      <c r="F20" s="198"/>
-      <c r="G20" s="190"/>
-      <c r="H20" s="199"/>
-      <c r="I20" s="132"/>
-      <c r="J20" s="132"/>
-      <c r="K20" s="132"/>
-      <c r="L20" s="132"/>
-      <c r="M20" s="132"/>
-      <c r="N20" s="132"/>
-      <c r="O20" s="132"/>
-      <c r="P20" s="132"/>
-      <c r="Q20" s="132"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="157"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="134"/>
+      <c r="I20" s="134"/>
+      <c r="J20" s="134"/>
+      <c r="K20" s="134"/>
+      <c r="L20" s="134"/>
+      <c r="M20" s="134"/>
+      <c r="N20" s="134"/>
+      <c r="O20" s="134"/>
+      <c r="P20" s="134"/>
+      <c r="Q20" s="134"/>
       <c r="S20" s="95"/>
       <c r="T20" s="94"/>
       <c r="U20" s="94"/>
@@ -5076,10 +5036,10 @@
       <c r="Y20" s="94"/>
       <c r="Z20" s="96"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:26" x14ac:dyDescent="0.2">
       <c r="R21" s="95"/>
       <c r="S21" s="94" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T21" s="94"/>
       <c r="U21" s="94"/>
@@ -5088,22 +5048,17 @@
       <c r="X21" s="94"/>
       <c r="Y21" s="96"/>
     </row>
-    <row r="22" spans="2:26" s="146" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="150" t="s">
-        <v>177</v>
-      </c>
-      <c r="R22" s="147"/>
-      <c r="S22" s="148"/>
-      <c r="T22" s="148"/>
-      <c r="U22" s="148"/>
-      <c r="V22" s="148"/>
-      <c r="W22" s="148"/>
-      <c r="X22" s="148"/>
-      <c r="Y22" s="149"/>
-    </row>
-    <row r="23" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="R22" s="95"/>
+      <c r="S22" s="94"/>
+      <c r="T22" s="94"/>
+      <c r="U22" s="94"/>
+      <c r="V22" s="94"/>
+      <c r="W22" s="94"/>
+      <c r="X22" s="94"/>
+      <c r="Y22" s="96"/>
+    </row>
+    <row r="23" spans="3:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R23" s="97"/>
       <c r="S23" s="98"/>
       <c r="T23" s="98"/>
@@ -5113,536 +5068,537 @@
       <c r="X23" s="98"/>
       <c r="Y23" s="99"/>
     </row>
-    <row r="24" spans="2:26" s="151" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="151" t="s">
+    <row r="24" spans="3:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="3:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="104" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="102" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="140" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="142" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="138"/>
+      <c r="H25" s="101"/>
+      <c r="I25" s="149"/>
+      <c r="J25" s="149"/>
+      <c r="K25" s="140"/>
+      <c r="L25" s="104" t="s">
+        <v>108</v>
+      </c>
+      <c r="M25" s="101"/>
+      <c r="N25" s="101"/>
+      <c r="O25" s="101"/>
+      <c r="P25" s="152"/>
+      <c r="Q25" s="153"/>
+    </row>
+    <row r="26" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C26" s="129" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="130">
+        <v>10.98</v>
+      </c>
+      <c r="E26" s="139"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="139" t="s">
+        <v>165</v>
+      </c>
+      <c r="H26" s="131" t="s">
+        <v>164</v>
+      </c>
+      <c r="I26" s="150" t="s">
+        <v>122</v>
+      </c>
+      <c r="J26" s="150" t="s">
+        <v>169</v>
+      </c>
+      <c r="K26" s="141"/>
+      <c r="L26" s="148"/>
+      <c r="M26" s="131" t="s">
+        <v>166</v>
+      </c>
+      <c r="N26" s="131" t="s">
+        <v>165</v>
+      </c>
+      <c r="O26" s="131" t="s">
+        <v>167</v>
+      </c>
+      <c r="P26" s="151" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q26" s="151" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C27" s="128">
+        <v>-5</v>
+      </c>
+      <c r="D27" s="132" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="25" spans="2:26" s="151" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="152" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="153" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="154" t="s">
-        <v>164</v>
-      </c>
-      <c r="F25" s="155" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="156"/>
-      <c r="H25" s="157"/>
-      <c r="I25" s="158"/>
-      <c r="J25" s="158"/>
-      <c r="K25" s="154"/>
-      <c r="L25" s="152" t="s">
-        <v>108</v>
-      </c>
-      <c r="M25" s="157"/>
-      <c r="N25" s="157"/>
-      <c r="O25" s="157"/>
-      <c r="P25" s="159"/>
-      <c r="Q25" s="160"/>
-    </row>
-    <row r="26" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="161" t="s">
-        <v>144</v>
-      </c>
-      <c r="D26" s="162" t="s">
-        <v>146</v>
-      </c>
-      <c r="E26" s="163"/>
-      <c r="F26" s="161"/>
-      <c r="G26" s="163" t="s">
-        <v>166</v>
-      </c>
-      <c r="H26" s="164" t="s">
-        <v>165</v>
-      </c>
-      <c r="I26" s="165" t="s">
-        <v>122</v>
-      </c>
-      <c r="J26" s="165" t="s">
-        <v>170</v>
-      </c>
-      <c r="K26" s="166"/>
-      <c r="L26" s="167"/>
-      <c r="M26" s="164" t="s">
-        <v>167</v>
-      </c>
-      <c r="N26" s="164" t="s">
-        <v>166</v>
-      </c>
-      <c r="O26" s="164" t="s">
-        <v>168</v>
-      </c>
-      <c r="P26" s="168" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q26" s="168" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="169">
-        <v>-5</v>
-      </c>
-      <c r="D27" s="170" t="s">
-        <v>162</v>
-      </c>
-      <c r="E27" s="171"/>
-      <c r="F27" s="172">
+      <c r="E27" s="133"/>
+      <c r="F27" s="143">
         <v>-58415.730470000002</v>
       </c>
-      <c r="G27" s="173">
+      <c r="G27" s="134">
         <f>F27-$F$28</f>
         <v>-61715.791369999999</v>
       </c>
-      <c r="H27" s="174">
+      <c r="H27" s="144">
         <f>D27/G27</f>
         <v>8.1044087566076682E-5</v>
       </c>
-      <c r="I27" s="174">
+      <c r="I27" s="144">
         <f>(G27)*$H$39</f>
         <v>-4.9915767788996455</v>
       </c>
-      <c r="J27" s="174">
+      <c r="J27" s="144">
         <f>D27-I27</f>
         <v>-1.0123221100354129E-2</v>
       </c>
-      <c r="L27" s="172">
+      <c r="L27" s="143">
         <v>802915</v>
       </c>
-      <c r="M27" s="173">
+      <c r="M27" s="134">
         <f>L27</f>
         <v>802915</v>
       </c>
-      <c r="N27" s="173">
+      <c r="N27" s="134">
         <f>M27-$M$28</f>
         <v>112432</v>
       </c>
-      <c r="O27" s="174">
+      <c r="O27" s="144">
         <f>D27/N27</f>
         <v>-4.448644514017361E-5</v>
       </c>
-      <c r="P27" s="173">
+      <c r="P27" s="134">
         <f>N27*$O$39</f>
         <v>-5.0045048311745859</v>
       </c>
-      <c r="Q27" s="174">
+      <c r="Q27" s="144">
         <f>D27-P27</f>
         <v>2.8048311745862975E-3</v>
       </c>
     </row>
-    <row r="28" spans="2:26" s="151" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="C28" s="175">
+    <row r="28" spans="3:26" ht="51" x14ac:dyDescent="0.2">
+      <c r="C28" s="87">
         <v>0</v>
       </c>
-      <c r="D28" s="176">
+      <c r="D28" s="53">
         <v>0</v>
       </c>
-      <c r="E28" s="177" t="s">
-        <v>163</v>
-      </c>
-      <c r="F28" s="172">
+      <c r="E28" s="136" t="s">
+        <v>162</v>
+      </c>
+      <c r="F28" s="143">
         <v>3300.0608999999999</v>
       </c>
-      <c r="G28" s="173">
+      <c r="G28" s="134">
         <f>F28-$F$28</f>
         <v>0</v>
       </c>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174">
+      <c r="H28" s="144"/>
+      <c r="I28" s="144">
         <f>(G28)*$H$39</f>
         <v>0</v>
       </c>
-      <c r="J28" s="174">
+      <c r="J28" s="144">
         <f>D28-I28</f>
         <v>0</v>
       </c>
-      <c r="L28" s="172">
+      <c r="L28" s="143">
         <v>690483</v>
       </c>
-      <c r="M28" s="173">
+      <c r="M28" s="134">
         <f>L28</f>
         <v>690483</v>
       </c>
-      <c r="N28" s="173">
+      <c r="N28" s="134">
         <f>M28-$M$28</f>
         <v>0</v>
       </c>
-      <c r="O28" s="174"/>
-      <c r="P28" s="173">
+      <c r="O28" s="144"/>
+      <c r="P28" s="134">
         <f>N28*$O$39</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="174"/>
-    </row>
-    <row r="29" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="175">
+      <c r="Q28" s="144"/>
+    </row>
+    <row r="29" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C29" s="87">
         <v>5</v>
       </c>
-      <c r="D29" s="176">
+      <c r="D29" s="53">
         <v>4.9725000000000001</v>
       </c>
-      <c r="E29" s="173"/>
-      <c r="F29" s="172">
+      <c r="E29" s="134"/>
+      <c r="F29" s="143">
         <v>65015.796090000003</v>
       </c>
-      <c r="G29" s="173">
+      <c r="G29" s="134">
         <f>F29-$F$28</f>
         <v>61715.735190000007</v>
       </c>
-      <c r="H29" s="174">
+      <c r="H29" s="144">
         <f>D29/G29</f>
         <v>8.0571024305090179E-5</v>
       </c>
-      <c r="I29" s="174">
+      <c r="I29" s="144">
         <f>(G29)*$H$39</f>
         <v>4.9915722350579932</v>
       </c>
-      <c r="J29" s="174">
+      <c r="J29" s="144">
         <f>D29-I29</f>
         <v>-1.9072235057993048E-2</v>
       </c>
-      <c r="L29" s="172">
+      <c r="L29" s="143">
         <v>578788</v>
       </c>
-      <c r="M29" s="173">
+      <c r="M29" s="134">
         <f>L29</f>
         <v>578788</v>
       </c>
-      <c r="N29" s="173">
+      <c r="N29" s="134">
         <f>M29-$M$28</f>
         <v>-111695</v>
       </c>
-      <c r="O29" s="174">
+      <c r="O29" s="144">
         <f>D29/N29</f>
         <v>-4.4518554993509113E-5</v>
       </c>
-      <c r="P29" s="173">
+      <c r="P29" s="134">
         <f>N29*$O$39</f>
         <v>4.9716999352323654</v>
       </c>
-      <c r="Q29" s="174">
+      <c r="Q29" s="144">
         <f>D29-P29</f>
         <v>8.0006476763472278E-4</v>
       </c>
     </row>
-    <row r="30" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="175">
+    <row r="30" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C30" s="87">
         <v>10</v>
       </c>
-      <c r="D30" s="176">
+      <c r="D30" s="53">
         <v>9.9755000000000003</v>
       </c>
-      <c r="E30" s="173"/>
-      <c r="F30" s="172">
+      <c r="E30" s="134"/>
+      <c r="F30" s="143">
         <v>126731.6297</v>
       </c>
-      <c r="G30" s="173">
+      <c r="G30" s="134">
         <f>F30-$F$28</f>
         <v>123431.56880000001</v>
       </c>
-      <c r="H30" s="174">
+      <c r="H30" s="144">
         <f>D30/G30</f>
         <v>8.0818060541413121E-5</v>
       </c>
-      <c r="I30" s="174">
+      <c r="I30" s="144">
         <f>(G30)*$H$39</f>
         <v>9.983152430331284</v>
       </c>
-      <c r="J30" s="174">
+      <c r="J30" s="144">
         <f>D30-I30</f>
         <v>-7.6524303312837105E-3</v>
       </c>
-      <c r="L30" s="172">
+      <c r="L30" s="143">
         <v>466368</v>
       </c>
-      <c r="M30" s="173">
+      <c r="M30" s="134">
         <f>L30</f>
         <v>466368</v>
       </c>
-      <c r="N30" s="173">
+      <c r="N30" s="134">
         <f>M30-$M$28</f>
         <v>-224115</v>
       </c>
-      <c r="O30" s="174">
+      <c r="O30" s="144">
         <f>D30/N30</f>
         <v>-4.4510630702987306E-5</v>
       </c>
-      <c r="P30" s="173">
+      <c r="P30" s="134">
         <f>N30*$O$39</f>
         <v>9.9756706297023285</v>
       </c>
-      <c r="Q30" s="174">
+      <c r="Q30" s="144">
         <f>D30-P30</f>
         <v>-1.7062970232828434E-4</v>
       </c>
     </row>
-    <row r="31" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="175">
+    <row r="31" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C31" s="87">
         <v>15</v>
       </c>
-      <c r="D31" s="176"/>
-      <c r="E31" s="173"/>
-      <c r="F31" s="172"/>
-      <c r="G31" s="173"/>
-      <c r="H31" s="174"/>
-      <c r="I31" s="174"/>
-      <c r="J31" s="174"/>
-      <c r="L31" s="172"/>
-      <c r="M31" s="173"/>
-      <c r="N31" s="173"/>
-      <c r="O31" s="174"/>
-      <c r="P31" s="173"/>
-      <c r="Q31" s="174"/>
-    </row>
-    <row r="32" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="175">
+      <c r="D31" s="53"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="143"/>
+      <c r="G31" s="134"/>
+      <c r="H31" s="144"/>
+      <c r="I31" s="144"/>
+      <c r="J31" s="144"/>
+      <c r="L31" s="143"/>
+      <c r="M31" s="134"/>
+      <c r="N31" s="134"/>
+      <c r="O31" s="144"/>
+      <c r="P31" s="134"/>
+      <c r="Q31" s="144"/>
+    </row>
+    <row r="32" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C32" s="87">
         <v>20</v>
       </c>
-      <c r="D32" s="178"/>
-      <c r="E32" s="179"/>
-      <c r="F32" s="172"/>
-      <c r="G32" s="173"/>
-      <c r="H32" s="174"/>
-      <c r="I32" s="174"/>
-      <c r="J32" s="174"/>
-      <c r="L32" s="172"/>
-      <c r="M32" s="173"/>
-      <c r="N32" s="173"/>
-      <c r="O32" s="174"/>
-      <c r="P32" s="173"/>
-      <c r="Q32" s="174"/>
-    </row>
-    <row r="33" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="175">
+      <c r="D32" s="111"/>
+      <c r="E32" s="135"/>
+      <c r="F32" s="143"/>
+      <c r="G32" s="134"/>
+      <c r="H32" s="144"/>
+      <c r="I32" s="144"/>
+      <c r="J32" s="144"/>
+      <c r="L32" s="143"/>
+      <c r="M32" s="134"/>
+      <c r="N32" s="134"/>
+      <c r="O32" s="144"/>
+      <c r="P32" s="134"/>
+      <c r="Q32" s="144"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C33" s="87">
         <v>25</v>
       </c>
-      <c r="D33" s="176"/>
-      <c r="E33" s="173"/>
-      <c r="F33" s="172"/>
-      <c r="G33" s="173"/>
-      <c r="H33" s="174"/>
-      <c r="I33" s="174"/>
-      <c r="J33" s="174"/>
-      <c r="L33" s="172"/>
-      <c r="M33" s="173"/>
-      <c r="N33" s="173"/>
-      <c r="O33" s="174"/>
-      <c r="P33" s="173"/>
-      <c r="Q33" s="174"/>
-    </row>
-    <row r="34" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="175">
+      <c r="D33" s="53"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="143"/>
+      <c r="G33" s="134"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="144"/>
+      <c r="J33" s="144"/>
+      <c r="L33" s="143"/>
+      <c r="M33" s="134"/>
+      <c r="N33" s="134"/>
+      <c r="O33" s="144"/>
+      <c r="P33" s="134"/>
+      <c r="Q33" s="144"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C34" s="87">
         <v>30</v>
       </c>
-      <c r="D34" s="176"/>
-      <c r="E34" s="173"/>
-      <c r="F34" s="172"/>
-      <c r="G34" s="173"/>
-      <c r="H34" s="174"/>
-      <c r="I34" s="174"/>
-      <c r="J34" s="174"/>
-      <c r="L34" s="172"/>
-      <c r="M34" s="173"/>
-      <c r="N34" s="173"/>
-      <c r="O34" s="174"/>
-      <c r="P34" s="173"/>
-      <c r="Q34" s="174"/>
-    </row>
-    <row r="35" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="175">
+      <c r="D34" s="53"/>
+      <c r="E34" s="134"/>
+      <c r="F34" s="143"/>
+      <c r="G34" s="134"/>
+      <c r="H34" s="144"/>
+      <c r="I34" s="144"/>
+      <c r="J34" s="144"/>
+      <c r="L34" s="143"/>
+      <c r="M34" s="134"/>
+      <c r="N34" s="134"/>
+      <c r="O34" s="144"/>
+      <c r="P34" s="134"/>
+      <c r="Q34" s="144"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C35" s="87">
         <v>35</v>
       </c>
-      <c r="D35" s="176">
+      <c r="D35" s="53">
         <v>34.9801</v>
       </c>
-      <c r="E35" s="173"/>
-      <c r="F35" s="172">
+      <c r="E35" s="134"/>
+      <c r="F35" s="143">
         <v>435310.86090000003</v>
       </c>
-      <c r="G35" s="173">
+      <c r="G35" s="134">
         <f>F35-$F$28</f>
         <v>432010.80000000005</v>
       </c>
-      <c r="H35" s="174">
+      <c r="H35" s="144">
         <f>D35/G35</f>
         <v>8.0970429442967615E-5</v>
       </c>
-      <c r="I35" s="174">
+      <c r="I35" s="144">
         <f>(G35)*$H$39</f>
         <v>34.941058514273401</v>
       </c>
-      <c r="J35" s="174">
+      <c r="J35" s="144">
         <f>D35-I35</f>
         <v>3.904148572659949E-2</v>
       </c>
-      <c r="L35" s="172">
+      <c r="L35" s="143">
         <v>2147388488</v>
       </c>
-      <c r="M35" s="173">
+      <c r="M35" s="134">
         <f>L35-2147483648</f>
         <v>-95160</v>
       </c>
-      <c r="N35" s="173">
+      <c r="N35" s="134">
         <f>M35-$M$28</f>
         <v>-785643</v>
       </c>
-      <c r="O35" s="174">
+      <c r="O35" s="144">
         <f>D35/N35</f>
         <v>-4.4524166828954117E-5</v>
       </c>
-      <c r="P35" s="173">
+      <c r="P35" s="134">
         <f>N35*$O$39</f>
         <v>34.970063585798485</v>
       </c>
-      <c r="Q35" s="174">
+      <c r="Q35" s="144">
         <f>D35-P35</f>
         <v>1.0036414201515242E-2</v>
       </c>
     </row>
-    <row r="36" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="180">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C36" s="90">
         <v>40</v>
       </c>
-      <c r="D36" s="181"/>
-      <c r="E36" s="173"/>
-      <c r="F36" s="172"/>
-      <c r="G36" s="173"/>
-      <c r="H36" s="174"/>
-      <c r="I36" s="174"/>
-      <c r="J36" s="174"/>
-      <c r="L36" s="172"/>
-      <c r="M36" s="173"/>
-      <c r="N36" s="173"/>
-      <c r="O36" s="174"/>
-      <c r="P36" s="173"/>
-      <c r="Q36" s="174"/>
-    </row>
-    <row r="37" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="180">
+      <c r="D36" s="127"/>
+      <c r="E36" s="134"/>
+      <c r="F36" s="143"/>
+      <c r="G36" s="134"/>
+      <c r="H36" s="144"/>
+      <c r="I36" s="144"/>
+      <c r="J36" s="144"/>
+      <c r="L36" s="143"/>
+      <c r="M36" s="134"/>
+      <c r="N36" s="134"/>
+      <c r="O36" s="144"/>
+      <c r="P36" s="134"/>
+      <c r="Q36" s="144"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C37" s="90">
         <v>45</v>
       </c>
-      <c r="D37" s="181">
+      <c r="D37" s="127">
         <v>44.988999999999997</v>
       </c>
-      <c r="E37" s="173"/>
-      <c r="F37" s="172">
+      <c r="E37" s="134"/>
+      <c r="F37" s="143">
         <v>558742.5281</v>
       </c>
-      <c r="G37" s="173">
+      <c r="G37" s="134">
         <f>F37-$F$28</f>
         <v>555442.46719999996</v>
       </c>
-      <c r="H37" s="174">
+      <c r="H37" s="144">
         <f>D37/G37</f>
         <v>8.0996687607972658E-5</v>
       </c>
-      <c r="I37" s="174">
+      <c r="I37" s="144">
         <f>(G37)*$H$39</f>
         <v>44.924218903202373</v>
       </c>
-      <c r="J37" s="174">
+      <c r="J37" s="144">
         <f>D37-I37</f>
         <v>6.4781096797624116E-2</v>
       </c>
-      <c r="L37" s="172">
+      <c r="L37" s="143">
         <v>2147163532</v>
       </c>
-      <c r="M37" s="173">
+      <c r="M37" s="134">
         <f>L37-2147483648</f>
         <v>-320116</v>
       </c>
-      <c r="N37" s="173">
+      <c r="N37" s="134">
         <f>M37-$M$28</f>
         <v>-1010599</v>
       </c>
-      <c r="O37" s="174">
+      <c r="O37" s="144">
         <f>D37/N37</f>
         <v>-4.4517162593669689E-5</v>
       </c>
-      <c r="P37" s="173">
+      <c r="P37" s="134">
         <f>N37*$O$39</f>
         <v>44.983168296216427</v>
       </c>
-      <c r="Q37" s="174">
+      <c r="Q37" s="144">
         <f>D37-P37</f>
         <v>5.8317037835706742E-3</v>
       </c>
     </row>
-    <row r="38" spans="3:17" s="151" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="182" t="s">
+    <row r="38" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="173"/>
-      <c r="F38" s="172"/>
-      <c r="G38" s="173"/>
-      <c r="H38" s="174"/>
-      <c r="I38" s="174"/>
-      <c r="J38" s="174"/>
-      <c r="L38" s="172"/>
-      <c r="M38" s="173"/>
-      <c r="N38" s="173"/>
-      <c r="O38" s="174"/>
-      <c r="P38" s="173"/>
-      <c r="Q38" s="174"/>
-    </row>
-    <row r="39" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="F39" s="172"/>
-      <c r="G39" s="173" t="s">
-        <v>169</v>
-      </c>
-      <c r="H39" s="174">
+      <c r="D38" s="56"/>
+      <c r="E38" s="134"/>
+      <c r="F38" s="143"/>
+      <c r="G38" s="134"/>
+      <c r="H38" s="144"/>
+      <c r="I38" s="144"/>
+      <c r="J38" s="144"/>
+      <c r="L38" s="143"/>
+      <c r="M38" s="134"/>
+      <c r="N38" s="134"/>
+      <c r="O38" s="144"/>
+      <c r="P38" s="134"/>
+      <c r="Q38" s="144"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="F39" s="143"/>
+      <c r="G39" s="134" t="s">
+        <v>168</v>
+      </c>
+      <c r="H39" s="144">
         <f>AVERAGE(H27:H37)</f>
         <v>8.0880057892704057E-5</v>
       </c>
-      <c r="I39" s="174"/>
-      <c r="J39" s="174"/>
-      <c r="L39" s="172"/>
-      <c r="M39" s="173"/>
-      <c r="N39" s="173" t="s">
-        <v>169</v>
-      </c>
-      <c r="O39" s="174">
+      <c r="I39" s="144"/>
+      <c r="J39" s="144"/>
+      <c r="L39" s="143"/>
+      <c r="M39" s="134"/>
+      <c r="N39" s="134" t="s">
+        <v>168</v>
+      </c>
+      <c r="O39" s="144">
         <f>AVERAGE(O27:O37)</f>
         <v>-4.4511392051858772E-5</v>
       </c>
-      <c r="P39" s="173"/>
-      <c r="Q39" s="174"/>
-    </row>
-    <row r="40" spans="3:17" s="151" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F40" s="184"/>
-      <c r="G40" s="185" t="s">
-        <v>166</v>
-      </c>
-      <c r="H40" s="186">
+      <c r="P39" s="134"/>
+      <c r="Q39" s="144"/>
+    </row>
+    <row r="40" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="145"/>
+      <c r="G40" s="146" t="s">
+        <v>165</v>
+      </c>
+      <c r="H40" s="147">
         <f>-F28</f>
         <v>-3300.0608999999999</v>
       </c>
-      <c r="I40" s="186"/>
-      <c r="J40" s="186"/>
-      <c r="L40" s="184"/>
-      <c r="M40" s="185"/>
-      <c r="N40" s="185" t="s">
-        <v>166</v>
-      </c>
-      <c r="O40" s="186">
+      <c r="I40" s="147"/>
+      <c r="J40" s="147"/>
+      <c r="L40" s="145"/>
+      <c r="M40" s="146"/>
+      <c r="N40" s="146" t="s">
+        <v>165</v>
+      </c>
+      <c r="O40" s="147">
         <f>-M28</f>
         <v>-690483</v>
       </c>
-      <c r="P40" s="185"/>
-      <c r="Q40" s="186"/>
-    </row>
-    <row r="46" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P40" s="146"/>
+      <c r="Q40" s="147"/>
+    </row>
+    <row r="45" spans="1:17" s="158" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A45" s="158" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C47" s="104" t="s">
         <v>61</v>
       </c>
@@ -5652,314 +5608,283 @@
       <c r="E47" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="134" t="s">
-        <v>175</v>
+      <c r="F47" s="138" t="s">
+        <v>174</v>
       </c>
       <c r="G47" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="H47" s="101" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="48" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C48" s="128" t="s">
+      <c r="H47" s="137" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C48" s="129" t="s">
         <v>144</v>
       </c>
-      <c r="D48" s="129" t="s">
-        <v>146</v>
-      </c>
-      <c r="E48" s="129"/>
-      <c r="F48" s="129"/>
-      <c r="G48" s="129"/>
+      <c r="D48" s="130"/>
+      <c r="E48" s="130"/>
+      <c r="F48" s="130"/>
+      <c r="G48" s="130"/>
       <c r="H48" s="130"/>
     </row>
-    <row r="49" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="127">
+    <row r="49" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C49" s="128">
         <v>-5</v>
       </c>
-      <c r="D49" s="192">
-        <v>-5.0016999999999996</v>
-      </c>
-      <c r="E49" s="192">
-        <v>-5.0111989056178103</v>
-      </c>
-      <c r="F49" s="193">
+      <c r="D49" s="132" t="s">
+        <v>161</v>
+      </c>
+      <c r="E49" s="132" t="s">
+        <v>175</v>
+      </c>
+      <c r="F49" s="130">
         <f>ABS(D49-E49)</f>
-        <v>9.4989056178107489E-3</v>
-      </c>
-      <c r="G49" s="192">
-        <v>-5.0043320620675003</v>
-      </c>
-      <c r="H49" s="197">
-        <f>ABS(D49-G49)</f>
-        <v>2.6320620675006623E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>9.4989056000001071E-3</v>
+      </c>
+      <c r="G49" s="132" t="s">
+        <v>176</v>
+      </c>
+      <c r="H49" s="137">
+        <f t="shared" ref="H49:H59" si="2">ABS(D49-G49)</f>
+        <v>2.6320600000007133E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C50" s="87">
         <v>0</v>
       </c>
-      <c r="D50" s="194">
+      <c r="D50" s="53">
         <v>0</v>
       </c>
-      <c r="E50" s="194">
-        <v>-1.19267335010034E-2</v>
-      </c>
-      <c r="F50" s="193">
-        <f t="shared" ref="F50:F60" si="2">ABS(D50-E50)</f>
-        <v>1.19267335010034E-2</v>
-      </c>
-      <c r="G50" s="194">
-        <v>9.3083603649901604E-4</v>
-      </c>
-      <c r="H50" s="197">
-        <f>ABS(D50-G50)</f>
-        <v>9.3083603649901604E-4</v>
-      </c>
-      <c r="L50" s="143"/>
-      <c r="M50" s="142" t="s">
-        <v>173</v>
-      </c>
-      <c r="N50" s="140" t="s">
-        <v>166</v>
-      </c>
-      <c r="O50" s="141" t="s">
+      <c r="E50" s="132" t="s">
+        <v>177</v>
+      </c>
+      <c r="F50" s="130">
+        <f t="shared" ref="F50:F59" si="3">ABS(D50-E50)</f>
+        <v>1.19267335E-2</v>
+      </c>
+      <c r="G50" s="132" t="s">
+        <v>178</v>
+      </c>
+      <c r="H50" s="137">
+        <f t="shared" si="2"/>
+        <v>9.3083602999999998E-4</v>
+      </c>
+      <c r="K50" s="134"/>
+      <c r="L50" s="134" t="s">
+        <v>172</v>
+      </c>
+      <c r="M50" s="134" t="s">
+        <v>165</v>
+      </c>
+      <c r="N50" s="134" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C51" s="87">
         <v>5</v>
       </c>
-      <c r="D51" s="194">
+      <c r="D51" s="53">
         <v>4.9725000000000001</v>
       </c>
-      <c r="E51" s="194">
-        <v>4.9873340469257803</v>
-      </c>
-      <c r="F51" s="193">
+      <c r="E51" s="132" t="s">
+        <v>179</v>
+      </c>
+      <c r="F51" s="130">
+        <f t="shared" si="3"/>
+        <v>1.4834046919999899E-2</v>
+      </c>
+      <c r="G51" s="132" t="s">
+        <v>180</v>
+      </c>
+      <c r="H51" s="137">
         <f t="shared" si="2"/>
-        <v>1.4834046925780164E-2</v>
-      </c>
-      <c r="G51" s="194">
-        <v>4.9733838690139898</v>
-      </c>
-      <c r="H51" s="197">
-        <f>ABS(D51-G51)</f>
-        <v>8.8386901398962436E-4</v>
-      </c>
-      <c r="L51" s="144" t="s">
-        <v>171</v>
-      </c>
-      <c r="M51" s="103">
-        <v>8.1004693299999996E-5</v>
-      </c>
-      <c r="N51" s="189">
-        <v>-0.279250575</v>
-      </c>
-      <c r="O51" s="187">
+        <v>8.8386899999992607E-4</v>
+      </c>
+      <c r="K51" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="L51" s="134">
+        <v>8.1041246399999998E-5</v>
+      </c>
+      <c r="M51" s="134">
+        <v>-8.1453097600000003E-3</v>
+      </c>
+      <c r="N51" s="134">
         <f>MAX(F49:F59)</f>
-        <v>1.4834046925780164E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1.4834046919999899E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C52" s="87">
         <v>10</v>
       </c>
-      <c r="D52" s="194">
+      <c r="D52" s="53">
         <v>9.9755000000000003</v>
       </c>
-      <c r="E52" s="194">
-        <v>9.98660622025767</v>
-      </c>
-      <c r="F52" s="193">
+      <c r="E52" s="132" t="s">
+        <v>181</v>
+      </c>
+      <c r="F52" s="130">
+        <f t="shared" si="3"/>
+        <v>1.1106220000000278E-2</v>
+      </c>
+      <c r="G52" s="132" t="s">
+        <v>182</v>
+      </c>
+      <c r="H52" s="137">
         <f t="shared" si="2"/>
-        <v>1.1106220257669719E-2</v>
-      </c>
-      <c r="G52" s="194">
-        <v>9.9781125495039902</v>
-      </c>
-      <c r="H52" s="197">
-        <f>ABS(D52-G52)</f>
-        <v>2.6125495039899249E-3</v>
-      </c>
-      <c r="L52" s="145" t="s">
-        <v>172</v>
-      </c>
-      <c r="M52" s="56">
-        <v>-4.4518134500000001E-5</v>
-      </c>
-      <c r="N52" s="191">
-        <v>30.739945899999999</v>
-      </c>
-      <c r="O52" s="188">
+        <v>2.6125495000002275E-3</v>
+      </c>
+      <c r="K52" s="134" t="s">
+        <v>171</v>
+      </c>
+      <c r="L52" s="134">
+        <v>-4.4511401799999998E-5</v>
+      </c>
+      <c r="M52" s="134">
+        <v>30.7267127</v>
+      </c>
+      <c r="N52" s="134">
         <f>MAX(H49:H59)</f>
-        <v>3.8084209800004487E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.2">
+        <v>3.8084999999981051E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C53" s="87">
         <v>15</v>
       </c>
-      <c r="D53" s="194"/>
-      <c r="E53" s="194"/>
-      <c r="F53" s="193">
+      <c r="D53" s="53"/>
+      <c r="E53" s="132"/>
+      <c r="F53" s="130">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G53" s="132"/>
+      <c r="H53" s="137">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G53" s="194"/>
-      <c r="H53" s="197">
-        <f>ABS(D53-G53)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C54" s="87">
         <v>20</v>
       </c>
-      <c r="D54" s="195"/>
-      <c r="E54" s="195"/>
-      <c r="F54" s="193">
+      <c r="D54" s="111"/>
+      <c r="E54" s="132"/>
+      <c r="F54" s="130">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G54" s="132"/>
+      <c r="H54" s="137">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G54" s="195"/>
-      <c r="H54" s="197">
-        <f>ABS(D54-G54)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C55" s="87">
         <v>25</v>
       </c>
-      <c r="D55" s="194"/>
-      <c r="E55" s="194"/>
-      <c r="F55" s="193">
+      <c r="D55" s="53"/>
+      <c r="E55" s="132"/>
+      <c r="F55" s="130">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G55" s="132"/>
+      <c r="H55" s="137">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G55" s="194"/>
-      <c r="H55" s="197">
-        <f>ABS(D55-G55)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C56" s="87">
         <v>30</v>
       </c>
-      <c r="D56" s="194"/>
-      <c r="E56" s="194"/>
-      <c r="F56" s="193">
+      <c r="D56" s="53"/>
+      <c r="E56" s="132"/>
+      <c r="F56" s="130">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G56" s="132"/>
+      <c r="H56" s="137">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G56" s="194"/>
-      <c r="H56" s="197">
-        <f>ABS(D56-G56)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C57" s="87">
         <v>35</v>
       </c>
-      <c r="D57" s="194">
+      <c r="D57" s="53">
         <v>34.9801</v>
       </c>
-      <c r="E57" s="194">
-        <v>34.982972202363399</v>
-      </c>
-      <c r="F57" s="193">
+      <c r="E57" s="132" t="s">
+        <v>183</v>
+      </c>
+      <c r="F57" s="130">
+        <f t="shared" si="3"/>
+        <v>2.8722022999971841E-3</v>
+      </c>
+      <c r="G57" s="132" t="s">
+        <v>184</v>
+      </c>
+      <c r="H57" s="137">
         <f t="shared" si="2"/>
-        <v>2.8722023633989124E-3</v>
-      </c>
-      <c r="G57" s="194">
-        <v>34.97629157902</v>
-      </c>
-      <c r="H57" s="197">
-        <f>ABS(D57-G57)</f>
-        <v>3.8084209800004487E-3</v>
-      </c>
-      <c r="K57" s="139"/>
-    </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.2">
+        <v>3.8084999999981051E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C58" s="90">
         <v>40</v>
       </c>
-      <c r="D58" s="196"/>
-      <c r="E58" s="196"/>
-      <c r="F58" s="193">
+      <c r="D58" s="127"/>
+      <c r="E58" s="132"/>
+      <c r="F58" s="130">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G58" s="132"/>
+      <c r="H58" s="137">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G58" s="196"/>
-      <c r="H58" s="197">
-        <f>ABS(D58-G58)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C59" s="90">
         <v>45</v>
       </c>
-      <c r="D59" s="196">
+      <c r="D59" s="127">
         <v>44.988999999999997</v>
       </c>
-      <c r="E59" s="196">
-        <v>44.981516547407097</v>
-      </c>
-      <c r="F59" s="193">
+      <c r="E59" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="F59" s="130">
+        <f t="shared" si="3"/>
+        <v>7.483452599998941E-3</v>
+      </c>
+      <c r="G59" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="H59" s="137">
         <f t="shared" si="2"/>
-        <v>7.483452592900619E-3</v>
-      </c>
-      <c r="G59" s="196">
-        <v>44.9909130436019</v>
-      </c>
-      <c r="H59" s="197">
-        <f>ABS(D59-G59)</f>
-        <v>1.9130436019025865E-3</v>
-      </c>
-      <c r="J59" s="138"/>
-    </row>
-    <row r="60" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1.913043000001835E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C60" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="D60" s="190"/>
-      <c r="E60" s="190"/>
-      <c r="F60" s="198">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G60" s="190"/>
-      <c r="H60" s="199">
-        <f>ABS(D60-G60)</f>
-        <v>0</v>
-      </c>
-      <c r="L60" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="61" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="L61" t="s">
-        <v>180</v>
-      </c>
-      <c r="M61">
-        <f>M51/M11</f>
-        <v>0.99954895683835387</v>
-      </c>
-    </row>
-    <row r="62" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="L62" t="s">
-        <v>181</v>
-      </c>
-      <c r="M62">
-        <f>M52/M12</f>
-        <v>1.0001512578738871</v>
-      </c>
+      <c r="D60" s="56"/>
+      <c r="E60" s="56"/>
+      <c r="F60" s="56"/>
+      <c r="G60" s="56"/>
+      <c r="H60" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6013,7 +5938,7 @@
       <c r="B4" s="116"/>
       <c r="C4" s="116"/>
       <c r="D4" s="116" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E4" s="116"/>
       <c r="F4" s="116"/>
@@ -6116,22 +6041,22 @@
         <v>111</v>
       </c>
       <c r="C12" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="122" t="s">
         <v>148</v>
       </c>
-      <c r="D12" s="122" t="s">
+      <c r="E12" s="122" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="122" t="s">
+      <c r="F12" s="122" t="s">
         <v>150</v>
       </c>
-      <c r="F12" s="122" t="s">
+      <c r="G12" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="G12" s="122" t="s">
-        <v>152</v>
-      </c>
       <c r="H12" s="123" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K12" s="95">
         <v>6</v>
@@ -6281,22 +6206,22 @@
         <v>111</v>
       </c>
       <c r="C20" s="121" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="122" t="s">
         <v>153</v>
       </c>
-      <c r="D20" s="122" t="s">
+      <c r="E20" s="122" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="122" t="s">
+      <c r="F20" s="122" t="s">
         <v>155</v>
       </c>
-      <c r="F20" s="122" t="s">
+      <c r="G20" s="122" t="s">
         <v>156</v>
       </c>
-      <c r="G20" s="122" t="s">
+      <c r="H20" s="123" t="s">
         <v>157</v>
-      </c>
-      <c r="H20" s="123" t="s">
-        <v>158</v>
       </c>
       <c r="K20" s="95"/>
       <c r="L20" s="94"/>

</xml_diff>

<commit_message>
update excel to Anders version
</commit_message>
<xml_diff>
--- a/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
+++ b/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anderssandstrom/ecmc_bifrost_vac_tank_sat/docs/testplan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federicorojas/ecmc_bifrost_vac_tank_sat/docs/testplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38649EA-5FEF-3C46-83BB-612BD7FCF9DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0437A34B-646D-704B-9256-CB0948287335}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="520" windowWidth="27800" windowHeight="20660" activeTab="5" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="16520" activeTab="3" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="15" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="184">
   <si>
     <t>General Inspection</t>
   </si>
@@ -683,13 +683,19 @@
   <si>
     <t>posital</t>
   </si>
+  <si>
+    <t>Low Kill Switch</t>
+  </si>
+  <si>
+    <t>-4.57367765711</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1844,21 +1850,21 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3496,8 +3502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856B0310-C035-6C4C-A5AB-B339976BEC09}">
   <dimension ref="B2:S60"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3507,6 +3513,7 @@
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
@@ -3618,7 +3625,7 @@
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B14" s="86"/>
       <c r="C14" s="81" t="s">
-        <v>45</v>
+        <v>182</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>53</v>
@@ -3683,7 +3690,9 @@
       <c r="D16" s="54"/>
       <c r="E16" s="54"/>
       <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
+      <c r="G16" s="54" t="s">
+        <v>183</v>
+      </c>
       <c r="H16" s="54"/>
       <c r="I16" s="58"/>
       <c r="L16" s="95"/>
@@ -4467,7 +4476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CEB521-8DC8-0C48-A601-3238D1EFF0A3}">
   <dimension ref="B2:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
@@ -5692,7 +5701,7 @@
         <v>-5.0043320620675003</v>
       </c>
       <c r="H49" s="197">
-        <f>ABS(D49-G49)</f>
+        <f t="shared" ref="H49:H60" si="2">ABS(D49-G49)</f>
         <v>2.6320620675006623E-3</v>
       </c>
     </row>
@@ -5707,14 +5716,14 @@
         <v>-1.19267335010034E-2</v>
       </c>
       <c r="F50" s="193">
-        <f t="shared" ref="F50:F60" si="2">ABS(D50-E50)</f>
+        <f t="shared" ref="F50:F60" si="3">ABS(D50-E50)</f>
         <v>1.19267335010034E-2</v>
       </c>
       <c r="G50" s="194">
         <v>9.3083603649901604E-4</v>
       </c>
       <c r="H50" s="197">
-        <f>ABS(D50-G50)</f>
+        <f t="shared" si="2"/>
         <v>9.3083603649901604E-4</v>
       </c>
       <c r="L50" s="143"/>
@@ -5739,14 +5748,14 @@
         <v>4.9873340469257803</v>
       </c>
       <c r="F51" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4834046925780164E-2</v>
       </c>
       <c r="G51" s="194">
         <v>4.9733838690139898</v>
       </c>
       <c r="H51" s="197">
-        <f>ABS(D51-G51)</f>
+        <f t="shared" si="2"/>
         <v>8.8386901398962436E-4</v>
       </c>
       <c r="L51" s="144" t="s">
@@ -5774,14 +5783,14 @@
         <v>9.98660622025767</v>
       </c>
       <c r="F52" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1106220257669719E-2</v>
       </c>
       <c r="G52" s="194">
         <v>9.9781125495039902</v>
       </c>
       <c r="H52" s="197">
-        <f>ABS(D52-G52)</f>
+        <f t="shared" si="2"/>
         <v>2.6125495039899249E-3</v>
       </c>
       <c r="L52" s="145" t="s">
@@ -5805,12 +5814,12 @@
       <c r="D53" s="194"/>
       <c r="E53" s="194"/>
       <c r="F53" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G53" s="194"/>
       <c r="H53" s="197">
-        <f>ABS(D53-G53)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5821,12 +5830,12 @@
       <c r="D54" s="195"/>
       <c r="E54" s="195"/>
       <c r="F54" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G54" s="195"/>
       <c r="H54" s="197">
-        <f>ABS(D54-G54)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5837,12 +5846,12 @@
       <c r="D55" s="194"/>
       <c r="E55" s="194"/>
       <c r="F55" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G55" s="194"/>
       <c r="H55" s="197">
-        <f>ABS(D55-G55)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5853,12 +5862,12 @@
       <c r="D56" s="194"/>
       <c r="E56" s="194"/>
       <c r="F56" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G56" s="194"/>
       <c r="H56" s="197">
-        <f>ABS(D56-G56)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5873,14 +5882,14 @@
         <v>34.982972202363399</v>
       </c>
       <c r="F57" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.8722023633989124E-3</v>
       </c>
       <c r="G57" s="194">
         <v>34.97629157902</v>
       </c>
       <c r="H57" s="197">
-        <f>ABS(D57-G57)</f>
+        <f t="shared" si="2"/>
         <v>3.8084209800004487E-3</v>
       </c>
       <c r="K57" s="139"/>
@@ -5892,12 +5901,12 @@
       <c r="D58" s="196"/>
       <c r="E58" s="196"/>
       <c r="F58" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G58" s="196"/>
       <c r="H58" s="197">
-        <f>ABS(D58-G58)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5912,14 +5921,14 @@
         <v>44.981516547407097</v>
       </c>
       <c r="F59" s="193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.483452592900619E-3</v>
       </c>
       <c r="G59" s="196">
         <v>44.9909130436019</v>
       </c>
       <c r="H59" s="197">
-        <f>ABS(D59-G59)</f>
+        <f t="shared" si="2"/>
         <v>1.9130436019025865E-3</v>
       </c>
       <c r="J59" s="138"/>
@@ -5931,12 +5940,12 @@
       <c r="D60" s="190"/>
       <c r="E60" s="190"/>
       <c r="F60" s="198">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G60" s="190"/>
       <c r="H60" s="199">
-        <f>ABS(D60-G60)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L60" t="s">

</xml_diff>

<commit_message>
Go back to Anders version
</commit_message>
<xml_diff>
--- a/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
+++ b/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federicorojas/ecmc_bifrost_vac_tank_sat/docs/testplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE262FA3-E382-6342-878C-A941B1455E5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0437A34B-646D-704B-9256-CB0948287335}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="5" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="16520" activeTab="3" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="15" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="184">
   <si>
     <t>General Inspection</t>
   </si>
@@ -576,6 +576,9 @@
     <t>hardstop high</t>
   </si>
   <si>
+    <t>10.98</t>
+  </si>
+  <si>
     <t>-5,0177</t>
   </si>
   <si>
@@ -663,53 +666,38 @@
     <t>OL diff abs</t>
   </si>
   <si>
-    <t>-5,0111989056</t>
-  </si>
-  <si>
-    <t>-5,00433206</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -0,01192673350</t>
-  </si>
-  <si>
-    <t>0,00093083603</t>
-  </si>
-  <si>
-    <t>4,98733404692</t>
-  </si>
-  <si>
-    <t>4,973383869</t>
-  </si>
-  <si>
-    <t>9,986606220</t>
-  </si>
-  <si>
-    <t>9,97811254950</t>
-  </si>
-  <si>
-    <t>34,9829722023</t>
-  </si>
-  <si>
-    <t>34,9762915</t>
-  </si>
-  <si>
-    <t>44,9815165474</t>
-  </si>
-  <si>
-    <t>44,990913043</t>
-  </si>
-  <si>
-    <t>AFTER COLLISION</t>
+    <t>After collision</t>
+  </si>
+  <si>
+    <t>BELOW AFTER COLLISION</t>
   </si>
   <si>
     <t>BEFORE COLLISION</t>
+  </si>
+  <si>
+    <t>Gear ratio DIFF (before vs after collision)</t>
+  </si>
+  <si>
+    <t>Open loop</t>
+  </si>
+  <si>
+    <t>posital</t>
+  </si>
+  <si>
+    <t>Low Kill Switch</t>
+  </si>
+  <si>
+    <t>-4.57367765711</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -809,9 +797,31 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -856,12 +866,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="57">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -1564,24 +1574,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1785,44 +1782,89 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="42" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3460,8 +3502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856B0310-C035-6C4C-A5AB-B339976BEC09}">
   <dimension ref="B2:S60"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3471,6 +3513,7 @@
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
@@ -3582,7 +3625,7 @@
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B14" s="86"/>
       <c r="C14" s="81" t="s">
-        <v>45</v>
+        <v>182</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>53</v>
@@ -3647,7 +3690,9 @@
       <c r="D16" s="54"/>
       <c r="E16" s="54"/>
       <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
+      <c r="G16" s="54" t="s">
+        <v>183</v>
+      </c>
       <c r="H16" s="54"/>
       <c r="I16" s="58"/>
       <c r="L16" s="95"/>
@@ -4429,23 +4474,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CEB521-8DC8-0C48-A601-3238D1EFF0A3}">
-  <dimension ref="A2:Z60"/>
+  <dimension ref="B2:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="13.6640625" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>109</v>
       </c>
@@ -4453,7 +4502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>96</v>
       </c>
@@ -4464,13 +4513,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="158" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="158" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:26" s="146" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="150" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>124</v>
       </c>
@@ -4483,24 +4532,24 @@
       <c r="E7" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="138" t="s">
-        <v>174</v>
+      <c r="F7" s="134" t="s">
+        <v>175</v>
       </c>
       <c r="G7" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="H7" s="137" t="s">
-        <v>173</v>
-      </c>
-      <c r="I7" s="137"/>
-      <c r="J7" s="137"/>
-      <c r="K7" s="137"/>
-      <c r="L7" s="137"/>
-      <c r="M7" s="154"/>
-      <c r="N7" s="154"/>
-      <c r="O7" s="154"/>
-      <c r="P7" s="154"/>
-      <c r="Q7" s="154"/>
+      <c r="H7" s="101" t="s">
+        <v>174</v>
+      </c>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="133"/>
+      <c r="M7" s="135"/>
+      <c r="N7" s="135"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="135"/>
       <c r="S7" s="91" t="s">
         <v>100</v>
       </c>
@@ -4514,36 +4563,36 @@
       <c r="Y7" s="92"/>
       <c r="Z7" s="93"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C8" s="129" t="s">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="C8" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="130">
+      <c r="D8" s="129">
         <v>-10.98</v>
       </c>
-      <c r="E8" s="130">
+      <c r="E8" s="129">
         <v>-10.978210375023499</v>
       </c>
-      <c r="F8" s="130">
+      <c r="F8" s="129">
         <f>ABS(D8-E8)</f>
         <v>1.7896249765012584E-3</v>
       </c>
-      <c r="G8" s="130">
+      <c r="G8" s="129">
         <v>-10.974417235955199</v>
       </c>
-      <c r="H8" s="137">
+      <c r="H8" s="130">
         <f>ABS(D8-G8)</f>
         <v>5.5827640448011806E-3</v>
       </c>
-      <c r="I8" s="137"/>
-      <c r="J8" s="137"/>
-      <c r="K8" s="137"/>
-      <c r="L8" s="137"/>
-      <c r="M8" s="137"/>
-      <c r="N8" s="137"/>
-      <c r="O8" s="137"/>
-      <c r="P8" s="137"/>
-      <c r="Q8" s="137"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="133"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="133"/>
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
+      <c r="P8" s="133"/>
+      <c r="Q8" s="133"/>
       <c r="S8" s="124"/>
       <c r="T8" s="125"/>
       <c r="U8" s="125"/>
@@ -4553,36 +4602,36 @@
       <c r="Y8" s="125"/>
       <c r="Z8" s="126"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C9" s="128">
+    <row r="9" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="127">
         <v>-5</v>
       </c>
-      <c r="D9" s="132" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="132">
+      <c r="D9" s="192" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="192">
         <v>-5.0096773753587298</v>
       </c>
-      <c r="F9" s="130">
+      <c r="F9" s="193">
         <f t="shared" ref="F9:F19" si="0">ABS(D9-E9)</f>
         <v>8.0226246412697932E-3</v>
       </c>
-      <c r="G9" s="132">
+      <c r="G9" s="192">
         <v>-5.0102009745677902</v>
       </c>
-      <c r="H9" s="137">
+      <c r="H9" s="197">
         <f t="shared" ref="H9:H19" si="1">ABS(D9-G9)</f>
         <v>7.4990254322093719E-3</v>
       </c>
-      <c r="I9" s="133"/>
-      <c r="J9" s="133"/>
-      <c r="K9" s="134"/>
-      <c r="L9" s="134"/>
-      <c r="M9" s="155"/>
-      <c r="N9" s="156"/>
-      <c r="O9" s="156"/>
-      <c r="P9" s="156"/>
-      <c r="Q9" s="156"/>
+      <c r="I9" s="131"/>
+      <c r="J9" s="131"/>
+      <c r="K9" s="132"/>
+      <c r="L9" s="132"/>
+      <c r="M9" s="136"/>
+      <c r="N9" s="137"/>
+      <c r="O9" s="137"/>
+      <c r="P9" s="137"/>
+      <c r="Q9" s="137"/>
       <c r="S9" s="95">
         <v>5</v>
       </c>
@@ -4594,42 +4643,42 @@
       <c r="Y9" s="94"/>
       <c r="Z9" s="96"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="87">
         <v>0</v>
       </c>
-      <c r="D10" s="53">
+      <c r="D10" s="194">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="E10" s="132">
+      <c r="E10" s="194">
         <v>-8.1487286875825005E-3</v>
       </c>
-      <c r="F10" s="130">
+      <c r="F10" s="193">
         <f t="shared" si="0"/>
         <v>2.7348728687582501E-2</v>
       </c>
-      <c r="G10" s="132">
+      <c r="G10" s="194">
         <v>-1.17485980349982E-2</v>
       </c>
-      <c r="H10" s="137">
+      <c r="H10" s="197">
         <f t="shared" si="1"/>
         <v>3.09485980349982E-2</v>
       </c>
-      <c r="I10" s="133"/>
-      <c r="J10" s="133"/>
-      <c r="K10" s="134"/>
-      <c r="L10" s="134"/>
-      <c r="M10" s="134" t="s">
-        <v>172</v>
-      </c>
-      <c r="N10" s="134" t="s">
-        <v>165</v>
-      </c>
-      <c r="O10" s="134" t="s">
+      <c r="I10" s="131"/>
+      <c r="J10" s="131"/>
+      <c r="K10" s="132"/>
+      <c r="L10" s="143"/>
+      <c r="M10" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="N10" s="140" t="s">
+        <v>166</v>
+      </c>
+      <c r="O10" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="134"/>
-      <c r="Q10" s="134"/>
+      <c r="P10" s="132"/>
+      <c r="Q10" s="132"/>
       <c r="S10" s="95"/>
       <c r="T10" s="94"/>
       <c r="U10" s="94"/>
@@ -4639,45 +4688,45 @@
       <c r="Y10" s="94"/>
       <c r="Z10" s="96"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C11" s="87">
         <v>5</v>
       </c>
-      <c r="D11" s="53">
+      <c r="D11" s="194">
         <v>4.9862000000000002</v>
       </c>
-      <c r="E11" s="132">
+      <c r="E11" s="194">
         <v>4.9933787789488502</v>
       </c>
-      <c r="F11" s="130">
+      <c r="F11" s="193">
         <f t="shared" si="0"/>
         <v>7.1787789488499953E-3</v>
       </c>
-      <c r="G11" s="132">
+      <c r="G11" s="194">
         <v>4.9956060588578</v>
       </c>
-      <c r="H11" s="137">
+      <c r="H11" s="197">
         <f t="shared" si="1"/>
         <v>9.4060588577997706E-3</v>
       </c>
-      <c r="I11" s="133"/>
-      <c r="J11" s="133"/>
-      <c r="K11" s="134"/>
-      <c r="L11" s="134" t="s">
-        <v>170</v>
-      </c>
-      <c r="M11" s="134">
+      <c r="I11" s="131"/>
+      <c r="J11" s="131"/>
+      <c r="K11" s="132"/>
+      <c r="L11" s="144" t="s">
+        <v>171</v>
+      </c>
+      <c r="M11" s="103">
         <v>8.1041246399999998E-5</v>
       </c>
-      <c r="N11" s="134">
+      <c r="N11" s="189">
         <v>-8.1453097600000003E-3</v>
       </c>
-      <c r="O11" s="134">
+      <c r="O11" s="187">
         <f>MAX(F9:F19)</f>
         <v>2.7348728687582501E-2</v>
       </c>
-      <c r="P11" s="134"/>
-      <c r="Q11" s="134"/>
+      <c r="P11" s="132"/>
+      <c r="Q11" s="132"/>
       <c r="S11" s="95"/>
       <c r="T11" s="94"/>
       <c r="U11" s="94"/>
@@ -4687,45 +4736,45 @@
       <c r="Y11" s="94"/>
       <c r="Z11" s="96"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="87">
         <v>10</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="194">
         <v>9.9887999999999995</v>
       </c>
-      <c r="E12" s="132">
+      <c r="E12" s="194">
         <v>9.9949074254174004</v>
       </c>
-      <c r="F12" s="130">
+      <c r="F12" s="193">
         <f t="shared" si="0"/>
         <v>6.1074254174009468E-3</v>
       </c>
-      <c r="G12" s="132">
+      <c r="G12" s="194">
         <v>9.9986431097759993</v>
       </c>
-      <c r="H12" s="137">
+      <c r="H12" s="197">
         <f t="shared" si="1"/>
         <v>9.843109775999892E-3</v>
       </c>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="134"/>
-      <c r="L12" s="134" t="s">
-        <v>171</v>
-      </c>
-      <c r="M12" s="134">
+      <c r="I12" s="131"/>
+      <c r="J12" s="131"/>
+      <c r="K12" s="132"/>
+      <c r="L12" s="145" t="s">
+        <v>172</v>
+      </c>
+      <c r="M12" s="56">
         <v>-4.4511401799999998E-5</v>
       </c>
-      <c r="N12" s="134">
+      <c r="N12" s="191">
         <v>30.7267127</v>
       </c>
-      <c r="O12" s="134">
+      <c r="O12" s="188">
         <f>MAX(H9:H19)</f>
         <v>3.09485980349982E-2</v>
       </c>
-      <c r="P12" s="134"/>
-      <c r="Q12" s="134"/>
+      <c r="P12" s="132"/>
+      <c r="Q12" s="132"/>
       <c r="S12" s="95"/>
       <c r="T12" s="94"/>
       <c r="U12" s="94"/>
@@ -4735,36 +4784,36 @@
       <c r="Y12" s="94"/>
       <c r="Z12" s="96"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C13" s="87">
         <v>15</v>
       </c>
-      <c r="D13" s="53">
+      <c r="D13" s="194">
         <v>14.989699999999999</v>
       </c>
-      <c r="E13" s="132">
+      <c r="E13" s="194">
         <v>14.9964355029764</v>
       </c>
-      <c r="F13" s="130">
+      <c r="F13" s="193">
         <f t="shared" si="0"/>
         <v>6.7355029764009089E-3</v>
       </c>
-      <c r="G13" s="132">
+      <c r="G13" s="194">
         <v>15.0015911378906</v>
       </c>
-      <c r="H13" s="137">
+      <c r="H13" s="197">
         <f t="shared" si="1"/>
         <v>1.1891137890600589E-2</v>
       </c>
-      <c r="I13" s="133"/>
-      <c r="J13" s="133"/>
-      <c r="K13" s="134"/>
-      <c r="L13" s="134"/>
-      <c r="M13" s="134"/>
-      <c r="N13" s="134"/>
-      <c r="O13" s="134"/>
-      <c r="P13" s="134"/>
-      <c r="Q13" s="134"/>
+      <c r="I13" s="131"/>
+      <c r="J13" s="131"/>
+      <c r="K13" s="132"/>
+      <c r="L13" s="132"/>
+      <c r="M13" s="132"/>
+      <c r="N13" s="132"/>
+      <c r="O13" s="132"/>
+      <c r="P13" s="132"/>
+      <c r="Q13" s="132"/>
       <c r="S13" s="95"/>
       <c r="T13" s="94"/>
       <c r="U13" s="94"/>
@@ -4774,36 +4823,36 @@
       <c r="Y13" s="94"/>
       <c r="Z13" s="96"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C14" s="87">
         <v>20</v>
       </c>
-      <c r="D14" s="111">
+      <c r="D14" s="195">
         <v>19.995100000000001</v>
       </c>
-      <c r="E14" s="132">
+      <c r="E14" s="195">
         <v>19.997963580535298</v>
       </c>
-      <c r="F14" s="130">
+      <c r="F14" s="193">
         <f t="shared" si="0"/>
         <v>2.8635805352976718E-3</v>
       </c>
-      <c r="G14" s="132">
+      <c r="G14" s="195">
         <v>19.997906967136899</v>
       </c>
-      <c r="H14" s="137">
+      <c r="H14" s="197">
         <f t="shared" si="1"/>
         <v>2.8069671368982085E-3</v>
       </c>
-      <c r="I14" s="133"/>
-      <c r="J14" s="133"/>
-      <c r="K14" s="134"/>
-      <c r="L14" s="134"/>
-      <c r="M14" s="134"/>
-      <c r="N14" s="134"/>
-      <c r="O14" s="134"/>
-      <c r="P14" s="134"/>
-      <c r="Q14" s="134"/>
+      <c r="I14" s="131"/>
+      <c r="J14" s="131"/>
+      <c r="K14" s="132"/>
+      <c r="L14" s="132"/>
+      <c r="M14" s="132"/>
+      <c r="N14" s="132"/>
+      <c r="O14" s="132"/>
+      <c r="P14" s="132"/>
+      <c r="Q14" s="132"/>
       <c r="S14" s="95"/>
       <c r="T14" s="94"/>
       <c r="U14" s="94"/>
@@ -4813,36 +4862,36 @@
       <c r="Y14" s="94"/>
       <c r="Z14" s="96"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C15" s="87">
         <v>25</v>
       </c>
-      <c r="D15" s="53">
+      <c r="D15" s="194">
         <v>24.9998</v>
       </c>
-      <c r="E15" s="132">
+      <c r="E15" s="194">
         <v>24.9994916580943</v>
       </c>
-      <c r="F15" s="130">
+      <c r="F15" s="193">
         <f t="shared" si="0"/>
         <v>3.0834190570061537E-4</v>
       </c>
-      <c r="G15" s="132">
+      <c r="G15" s="194">
         <v>24.997071526098601</v>
       </c>
-      <c r="H15" s="137">
+      <c r="H15" s="197">
         <f t="shared" si="1"/>
         <v>2.7284739013992976E-3</v>
       </c>
-      <c r="I15" s="133"/>
-      <c r="J15" s="133"/>
-      <c r="K15" s="134"/>
-      <c r="L15" s="134"/>
-      <c r="M15" s="134"/>
-      <c r="N15" s="134"/>
-      <c r="O15" s="134"/>
-      <c r="P15" s="134"/>
-      <c r="Q15" s="134"/>
+      <c r="I15" s="131"/>
+      <c r="J15" s="131"/>
+      <c r="K15" s="132"/>
+      <c r="L15" s="132"/>
+      <c r="M15" s="132"/>
+      <c r="N15" s="132"/>
+      <c r="O15" s="132"/>
+      <c r="P15" s="132"/>
+      <c r="Q15" s="132"/>
       <c r="S15" s="95"/>
       <c r="T15" s="94"/>
       <c r="U15" s="94"/>
@@ -4852,36 +4901,36 @@
       <c r="Y15" s="94"/>
       <c r="Z15" s="96"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C16" s="87">
         <v>30</v>
       </c>
-      <c r="D16" s="53">
+      <c r="D16" s="194">
         <v>29.996500000000001</v>
       </c>
-      <c r="E16" s="132">
+      <c r="E16" s="194">
         <v>30.001019735653301</v>
       </c>
-      <c r="F16" s="130">
+      <c r="F16" s="193">
         <f t="shared" si="0"/>
         <v>4.5197356533002164E-3</v>
       </c>
-      <c r="G16" s="132">
+      <c r="G16" s="194">
         <v>29.995123300015202</v>
       </c>
-      <c r="H16" s="137">
+      <c r="H16" s="197">
         <f t="shared" si="1"/>
         <v>1.376699984799501E-3</v>
       </c>
-      <c r="I16" s="133"/>
-      <c r="J16" s="133"/>
-      <c r="K16" s="134"/>
-      <c r="L16" s="134"/>
-      <c r="M16" s="134"/>
-      <c r="N16" s="134"/>
-      <c r="O16" s="134"/>
-      <c r="P16" s="134"/>
-      <c r="Q16" s="134"/>
+      <c r="I16" s="131"/>
+      <c r="J16" s="131"/>
+      <c r="K16" s="132"/>
+      <c r="L16" s="132"/>
+      <c r="M16" s="132"/>
+      <c r="N16" s="132"/>
+      <c r="O16" s="132"/>
+      <c r="P16" s="132"/>
+      <c r="Q16" s="132"/>
       <c r="S16" s="95"/>
       <c r="T16" s="94"/>
       <c r="U16" s="94"/>
@@ -4891,36 +4940,36 @@
       <c r="Y16" s="94"/>
       <c r="Z16" s="96"/>
     </row>
-    <row r="17" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C17" s="87">
         <v>35</v>
       </c>
-      <c r="D17" s="53">
+      <c r="D17" s="194">
         <v>35.000500000000002</v>
       </c>
-      <c r="E17" s="132">
+      <c r="E17" s="194">
         <v>35.002548380501104</v>
       </c>
-      <c r="F17" s="130">
+      <c r="F17" s="193">
         <f t="shared" si="0"/>
         <v>2.0483805011011214E-3</v>
       </c>
-      <c r="G17" s="132">
+      <c r="G17" s="194">
         <v>34.997359145700898</v>
       </c>
-      <c r="H17" s="137">
+      <c r="H17" s="197">
         <f t="shared" si="1"/>
         <v>3.1408542991044897E-3</v>
       </c>
-      <c r="I17" s="133"/>
-      <c r="J17" s="133"/>
-      <c r="K17" s="134"/>
-      <c r="L17" s="134"/>
-      <c r="M17" s="134"/>
-      <c r="N17" s="134"/>
-      <c r="O17" s="134"/>
-      <c r="P17" s="134"/>
-      <c r="Q17" s="134"/>
+      <c r="I17" s="131"/>
+      <c r="J17" s="131"/>
+      <c r="K17" s="132"/>
+      <c r="L17" s="132"/>
+      <c r="M17" s="132"/>
+      <c r="N17" s="132"/>
+      <c r="O17" s="132"/>
+      <c r="P17" s="132"/>
+      <c r="Q17" s="132"/>
       <c r="S17" s="95"/>
       <c r="T17" s="94"/>
       <c r="U17" s="94"/>
@@ -4930,35 +4979,35 @@
       <c r="Y17" s="94"/>
       <c r="Z17" s="96"/>
     </row>
-    <row r="18" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C18" s="90">
         <v>40</v>
       </c>
-      <c r="D18" s="127">
+      <c r="D18" s="196">
         <v>40.009500000000003</v>
       </c>
-      <c r="E18" s="132">
+      <c r="E18" s="196">
         <v>40.004076458060098</v>
       </c>
-      <c r="F18" s="130">
+      <c r="F18" s="193">
         <f t="shared" si="0"/>
         <v>5.4235419399049078E-3</v>
       </c>
-      <c r="G18" s="132">
+      <c r="G18" s="196">
         <v>40.004891848200899</v>
       </c>
-      <c r="H18" s="137">
+      <c r="H18" s="197">
         <f t="shared" si="1"/>
         <v>4.608151799104121E-3</v>
       </c>
-      <c r="I18" s="133"/>
-      <c r="J18" s="133"/>
-      <c r="L18" s="134"/>
-      <c r="M18" s="134"/>
-      <c r="N18" s="134"/>
-      <c r="O18" s="134"/>
-      <c r="P18" s="134"/>
-      <c r="Q18" s="134"/>
+      <c r="I18" s="131"/>
+      <c r="J18" s="131"/>
+      <c r="L18" s="132"/>
+      <c r="M18" s="132"/>
+      <c r="N18" s="132"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="132"/>
+      <c r="Q18" s="132"/>
       <c r="S18" s="95"/>
       <c r="T18" s="94"/>
       <c r="U18" s="94"/>
@@ -4968,36 +5017,36 @@
       <c r="Y18" s="94"/>
       <c r="Z18" s="96"/>
     </row>
-    <row r="19" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C19" s="90">
         <v>45</v>
       </c>
-      <c r="D19" s="127">
+      <c r="D19" s="196">
         <v>45.012700000000002</v>
       </c>
-      <c r="E19" s="132">
+      <c r="E19" s="196">
         <v>45.005604535619099</v>
       </c>
-      <c r="F19" s="130">
+      <c r="F19" s="193">
         <f t="shared" si="0"/>
         <v>7.0954643809031381E-3</v>
       </c>
-      <c r="G19" s="132">
+      <c r="G19" s="196">
         <v>45.0113562770578</v>
       </c>
-      <c r="H19" s="137">
+      <c r="H19" s="197">
         <f t="shared" si="1"/>
         <v>1.3437229422024188E-3</v>
       </c>
-      <c r="I19" s="133"/>
-      <c r="J19" s="133"/>
-      <c r="K19" s="134"/>
-      <c r="L19" s="134"/>
-      <c r="M19" s="134"/>
-      <c r="N19" s="134"/>
-      <c r="O19" s="134"/>
-      <c r="P19" s="134"/>
-      <c r="Q19" s="134"/>
+      <c r="I19" s="131"/>
+      <c r="J19" s="131"/>
+      <c r="K19" s="132"/>
+      <c r="L19" s="132"/>
+      <c r="M19" s="132"/>
+      <c r="N19" s="132"/>
+      <c r="O19" s="132"/>
+      <c r="P19" s="132"/>
+      <c r="Q19" s="132"/>
       <c r="S19" s="95"/>
       <c r="T19" s="94"/>
       <c r="U19" s="94"/>
@@ -5007,26 +5056,26 @@
       <c r="Y19" s="94"/>
       <c r="Z19" s="96"/>
     </row>
-    <row r="20" spans="3:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="D20" s="56">
+      <c r="D20" s="190">
         <v>48.5</v>
       </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="157"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="134"/>
-      <c r="I20" s="134"/>
-      <c r="J20" s="134"/>
-      <c r="K20" s="134"/>
-      <c r="L20" s="134"/>
-      <c r="M20" s="134"/>
-      <c r="N20" s="134"/>
-      <c r="O20" s="134"/>
-      <c r="P20" s="134"/>
-      <c r="Q20" s="134"/>
+      <c r="E20" s="190"/>
+      <c r="F20" s="198"/>
+      <c r="G20" s="190"/>
+      <c r="H20" s="199"/>
+      <c r="I20" s="132"/>
+      <c r="J20" s="132"/>
+      <c r="K20" s="132"/>
+      <c r="L20" s="132"/>
+      <c r="M20" s="132"/>
+      <c r="N20" s="132"/>
+      <c r="O20" s="132"/>
+      <c r="P20" s="132"/>
+      <c r="Q20" s="132"/>
       <c r="S20" s="95"/>
       <c r="T20" s="94"/>
       <c r="U20" s="94"/>
@@ -5036,10 +5085,10 @@
       <c r="Y20" s="94"/>
       <c r="Z20" s="96"/>
     </row>
-    <row r="21" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="R21" s="95"/>
       <c r="S21" s="94" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="T21" s="94"/>
       <c r="U21" s="94"/>
@@ -5048,17 +5097,22 @@
       <c r="X21" s="94"/>
       <c r="Y21" s="96"/>
     </row>
-    <row r="22" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="R22" s="95"/>
-      <c r="S22" s="94"/>
-      <c r="T22" s="94"/>
-      <c r="U22" s="94"/>
-      <c r="V22" s="94"/>
-      <c r="W22" s="94"/>
-      <c r="X22" s="94"/>
-      <c r="Y22" s="96"/>
-    </row>
-    <row r="23" spans="3:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:26" s="146" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150" t="s">
+        <v>177</v>
+      </c>
+      <c r="R22" s="147"/>
+      <c r="S22" s="148"/>
+      <c r="T22" s="148"/>
+      <c r="U22" s="148"/>
+      <c r="V22" s="148"/>
+      <c r="W22" s="148"/>
+      <c r="X22" s="148"/>
+      <c r="Y22" s="149"/>
+    </row>
+    <row r="23" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R23" s="97"/>
       <c r="S23" s="98"/>
       <c r="T23" s="98"/>
@@ -5068,537 +5122,536 @@
       <c r="X23" s="98"/>
       <c r="Y23" s="99"/>
     </row>
-    <row r="24" spans="3:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="3:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="104" t="s">
+    <row r="24" spans="2:26" s="151" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="151" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="2:26" s="151" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="152" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="102" t="s">
+      <c r="D25" s="153" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="140" t="s">
-        <v>163</v>
-      </c>
-      <c r="F25" s="142" t="s">
+      <c r="E25" s="154" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" s="155" t="s">
         <v>107</v>
       </c>
-      <c r="G25" s="138"/>
-      <c r="H25" s="101"/>
-      <c r="I25" s="149"/>
-      <c r="J25" s="149"/>
-      <c r="K25" s="140"/>
-      <c r="L25" s="104" t="s">
+      <c r="G25" s="156"/>
+      <c r="H25" s="157"/>
+      <c r="I25" s="158"/>
+      <c r="J25" s="158"/>
+      <c r="K25" s="154"/>
+      <c r="L25" s="152" t="s">
         <v>108</v>
       </c>
-      <c r="M25" s="101"/>
-      <c r="N25" s="101"/>
-      <c r="O25" s="101"/>
-      <c r="P25" s="152"/>
-      <c r="Q25" s="153"/>
-    </row>
-    <row r="26" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C26" s="129" t="s">
+      <c r="M25" s="157"/>
+      <c r="N25" s="157"/>
+      <c r="O25" s="157"/>
+      <c r="P25" s="159"/>
+      <c r="Q25" s="160"/>
+    </row>
+    <row r="26" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="161" t="s">
         <v>144</v>
       </c>
-      <c r="D26" s="130">
-        <v>10.98</v>
-      </c>
-      <c r="E26" s="139"/>
-      <c r="F26" s="129"/>
-      <c r="G26" s="139" t="s">
+      <c r="D26" s="162" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" s="163"/>
+      <c r="F26" s="161"/>
+      <c r="G26" s="163" t="s">
+        <v>166</v>
+      </c>
+      <c r="H26" s="164" t="s">
         <v>165</v>
       </c>
-      <c r="H26" s="131" t="s">
-        <v>164</v>
-      </c>
-      <c r="I26" s="150" t="s">
+      <c r="I26" s="165" t="s">
         <v>122</v>
       </c>
-      <c r="J26" s="150" t="s">
-        <v>169</v>
-      </c>
-      <c r="K26" s="141"/>
-      <c r="L26" s="148"/>
-      <c r="M26" s="131" t="s">
+      <c r="J26" s="165" t="s">
+        <v>170</v>
+      </c>
+      <c r="K26" s="166"/>
+      <c r="L26" s="167"/>
+      <c r="M26" s="164" t="s">
+        <v>167</v>
+      </c>
+      <c r="N26" s="164" t="s">
         <v>166</v>
       </c>
-      <c r="N26" s="131" t="s">
-        <v>165</v>
-      </c>
-      <c r="O26" s="131" t="s">
-        <v>167</v>
-      </c>
-      <c r="P26" s="151" t="s">
+      <c r="O26" s="164" t="s">
+        <v>168</v>
+      </c>
+      <c r="P26" s="168" t="s">
         <v>122</v>
       </c>
-      <c r="Q26" s="151" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C27" s="128">
+      <c r="Q26" s="168" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="169">
         <v>-5</v>
       </c>
-      <c r="D27" s="132" t="s">
-        <v>161</v>
-      </c>
-      <c r="E27" s="133"/>
-      <c r="F27" s="143">
+      <c r="D27" s="170" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="171"/>
+      <c r="F27" s="172">
         <v>-58415.730470000002</v>
       </c>
-      <c r="G27" s="134">
+      <c r="G27" s="173">
         <f>F27-$F$28</f>
         <v>-61715.791369999999</v>
       </c>
-      <c r="H27" s="144">
+      <c r="H27" s="174">
         <f>D27/G27</f>
         <v>8.1044087566076682E-5</v>
       </c>
-      <c r="I27" s="144">
+      <c r="I27" s="174">
         <f>(G27)*$H$39</f>
         <v>-4.9915767788996455</v>
       </c>
-      <c r="J27" s="144">
+      <c r="J27" s="174">
         <f>D27-I27</f>
         <v>-1.0123221100354129E-2</v>
       </c>
-      <c r="L27" s="143">
+      <c r="L27" s="172">
         <v>802915</v>
       </c>
-      <c r="M27" s="134">
+      <c r="M27" s="173">
         <f>L27</f>
         <v>802915</v>
       </c>
-      <c r="N27" s="134">
+      <c r="N27" s="173">
         <f>M27-$M$28</f>
         <v>112432</v>
       </c>
-      <c r="O27" s="144">
+      <c r="O27" s="174">
         <f>D27/N27</f>
         <v>-4.448644514017361E-5</v>
       </c>
-      <c r="P27" s="134">
+      <c r="P27" s="173">
         <f>N27*$O$39</f>
         <v>-5.0045048311745859</v>
       </c>
-      <c r="Q27" s="144">
+      <c r="Q27" s="174">
         <f>D27-P27</f>
         <v>2.8048311745862975E-3</v>
       </c>
     </row>
-    <row r="28" spans="3:26" ht="51" x14ac:dyDescent="0.2">
-      <c r="C28" s="87">
+    <row r="28" spans="2:26" s="151" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="C28" s="175">
         <v>0</v>
       </c>
-      <c r="D28" s="53">
+      <c r="D28" s="176">
         <v>0</v>
       </c>
-      <c r="E28" s="136" t="s">
-        <v>162</v>
-      </c>
-      <c r="F28" s="143">
+      <c r="E28" s="177" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" s="172">
         <v>3300.0608999999999</v>
       </c>
-      <c r="G28" s="134">
+      <c r="G28" s="173">
         <f>F28-$F$28</f>
         <v>0</v>
       </c>
-      <c r="H28" s="144"/>
-      <c r="I28" s="144">
+      <c r="H28" s="174"/>
+      <c r="I28" s="174">
         <f>(G28)*$H$39</f>
         <v>0</v>
       </c>
-      <c r="J28" s="144">
+      <c r="J28" s="174">
         <f>D28-I28</f>
         <v>0</v>
       </c>
-      <c r="L28" s="143">
+      <c r="L28" s="172">
         <v>690483</v>
       </c>
-      <c r="M28" s="134">
+      <c r="M28" s="173">
         <f>L28</f>
         <v>690483</v>
       </c>
-      <c r="N28" s="134">
+      <c r="N28" s="173">
         <f>M28-$M$28</f>
         <v>0</v>
       </c>
-      <c r="O28" s="144"/>
-      <c r="P28" s="134">
+      <c r="O28" s="174"/>
+      <c r="P28" s="173">
         <f>N28*$O$39</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="144"/>
-    </row>
-    <row r="29" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C29" s="87">
+      <c r="Q28" s="174"/>
+    </row>
+    <row r="29" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="175">
         <v>5</v>
       </c>
-      <c r="D29" s="53">
+      <c r="D29" s="176">
         <v>4.9725000000000001</v>
       </c>
-      <c r="E29" s="134"/>
-      <c r="F29" s="143">
+      <c r="E29" s="173"/>
+      <c r="F29" s="172">
         <v>65015.796090000003</v>
       </c>
-      <c r="G29" s="134">
+      <c r="G29" s="173">
         <f>F29-$F$28</f>
         <v>61715.735190000007</v>
       </c>
-      <c r="H29" s="144">
+      <c r="H29" s="174">
         <f>D29/G29</f>
         <v>8.0571024305090179E-5</v>
       </c>
-      <c r="I29" s="144">
+      <c r="I29" s="174">
         <f>(G29)*$H$39</f>
         <v>4.9915722350579932</v>
       </c>
-      <c r="J29" s="144">
+      <c r="J29" s="174">
         <f>D29-I29</f>
         <v>-1.9072235057993048E-2</v>
       </c>
-      <c r="L29" s="143">
+      <c r="L29" s="172">
         <v>578788</v>
       </c>
-      <c r="M29" s="134">
+      <c r="M29" s="173">
         <f>L29</f>
         <v>578788</v>
       </c>
-      <c r="N29" s="134">
+      <c r="N29" s="173">
         <f>M29-$M$28</f>
         <v>-111695</v>
       </c>
-      <c r="O29" s="144">
+      <c r="O29" s="174">
         <f>D29/N29</f>
         <v>-4.4518554993509113E-5</v>
       </c>
-      <c r="P29" s="134">
+      <c r="P29" s="173">
         <f>N29*$O$39</f>
         <v>4.9716999352323654</v>
       </c>
-      <c r="Q29" s="144">
+      <c r="Q29" s="174">
         <f>D29-P29</f>
         <v>8.0006476763472278E-4</v>
       </c>
     </row>
-    <row r="30" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C30" s="87">
+    <row r="30" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="175">
         <v>10</v>
       </c>
-      <c r="D30" s="53">
+      <c r="D30" s="176">
         <v>9.9755000000000003</v>
       </c>
-      <c r="E30" s="134"/>
-      <c r="F30" s="143">
+      <c r="E30" s="173"/>
+      <c r="F30" s="172">
         <v>126731.6297</v>
       </c>
-      <c r="G30" s="134">
+      <c r="G30" s="173">
         <f>F30-$F$28</f>
         <v>123431.56880000001</v>
       </c>
-      <c r="H30" s="144">
+      <c r="H30" s="174">
         <f>D30/G30</f>
         <v>8.0818060541413121E-5</v>
       </c>
-      <c r="I30" s="144">
+      <c r="I30" s="174">
         <f>(G30)*$H$39</f>
         <v>9.983152430331284</v>
       </c>
-      <c r="J30" s="144">
+      <c r="J30" s="174">
         <f>D30-I30</f>
         <v>-7.6524303312837105E-3</v>
       </c>
-      <c r="L30" s="143">
+      <c r="L30" s="172">
         <v>466368</v>
       </c>
-      <c r="M30" s="134">
+      <c r="M30" s="173">
         <f>L30</f>
         <v>466368</v>
       </c>
-      <c r="N30" s="134">
+      <c r="N30" s="173">
         <f>M30-$M$28</f>
         <v>-224115</v>
       </c>
-      <c r="O30" s="144">
+      <c r="O30" s="174">
         <f>D30/N30</f>
         <v>-4.4510630702987306E-5</v>
       </c>
-      <c r="P30" s="134">
+      <c r="P30" s="173">
         <f>N30*$O$39</f>
         <v>9.9756706297023285</v>
       </c>
-      <c r="Q30" s="144">
+      <c r="Q30" s="174">
         <f>D30-P30</f>
         <v>-1.7062970232828434E-4</v>
       </c>
     </row>
-    <row r="31" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C31" s="87">
+    <row r="31" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="175">
         <v>15</v>
       </c>
-      <c r="D31" s="53"/>
-      <c r="E31" s="134"/>
-      <c r="F31" s="143"/>
-      <c r="G31" s="134"/>
-      <c r="H31" s="144"/>
-      <c r="I31" s="144"/>
-      <c r="J31" s="144"/>
-      <c r="L31" s="143"/>
-      <c r="M31" s="134"/>
-      <c r="N31" s="134"/>
-      <c r="O31" s="144"/>
-      <c r="P31" s="134"/>
-      <c r="Q31" s="144"/>
-    </row>
-    <row r="32" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="C32" s="87">
+      <c r="D31" s="176"/>
+      <c r="E31" s="173"/>
+      <c r="F31" s="172"/>
+      <c r="G31" s="173"/>
+      <c r="H31" s="174"/>
+      <c r="I31" s="174"/>
+      <c r="J31" s="174"/>
+      <c r="L31" s="172"/>
+      <c r="M31" s="173"/>
+      <c r="N31" s="173"/>
+      <c r="O31" s="174"/>
+      <c r="P31" s="173"/>
+      <c r="Q31" s="174"/>
+    </row>
+    <row r="32" spans="2:26" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="175">
         <v>20</v>
       </c>
-      <c r="D32" s="111"/>
-      <c r="E32" s="135"/>
-      <c r="F32" s="143"/>
-      <c r="G32" s="134"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="144"/>
-      <c r="J32" s="144"/>
-      <c r="L32" s="143"/>
-      <c r="M32" s="134"/>
-      <c r="N32" s="134"/>
-      <c r="O32" s="144"/>
-      <c r="P32" s="134"/>
-      <c r="Q32" s="144"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C33" s="87">
+      <c r="D32" s="178"/>
+      <c r="E32" s="179"/>
+      <c r="F32" s="172"/>
+      <c r="G32" s="173"/>
+      <c r="H32" s="174"/>
+      <c r="I32" s="174"/>
+      <c r="J32" s="174"/>
+      <c r="L32" s="172"/>
+      <c r="M32" s="173"/>
+      <c r="N32" s="173"/>
+      <c r="O32" s="174"/>
+      <c r="P32" s="173"/>
+      <c r="Q32" s="174"/>
+    </row>
+    <row r="33" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="175">
         <v>25</v>
       </c>
-      <c r="D33" s="53"/>
-      <c r="E33" s="134"/>
-      <c r="F33" s="143"/>
-      <c r="G33" s="134"/>
-      <c r="H33" s="144"/>
-      <c r="I33" s="144"/>
-      <c r="J33" s="144"/>
-      <c r="L33" s="143"/>
-      <c r="M33" s="134"/>
-      <c r="N33" s="134"/>
-      <c r="O33" s="144"/>
-      <c r="P33" s="134"/>
-      <c r="Q33" s="144"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C34" s="87">
+      <c r="D33" s="176"/>
+      <c r="E33" s="173"/>
+      <c r="F33" s="172"/>
+      <c r="G33" s="173"/>
+      <c r="H33" s="174"/>
+      <c r="I33" s="174"/>
+      <c r="J33" s="174"/>
+      <c r="L33" s="172"/>
+      <c r="M33" s="173"/>
+      <c r="N33" s="173"/>
+      <c r="O33" s="174"/>
+      <c r="P33" s="173"/>
+      <c r="Q33" s="174"/>
+    </row>
+    <row r="34" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="175">
         <v>30</v>
       </c>
-      <c r="D34" s="53"/>
-      <c r="E34" s="134"/>
-      <c r="F34" s="143"/>
-      <c r="G34" s="134"/>
-      <c r="H34" s="144"/>
-      <c r="I34" s="144"/>
-      <c r="J34" s="144"/>
-      <c r="L34" s="143"/>
-      <c r="M34" s="134"/>
-      <c r="N34" s="134"/>
-      <c r="O34" s="144"/>
-      <c r="P34" s="134"/>
-      <c r="Q34" s="144"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C35" s="87">
+      <c r="D34" s="176"/>
+      <c r="E34" s="173"/>
+      <c r="F34" s="172"/>
+      <c r="G34" s="173"/>
+      <c r="H34" s="174"/>
+      <c r="I34" s="174"/>
+      <c r="J34" s="174"/>
+      <c r="L34" s="172"/>
+      <c r="M34" s="173"/>
+      <c r="N34" s="173"/>
+      <c r="O34" s="174"/>
+      <c r="P34" s="173"/>
+      <c r="Q34" s="174"/>
+    </row>
+    <row r="35" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="175">
         <v>35</v>
       </c>
-      <c r="D35" s="53">
+      <c r="D35" s="176">
         <v>34.9801</v>
       </c>
-      <c r="E35" s="134"/>
-      <c r="F35" s="143">
+      <c r="E35" s="173"/>
+      <c r="F35" s="172">
         <v>435310.86090000003</v>
       </c>
-      <c r="G35" s="134">
+      <c r="G35" s="173">
         <f>F35-$F$28</f>
         <v>432010.80000000005</v>
       </c>
-      <c r="H35" s="144">
+      <c r="H35" s="174">
         <f>D35/G35</f>
         <v>8.0970429442967615E-5</v>
       </c>
-      <c r="I35" s="144">
+      <c r="I35" s="174">
         <f>(G35)*$H$39</f>
         <v>34.941058514273401</v>
       </c>
-      <c r="J35" s="144">
+      <c r="J35" s="174">
         <f>D35-I35</f>
         <v>3.904148572659949E-2</v>
       </c>
-      <c r="L35" s="143">
+      <c r="L35" s="172">
         <v>2147388488</v>
       </c>
-      <c r="M35" s="134">
+      <c r="M35" s="173">
         <f>L35-2147483648</f>
         <v>-95160</v>
       </c>
-      <c r="N35" s="134">
+      <c r="N35" s="173">
         <f>M35-$M$28</f>
         <v>-785643</v>
       </c>
-      <c r="O35" s="144">
+      <c r="O35" s="174">
         <f>D35/N35</f>
         <v>-4.4524166828954117E-5</v>
       </c>
-      <c r="P35" s="134">
+      <c r="P35" s="173">
         <f>N35*$O$39</f>
         <v>34.970063585798485</v>
       </c>
-      <c r="Q35" s="144">
+      <c r="Q35" s="174">
         <f>D35-P35</f>
         <v>1.0036414201515242E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C36" s="90">
+    <row r="36" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="180">
         <v>40</v>
       </c>
-      <c r="D36" s="127"/>
-      <c r="E36" s="134"/>
-      <c r="F36" s="143"/>
-      <c r="G36" s="134"/>
-      <c r="H36" s="144"/>
-      <c r="I36" s="144"/>
-      <c r="J36" s="144"/>
-      <c r="L36" s="143"/>
-      <c r="M36" s="134"/>
-      <c r="N36" s="134"/>
-      <c r="O36" s="144"/>
-      <c r="P36" s="134"/>
-      <c r="Q36" s="144"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C37" s="90">
+      <c r="D36" s="181"/>
+      <c r="E36" s="173"/>
+      <c r="F36" s="172"/>
+      <c r="G36" s="173"/>
+      <c r="H36" s="174"/>
+      <c r="I36" s="174"/>
+      <c r="J36" s="174"/>
+      <c r="L36" s="172"/>
+      <c r="M36" s="173"/>
+      <c r="N36" s="173"/>
+      <c r="O36" s="174"/>
+      <c r="P36" s="173"/>
+      <c r="Q36" s="174"/>
+    </row>
+    <row r="37" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="180">
         <v>45</v>
       </c>
-      <c r="D37" s="127">
+      <c r="D37" s="181">
         <v>44.988999999999997</v>
       </c>
-      <c r="E37" s="134"/>
-      <c r="F37" s="143">
+      <c r="E37" s="173"/>
+      <c r="F37" s="172">
         <v>558742.5281</v>
       </c>
-      <c r="G37" s="134">
+      <c r="G37" s="173">
         <f>F37-$F$28</f>
         <v>555442.46719999996</v>
       </c>
-      <c r="H37" s="144">
+      <c r="H37" s="174">
         <f>D37/G37</f>
         <v>8.0996687607972658E-5</v>
       </c>
-      <c r="I37" s="144">
+      <c r="I37" s="174">
         <f>(G37)*$H$39</f>
         <v>44.924218903202373</v>
       </c>
-      <c r="J37" s="144">
+      <c r="J37" s="174">
         <f>D37-I37</f>
         <v>6.4781096797624116E-2</v>
       </c>
-      <c r="L37" s="143">
+      <c r="L37" s="172">
         <v>2147163532</v>
       </c>
-      <c r="M37" s="134">
+      <c r="M37" s="173">
         <f>L37-2147483648</f>
         <v>-320116</v>
       </c>
-      <c r="N37" s="134">
+      <c r="N37" s="173">
         <f>M37-$M$28</f>
         <v>-1010599</v>
       </c>
-      <c r="O37" s="144">
+      <c r="O37" s="174">
         <f>D37/N37</f>
         <v>-4.4517162593669689E-5</v>
       </c>
-      <c r="P37" s="134">
+      <c r="P37" s="173">
         <f>N37*$O$39</f>
         <v>44.983168296216427</v>
       </c>
-      <c r="Q37" s="144">
+      <c r="Q37" s="174">
         <f>D37-P37</f>
         <v>5.8317037835706742E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="88" t="s">
+    <row r="38" spans="3:17" s="151" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="182" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="56"/>
-      <c r="E38" s="134"/>
-      <c r="F38" s="143"/>
-      <c r="G38" s="134"/>
-      <c r="H38" s="144"/>
-      <c r="I38" s="144"/>
-      <c r="J38" s="144"/>
-      <c r="L38" s="143"/>
-      <c r="M38" s="134"/>
-      <c r="N38" s="134"/>
-      <c r="O38" s="144"/>
-      <c r="P38" s="134"/>
-      <c r="Q38" s="144"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F39" s="143"/>
-      <c r="G39" s="134" t="s">
-        <v>168</v>
-      </c>
-      <c r="H39" s="144">
+      <c r="D38" s="183"/>
+      <c r="E38" s="173"/>
+      <c r="F38" s="172"/>
+      <c r="G38" s="173"/>
+      <c r="H38" s="174"/>
+      <c r="I38" s="174"/>
+      <c r="J38" s="174"/>
+      <c r="L38" s="172"/>
+      <c r="M38" s="173"/>
+      <c r="N38" s="173"/>
+      <c r="O38" s="174"/>
+      <c r="P38" s="173"/>
+      <c r="Q38" s="174"/>
+    </row>
+    <row r="39" spans="3:17" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F39" s="172"/>
+      <c r="G39" s="173" t="s">
+        <v>169</v>
+      </c>
+      <c r="H39" s="174">
         <f>AVERAGE(H27:H37)</f>
         <v>8.0880057892704057E-5</v>
       </c>
-      <c r="I39" s="144"/>
-      <c r="J39" s="144"/>
-      <c r="L39" s="143"/>
-      <c r="M39" s="134"/>
-      <c r="N39" s="134" t="s">
-        <v>168</v>
-      </c>
-      <c r="O39" s="144">
+      <c r="I39" s="174"/>
+      <c r="J39" s="174"/>
+      <c r="L39" s="172"/>
+      <c r="M39" s="173"/>
+      <c r="N39" s="173" t="s">
+        <v>169</v>
+      </c>
+      <c r="O39" s="174">
         <f>AVERAGE(O27:O37)</f>
         <v>-4.4511392051858772E-5</v>
       </c>
-      <c r="P39" s="134"/>
-      <c r="Q39" s="144"/>
-    </row>
-    <row r="40" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F40" s="145"/>
-      <c r="G40" s="146" t="s">
-        <v>165</v>
-      </c>
-      <c r="H40" s="147">
+      <c r="P39" s="173"/>
+      <c r="Q39" s="174"/>
+    </row>
+    <row r="40" spans="3:17" s="151" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="184"/>
+      <c r="G40" s="185" t="s">
+        <v>166</v>
+      </c>
+      <c r="H40" s="186">
         <f>-F28</f>
         <v>-3300.0608999999999</v>
       </c>
-      <c r="I40" s="147"/>
-      <c r="J40" s="147"/>
-      <c r="L40" s="145"/>
-      <c r="M40" s="146"/>
-      <c r="N40" s="146" t="s">
-        <v>165</v>
-      </c>
-      <c r="O40" s="147">
+      <c r="I40" s="186"/>
+      <c r="J40" s="186"/>
+      <c r="L40" s="184"/>
+      <c r="M40" s="185"/>
+      <c r="N40" s="185" t="s">
+        <v>166</v>
+      </c>
+      <c r="O40" s="186">
         <f>-M28</f>
         <v>-690483</v>
       </c>
-      <c r="P40" s="146"/>
-      <c r="Q40" s="147"/>
-    </row>
-    <row r="45" spans="1:17" s="158" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A45" s="158" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P40" s="185"/>
+      <c r="Q40" s="186"/>
+    </row>
+    <row r="46" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C47" s="104" t="s">
         <v>61</v>
       </c>
@@ -5608,283 +5661,314 @@
       <c r="E47" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="138" t="s">
-        <v>174</v>
+      <c r="F47" s="134" t="s">
+        <v>175</v>
       </c>
       <c r="G47" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="H47" s="137" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C48" s="129" t="s">
+      <c r="H47" s="101" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C48" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="D48" s="130"/>
-      <c r="E48" s="130"/>
-      <c r="F48" s="130"/>
-      <c r="G48" s="130"/>
+      <c r="D48" s="129" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" s="129"/>
+      <c r="F48" s="129"/>
+      <c r="G48" s="129"/>
       <c r="H48" s="130"/>
     </row>
-    <row r="49" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C49" s="128">
+    <row r="49" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="127">
         <v>-5</v>
       </c>
-      <c r="D49" s="132" t="s">
-        <v>161</v>
-      </c>
-      <c r="E49" s="132" t="s">
-        <v>175</v>
-      </c>
-      <c r="F49" s="130">
+      <c r="D49" s="192">
+        <v>-5.0016999999999996</v>
+      </c>
+      <c r="E49" s="192">
+        <v>-5.0111989056178103</v>
+      </c>
+      <c r="F49" s="193">
         <f>ABS(D49-E49)</f>
-        <v>9.4989056000001071E-3</v>
-      </c>
-      <c r="G49" s="132" t="s">
-        <v>176</v>
-      </c>
-      <c r="H49" s="137">
-        <f t="shared" ref="H49:H59" si="2">ABS(D49-G49)</f>
-        <v>2.6320600000007133E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="3:14" x14ac:dyDescent="0.2">
+        <v>9.4989056178107489E-3</v>
+      </c>
+      <c r="G49" s="192">
+        <v>-5.0043320620675003</v>
+      </c>
+      <c r="H49" s="197">
+        <f t="shared" ref="H49:H60" si="2">ABS(D49-G49)</f>
+        <v>2.6320620675006623E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C50" s="87">
         <v>0</v>
       </c>
-      <c r="D50" s="53">
+      <c r="D50" s="194">
         <v>0</v>
       </c>
-      <c r="E50" s="132" t="s">
-        <v>177</v>
-      </c>
-      <c r="F50" s="130">
-        <f t="shared" ref="F50:F59" si="3">ABS(D50-E50)</f>
-        <v>1.19267335E-2</v>
-      </c>
-      <c r="G50" s="132" t="s">
-        <v>178</v>
-      </c>
-      <c r="H50" s="137">
+      <c r="E50" s="194">
+        <v>-1.19267335010034E-2</v>
+      </c>
+      <c r="F50" s="193">
+        <f t="shared" ref="F50:F60" si="3">ABS(D50-E50)</f>
+        <v>1.19267335010034E-2</v>
+      </c>
+      <c r="G50" s="194">
+        <v>9.3083603649901604E-4</v>
+      </c>
+      <c r="H50" s="197">
         <f t="shared" si="2"/>
-        <v>9.3083602999999998E-4</v>
-      </c>
-      <c r="K50" s="134"/>
-      <c r="L50" s="134" t="s">
-        <v>172</v>
-      </c>
-      <c r="M50" s="134" t="s">
-        <v>165</v>
-      </c>
-      <c r="N50" s="134" t="s">
+        <v>9.3083603649901604E-4</v>
+      </c>
+      <c r="L50" s="143"/>
+      <c r="M50" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="N50" s="140" t="s">
+        <v>166</v>
+      </c>
+      <c r="O50" s="141" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C51" s="87">
         <v>5</v>
       </c>
-      <c r="D51" s="53">
+      <c r="D51" s="194">
         <v>4.9725000000000001</v>
       </c>
-      <c r="E51" s="132" t="s">
-        <v>179</v>
-      </c>
-      <c r="F51" s="130">
+      <c r="E51" s="194">
+        <v>4.9873340469257803</v>
+      </c>
+      <c r="F51" s="193">
         <f t="shared" si="3"/>
-        <v>1.4834046919999899E-2</v>
-      </c>
-      <c r="G51" s="132" t="s">
-        <v>180</v>
-      </c>
-      <c r="H51" s="137">
+        <v>1.4834046925780164E-2</v>
+      </c>
+      <c r="G51" s="194">
+        <v>4.9733838690139898</v>
+      </c>
+      <c r="H51" s="197">
         <f t="shared" si="2"/>
-        <v>8.8386899999992607E-4</v>
-      </c>
-      <c r="K51" s="134" t="s">
-        <v>170</v>
-      </c>
-      <c r="L51" s="134">
-        <v>8.1041246399999998E-5</v>
-      </c>
-      <c r="M51" s="134">
-        <v>-8.1453097600000003E-3</v>
-      </c>
-      <c r="N51" s="134">
+        <v>8.8386901398962436E-4</v>
+      </c>
+      <c r="L51" s="144" t="s">
+        <v>171</v>
+      </c>
+      <c r="M51" s="103">
+        <v>8.1004693299999996E-5</v>
+      </c>
+      <c r="N51" s="189">
+        <v>-0.279250575</v>
+      </c>
+      <c r="O51" s="187">
         <f>MAX(F49:F59)</f>
-        <v>1.4834046919999899E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="3:14" x14ac:dyDescent="0.2">
+        <v>1.4834046925780164E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C52" s="87">
         <v>10</v>
       </c>
-      <c r="D52" s="53">
+      <c r="D52" s="194">
         <v>9.9755000000000003</v>
       </c>
-      <c r="E52" s="132" t="s">
-        <v>181</v>
-      </c>
-      <c r="F52" s="130">
+      <c r="E52" s="194">
+        <v>9.98660622025767</v>
+      </c>
+      <c r="F52" s="193">
         <f t="shared" si="3"/>
-        <v>1.1106220000000278E-2</v>
-      </c>
-      <c r="G52" s="132" t="s">
-        <v>182</v>
-      </c>
-      <c r="H52" s="137">
+        <v>1.1106220257669719E-2</v>
+      </c>
+      <c r="G52" s="194">
+        <v>9.9781125495039902</v>
+      </c>
+      <c r="H52" s="197">
         <f t="shared" si="2"/>
-        <v>2.6125495000002275E-3</v>
-      </c>
-      <c r="K52" s="134" t="s">
-        <v>171</v>
-      </c>
-      <c r="L52" s="134">
-        <v>-4.4511401799999998E-5</v>
-      </c>
-      <c r="M52" s="134">
-        <v>30.7267127</v>
-      </c>
-      <c r="N52" s="134">
+        <v>2.6125495039899249E-3</v>
+      </c>
+      <c r="L52" s="145" t="s">
+        <v>172</v>
+      </c>
+      <c r="M52" s="56">
+        <v>-4.4518134500000001E-5</v>
+      </c>
+      <c r="N52" s="191">
+        <v>30.739945899999999</v>
+      </c>
+      <c r="O52" s="188">
         <f>MAX(H49:H59)</f>
-        <v>3.8084999999981051E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="3:14" x14ac:dyDescent="0.2">
+        <v>3.8084209800004487E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C53" s="87">
         <v>15</v>
       </c>
-      <c r="D53" s="53"/>
-      <c r="E53" s="132"/>
-      <c r="F53" s="130">
+      <c r="D53" s="194"/>
+      <c r="E53" s="194"/>
+      <c r="F53" s="193">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G53" s="132"/>
-      <c r="H53" s="137">
+      <c r="G53" s="194"/>
+      <c r="H53" s="197">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C54" s="87">
         <v>20</v>
       </c>
-      <c r="D54" s="111"/>
-      <c r="E54" s="132"/>
-      <c r="F54" s="130">
+      <c r="D54" s="195"/>
+      <c r="E54" s="195"/>
+      <c r="F54" s="193">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G54" s="132"/>
-      <c r="H54" s="137">
+      <c r="G54" s="195"/>
+      <c r="H54" s="197">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C55" s="87">
         <v>25</v>
       </c>
-      <c r="D55" s="53"/>
-      <c r="E55" s="132"/>
-      <c r="F55" s="130">
+      <c r="D55" s="194"/>
+      <c r="E55" s="194"/>
+      <c r="F55" s="193">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G55" s="132"/>
-      <c r="H55" s="137">
+      <c r="G55" s="194"/>
+      <c r="H55" s="197">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C56" s="87">
         <v>30</v>
       </c>
-      <c r="D56" s="53"/>
-      <c r="E56" s="132"/>
-      <c r="F56" s="130">
+      <c r="D56" s="194"/>
+      <c r="E56" s="194"/>
+      <c r="F56" s="193">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G56" s="132"/>
-      <c r="H56" s="137">
+      <c r="G56" s="194"/>
+      <c r="H56" s="197">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C57" s="87">
         <v>35</v>
       </c>
-      <c r="D57" s="53">
+      <c r="D57" s="194">
         <v>34.9801</v>
       </c>
-      <c r="E57" s="132" t="s">
-        <v>183</v>
-      </c>
-      <c r="F57" s="130">
+      <c r="E57" s="194">
+        <v>34.982972202363399</v>
+      </c>
+      <c r="F57" s="193">
         <f t="shared" si="3"/>
-        <v>2.8722022999971841E-3</v>
-      </c>
-      <c r="G57" s="132" t="s">
-        <v>184</v>
-      </c>
-      <c r="H57" s="137">
+        <v>2.8722023633989124E-3</v>
+      </c>
+      <c r="G57" s="194">
+        <v>34.97629157902</v>
+      </c>
+      <c r="H57" s="197">
         <f t="shared" si="2"/>
-        <v>3.8084999999981051E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="3:14" x14ac:dyDescent="0.2">
+        <v>3.8084209800004487E-3</v>
+      </c>
+      <c r="K57" s="139"/>
+    </row>
+    <row r="58" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C58" s="90">
         <v>40</v>
       </c>
-      <c r="D58" s="127"/>
-      <c r="E58" s="132"/>
-      <c r="F58" s="130">
+      <c r="D58" s="196"/>
+      <c r="E58" s="196"/>
+      <c r="F58" s="193">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G58" s="132"/>
-      <c r="H58" s="137">
+      <c r="G58" s="196"/>
+      <c r="H58" s="197">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C59" s="90">
         <v>45</v>
       </c>
-      <c r="D59" s="127">
+      <c r="D59" s="196">
         <v>44.988999999999997</v>
       </c>
-      <c r="E59" s="132" t="s">
-        <v>185</v>
-      </c>
-      <c r="F59" s="130">
+      <c r="E59" s="196">
+        <v>44.981516547407097</v>
+      </c>
+      <c r="F59" s="193">
         <f t="shared" si="3"/>
-        <v>7.483452599998941E-3</v>
-      </c>
-      <c r="G59" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="H59" s="137">
+        <v>7.483452592900619E-3</v>
+      </c>
+      <c r="G59" s="196">
+        <v>44.9909130436019</v>
+      </c>
+      <c r="H59" s="197">
         <f t="shared" si="2"/>
-        <v>1.913043000001835E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="3:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1.9130436019025865E-3</v>
+      </c>
+      <c r="J59" s="138"/>
+    </row>
+    <row r="60" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C60" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="D60" s="56"/>
-      <c r="E60" s="56"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="56"/>
+      <c r="D60" s="190"/>
+      <c r="E60" s="190"/>
+      <c r="F60" s="198">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G60" s="190"/>
+      <c r="H60" s="199">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L60" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="61" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="L61" t="s">
+        <v>180</v>
+      </c>
+      <c r="M61">
+        <f>M51/M11</f>
+        <v>0.99954895683835387</v>
+      </c>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="L62" t="s">
+        <v>181</v>
+      </c>
+      <c r="M62">
+        <f>M52/M12</f>
+        <v>1.0001512578738871</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5938,7 +6022,7 @@
       <c r="B4" s="116"/>
       <c r="C4" s="116"/>
       <c r="D4" s="116" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E4" s="116"/>
       <c r="F4" s="116"/>
@@ -6041,22 +6125,22 @@
         <v>111</v>
       </c>
       <c r="C12" s="121" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D12" s="122" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E12" s="122" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F12" s="122" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G12" s="122" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H12" s="123" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K12" s="95">
         <v>6</v>
@@ -6206,22 +6290,22 @@
         <v>111</v>
       </c>
       <c r="C20" s="121" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D20" s="122" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E20" s="122" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F20" s="122" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G20" s="122" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H20" s="123" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K20" s="95"/>
       <c r="L20" s="94"/>

</xml_diff>

<commit_message>
Update excel system repeatability table
</commit_message>
<xml_diff>
--- a/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
+++ b/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federicorojas/ecmc_bifrost_vac_tank_sat/docs/testplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0198AC8B-71C6-774C-B1C3-ADAA834497C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3914384D-DC1A-8842-BF9C-6817B8BBE72E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="16520" activeTab="6" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="183">
   <si>
     <t>General Inspection</t>
   </si>
@@ -573,39 +573,6 @@
     <t>-5,0177</t>
   </si>
   <si>
-    <t>-5,0168</t>
-  </si>
-  <si>
-    <t>-5,0185</t>
-  </si>
-  <si>
-    <t>-5,0184</t>
-  </si>
-  <si>
-    <t>-5,0197</t>
-  </si>
-  <si>
-    <t>-5,0196</t>
-  </si>
-  <si>
-    <t>-5,0073</t>
-  </si>
-  <si>
-    <t>-5,0064</t>
-  </si>
-  <si>
-    <t>-5,0065</t>
-  </si>
-  <si>
-    <t>-5,006</t>
-  </si>
-  <si>
-    <t>-5,0062</t>
-  </si>
-  <si>
-    <t>-5,0044</t>
-  </si>
-  <si>
     <t>Over 48,5 then collision with concrete</t>
   </si>
   <si>
@@ -700,14 +667,34 @@
   </si>
   <si>
     <t>Laser Scanner</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Repeatabilty</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>System repeatabilty</t>
+  </si>
+  <si>
+    <t>One value seems very high and could be a human error when taking the laser scanner data</t>
+  </si>
+  <si>
+    <t>Value of the system's repeatability without the possible outlier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -839,7 +826,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -876,8 +863,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="61">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -1645,11 +1650,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1930,6 +1948,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="60" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3568,7 +3608,7 @@
   <dimension ref="B2:S60"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3654,7 +3694,7 @@
         <v>934879</v>
       </c>
       <c r="F11" s="107" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="L11" s="93">
         <v>3</v>
@@ -3692,7 +3732,7 @@
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B14" s="84"/>
       <c r="C14" s="79" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D14" s="59" t="s">
         <v>53</v>
@@ -3741,10 +3781,10 @@
         <v>55</v>
       </c>
       <c r="J15" s="64" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="K15" s="63" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="L15" s="93"/>
       <c r="M15" s="92"/>
@@ -3908,7 +3948,7 @@
     <row r="23" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="84"/>
       <c r="C23" s="79" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D23" s="59" t="s">
         <v>53</v>
@@ -3957,10 +3997,10 @@
         <v>55</v>
       </c>
       <c r="J24" s="64" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="K24" s="63" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
@@ -4060,7 +4100,7 @@
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B32" s="84"/>
       <c r="C32" s="79" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D32" s="59" t="s">
         <v>53</v>
@@ -4101,10 +4141,10 @@
         <v>55</v>
       </c>
       <c r="J33" s="64" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="K33" s="63" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
@@ -4204,7 +4244,7 @@
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41" s="84"/>
       <c r="C41" s="79" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D41" s="59" t="s">
         <v>53</v>
@@ -4245,10 +4285,10 @@
         <v>55</v>
       </c>
       <c r="J42" s="64" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="K42" s="63" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -4389,10 +4429,10 @@
         <v>55</v>
       </c>
       <c r="J51" s="64" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="K51" s="63" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
@@ -4712,7 +4752,7 @@
   <dimension ref="B2:Z62"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4750,7 +4790,7 @@
     </row>
     <row r="5" spans="2:26" s="130" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E5" s="134" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -4768,13 +4808,13 @@
         <v>107</v>
       </c>
       <c r="F7" s="118" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="G7" s="99" t="s">
         <v>108</v>
       </c>
       <c r="H7" s="99" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="I7" s="117"/>
       <c r="J7" s="117"/>
@@ -4904,10 +4944,10 @@
       <c r="K10" s="116"/>
       <c r="L10" s="127"/>
       <c r="M10" s="126" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="N10" s="124" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="O10" s="125" t="s">
         <v>24</v>
@@ -4948,7 +4988,7 @@
       <c r="J11" s="115"/>
       <c r="K11" s="116"/>
       <c r="L11" s="128" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="M11" s="101">
         <v>8.1041246399999998E-5</v>
@@ -4996,7 +5036,7 @@
       <c r="J12" s="115"/>
       <c r="K12" s="116"/>
       <c r="L12" s="129" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="M12" s="55">
         <v>-4.4511401799999998E-5</v>
@@ -5323,7 +5363,7 @@
     <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="R21" s="93"/>
       <c r="S21" s="92" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="T21" s="92"/>
       <c r="U21" s="92"/>
@@ -5336,7 +5376,7 @@
       <c r="B22" s="134"/>
       <c r="D22" s="134"/>
       <c r="E22" s="134" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="R22" s="131"/>
       <c r="S22" s="132"/>
@@ -5359,7 +5399,7 @@
     </row>
     <row r="24" spans="2:26" s="135" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="135" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="2:26" s="135" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5370,7 +5410,7 @@
         <v>106</v>
       </c>
       <c r="E25" s="138" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="F25" s="139" t="s">
         <v>107</v>
@@ -5399,33 +5439,33 @@
       <c r="E26" s="147"/>
       <c r="F26" s="145"/>
       <c r="G26" s="147" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="H26" s="148" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="I26" s="149" t="s">
         <v>120</v>
       </c>
       <c r="J26" s="149" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="K26" s="150"/>
       <c r="L26" s="151"/>
       <c r="M26" s="148" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="N26" s="148" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="O26" s="148" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="P26" s="152" t="s">
         <v>120</v>
       </c>
       <c r="Q26" s="152" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="2:26" s="135" customFormat="1" x14ac:dyDescent="0.2">
@@ -5433,7 +5473,7 @@
         <v>-5</v>
       </c>
       <c r="D27" s="154" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E27" s="155"/>
       <c r="F27" s="156">
@@ -5487,7 +5527,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="161" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F28" s="156">
         <v>3300.0608999999999</v>
@@ -5838,7 +5878,7 @@
     <row r="39" spans="3:17" s="135" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F39" s="156"/>
       <c r="G39" s="157" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="H39" s="158">
         <f>AVERAGE(H27:H37)</f>
@@ -5849,7 +5889,7 @@
       <c r="L39" s="156"/>
       <c r="M39" s="157"/>
       <c r="N39" s="157" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="O39" s="158">
         <f>AVERAGE(O27:O37)</f>
@@ -5861,7 +5901,7 @@
     <row r="40" spans="3:17" s="135" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F40" s="168"/>
       <c r="G40" s="169" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="H40" s="170">
         <f>-F28</f>
@@ -5872,7 +5912,7 @@
       <c r="L40" s="168"/>
       <c r="M40" s="169"/>
       <c r="N40" s="169" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="O40" s="170">
         <f>-M28</f>
@@ -5883,7 +5923,7 @@
     </row>
     <row r="46" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5897,13 +5937,13 @@
         <v>107</v>
       </c>
       <c r="F47" s="118" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="G47" s="99" t="s">
         <v>108</v>
       </c>
       <c r="H47" s="99" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.2">
@@ -5963,10 +6003,10 @@
       </c>
       <c r="L50" s="127"/>
       <c r="M50" s="126" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="N50" s="124" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="O50" s="125" t="s">
         <v>24</v>
@@ -5994,7 +6034,7 @@
         <v>8.8386901398962436E-4</v>
       </c>
       <c r="L51" s="128" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="M51" s="101">
         <v>8.1004693299999996E-5</v>
@@ -6029,7 +6069,7 @@
         <v>2.6125495039899249E-3</v>
       </c>
       <c r="L52" s="129" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="M52" s="55">
         <v>-4.4518134500000001E-5</v>
@@ -6184,12 +6224,12 @@
         <v>0</v>
       </c>
       <c r="L60" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="3:15" x14ac:dyDescent="0.2">
       <c r="L61" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="M61">
         <f>M51/M11</f>
@@ -6198,7 +6238,7 @@
     </row>
     <row r="62" spans="3:15" x14ac:dyDescent="0.2">
       <c r="L62" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="M62">
         <f>M52/M12</f>
@@ -6212,15 +6252,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F11942-15E9-084A-9037-102332C5B852}">
-  <dimension ref="B2:X138"/>
+  <dimension ref="B2:X151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -6258,7 +6298,7 @@
       <c r="B4" s="104"/>
       <c r="C4" s="104"/>
       <c r="D4" s="104" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="E4" s="104"/>
       <c r="F4" s="104"/>
@@ -6278,7 +6318,7 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B6" s="104" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C6" s="104"/>
       <c r="D6" s="104">
@@ -6329,7 +6369,7 @@
         <v>109</v>
       </c>
       <c r="C10" s="187" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D10" s="187" t="s">
         <v>52</v>
@@ -6337,8 +6377,15 @@
       <c r="E10" s="188" t="s">
         <v>51</v>
       </c>
-      <c r="L10" s="93"/>
-      <c r="M10" s="92"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="207" t="s">
+        <v>180</v>
+      </c>
+      <c r="H10" s="208"/>
+      <c r="L10" s="213"/>
+      <c r="M10" s="92" t="s">
+        <v>181</v>
+      </c>
       <c r="N10" s="92"/>
       <c r="O10" s="92"/>
       <c r="P10" s="92"/>
@@ -6350,8 +6397,8 @@
       <c r="B11" s="184">
         <v>1</v>
       </c>
-      <c r="C11" s="189" t="s">
-        <v>145</v>
+      <c r="C11" s="194">
+        <v>-5.0167999999999999</v>
       </c>
       <c r="D11" s="190">
         <v>-5.0096773752999999</v>
@@ -6359,8 +6406,14 @@
       <c r="E11" s="191">
         <v>-5.0100229199999999</v>
       </c>
-      <c r="L11" s="93"/>
-      <c r="M11" s="92"/>
+      <c r="G11" s="212">
+        <f>MAX(C19,C31,C43,C55,C67,C79,C91,C103,C115,C127,C139,C151)</f>
+        <v>1.0099999999999554E-2</v>
+      </c>
+      <c r="L11" s="215"/>
+      <c r="M11" s="92" t="s">
+        <v>182</v>
+      </c>
       <c r="N11" s="92"/>
       <c r="O11" s="92"/>
       <c r="P11" s="92"/>
@@ -6372,14 +6425,18 @@
       <c r="B12" s="185">
         <v>2</v>
       </c>
-      <c r="C12" s="192" t="s">
-        <v>146</v>
+      <c r="C12" s="195">
+        <v>-5.0185000000000004</v>
       </c>
       <c r="D12" s="52">
         <v>-5.0096768055999998</v>
       </c>
       <c r="E12" s="58">
         <v>-5.0102009699999996</v>
+      </c>
+      <c r="G12" s="214">
+        <f>MAX(C19,C31,C43,C55,C79,C91,C103,C115,C127,C139,C151)</f>
+        <v>8.8000000000008072E-3</v>
       </c>
       <c r="L12" s="93"/>
       <c r="M12" s="92"/>
@@ -6394,8 +6451,8 @@
       <c r="B13" s="185">
         <v>3</v>
       </c>
-      <c r="C13" s="192" t="s">
-        <v>147</v>
+      <c r="C13" s="195">
+        <v>-5.0183999999999997</v>
       </c>
       <c r="D13" s="52">
         <v>-5.0096773752999999</v>
@@ -6416,8 +6473,8 @@
       <c r="B14" s="185">
         <v>4</v>
       </c>
-      <c r="C14" s="192" t="s">
-        <v>148</v>
+      <c r="C14" s="195">
+        <v>-5.0197000000000003</v>
       </c>
       <c r="D14" s="52">
         <v>-5.0096768055999998</v>
@@ -6438,8 +6495,8 @@
       <c r="B15" s="185">
         <v>5</v>
       </c>
-      <c r="C15" s="192" t="s">
-        <v>149</v>
+      <c r="C15" s="195">
+        <v>-5.0195999999999996</v>
       </c>
       <c r="D15" s="52">
         <v>-5.0096773752999999</v>
@@ -6460,13 +6517,13 @@
       <c r="B16" s="186">
         <v>6</v>
       </c>
-      <c r="C16" s="193" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="56">
+      <c r="C16" s="199">
+        <v>-5.0195999999999996</v>
+      </c>
+      <c r="D16" s="200">
         <v>-5.0096773752999999</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="201">
         <v>-5.0107796200000001</v>
       </c>
       <c r="L16" s="93"/>
@@ -6479,6 +6536,21 @@
       <c r="S16" s="94"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="202">
+        <f>MAX(C11:C16)-MIN(C11:C16)</f>
+        <v>2.9000000000003467E-3</v>
+      </c>
+      <c r="D17" s="203">
+        <f>MAX(D11:D16)-MIN(D11:D16)</f>
+        <v>5.6970000006373311E-7</v>
+      </c>
+      <c r="E17" s="204">
+        <f>MAX(E11:E16)-MIN(E11:E16)</f>
+        <v>8.9023000000043595E-4</v>
+      </c>
       <c r="L17" s="93"/>
       <c r="M17" s="92"/>
       <c r="N17" s="92"/>
@@ -6489,6 +6561,21 @@
       <c r="S17" s="94"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B18" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="205">
+        <f>STDEV(C11:C16)</f>
+        <v>1.1254628677422305E-3</v>
+      </c>
+      <c r="D18" s="52">
+        <f>STDEV(D11:D16)</f>
+        <v>2.9419181501082702E-7</v>
+      </c>
+      <c r="E18" s="58">
+        <f>STDEV(E11:E16)</f>
+        <v>3.3859959980799518E-4</v>
+      </c>
       <c r="L18" s="93"/>
       <c r="M18" s="92"/>
       <c r="N18" s="92"/>
@@ -6498,7 +6585,16 @@
       <c r="R18" s="92"/>
       <c r="S18" s="94"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="206">
+        <f>MAX(C17:E17)</f>
+        <v>2.9000000000003467E-3</v>
+      </c>
+      <c r="D19" s="56"/>
+      <c r="E19" s="54"/>
       <c r="L19" s="93"/>
       <c r="M19" s="92"/>
       <c r="N19" s="92"/>
@@ -6508,16 +6604,7 @@
       <c r="R19" s="92"/>
       <c r="S19" s="94"/>
     </row>
-    <row r="20" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="104" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="105" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="104" t="s">
-        <v>112</v>
-      </c>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="L20" s="93"/>
       <c r="M20" s="92"/>
       <c r="N20" s="92"/>
@@ -6528,17 +6615,14 @@
       <c r="S20" s="94"/>
     </row>
     <row r="21" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D21" s="187" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="188" t="s">
-        <v>51</v>
+      <c r="B21" s="104" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="104" t="s">
+        <v>112</v>
       </c>
       <c r="L21" s="93"/>
       <c r="M21" s="92"/>
@@ -6550,421 +6634,502 @@
       <c r="S21" s="94"/>
     </row>
     <row r="22" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="184">
+      <c r="B22" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="187" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="188" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" s="93"/>
+      <c r="M22" s="92"/>
+      <c r="N22" s="92"/>
+      <c r="O22" s="92"/>
+      <c r="P22" s="92"/>
+      <c r="Q22" s="92"/>
+      <c r="R22" s="92"/>
+      <c r="S22" s="94"/>
+    </row>
+    <row r="23" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="184">
         <v>1</v>
       </c>
-      <c r="C22" s="189" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="190">
+      <c r="C23" s="194">
+        <v>-5.0072999999999999</v>
+      </c>
+      <c r="D23" s="190">
         <v>-5.0096699600000001</v>
       </c>
-      <c r="E22" s="191">
+      <c r="E23" s="191">
         <v>-4.9966695000000003</v>
       </c>
-      <c r="L22" s="95"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="96"/>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="96"/>
-      <c r="S22" s="97"/>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="185">
-        <v>2</v>
-      </c>
-      <c r="C23" s="192" t="s">
-        <v>151</v>
-      </c>
-      <c r="D23" s="52">
-        <v>-5.0096699600000001</v>
-      </c>
-      <c r="E23" s="58">
-        <v>-4.9970701100000001</v>
-      </c>
+      <c r="L23" s="95"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="96"/>
+      <c r="R23" s="96"/>
+      <c r="S23" s="97"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B24" s="185">
-        <v>3</v>
-      </c>
-      <c r="C24" s="192" t="s">
-        <v>152</v>
+        <v>2</v>
+      </c>
+      <c r="C24" s="195">
+        <v>-5.0064000000000002</v>
       </c>
       <c r="D24" s="52">
         <v>-5.0096699600000001</v>
       </c>
       <c r="E24" s="58">
-        <v>-4.99684755</v>
+        <v>-4.9970701100000001</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B25" s="185">
-        <v>4</v>
-      </c>
-      <c r="C25" s="192" t="s">
-        <v>153</v>
+        <v>3</v>
+      </c>
+      <c r="C25" s="195">
+        <v>-5.0065</v>
       </c>
       <c r="D25" s="52">
         <v>-5.0096699600000001</v>
       </c>
       <c r="E25" s="58">
-        <v>-4.9967140099999998</v>
+        <v>-4.99684755</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B26" s="185">
-        <v>5</v>
-      </c>
-      <c r="C26" s="192" t="s">
-        <v>154</v>
+        <v>4</v>
+      </c>
+      <c r="C26" s="195">
+        <v>-5.0060000000000002</v>
       </c>
       <c r="D26" s="52">
         <v>-5.0096699600000001</v>
       </c>
       <c r="E26" s="58">
+        <v>-4.9967140099999998</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B27" s="185">
+        <v>5</v>
+      </c>
+      <c r="C27" s="195">
+        <v>-5.0061999999999998</v>
+      </c>
+      <c r="D27" s="52">
+        <v>-5.0096699600000001</v>
+      </c>
+      <c r="E27" s="58">
         <v>-4.99653597</v>
       </c>
     </row>
-    <row r="27" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="186">
+    <row r="28" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="186">
         <v>6</v>
       </c>
-      <c r="C27" s="193" t="s">
-        <v>155</v>
-      </c>
-      <c r="D27" s="56">
+      <c r="C28" s="196">
+        <v>-5.0044000000000004</v>
+      </c>
+      <c r="D28" s="56">
         <v>-5.0096699600000001</v>
       </c>
-      <c r="E27" s="54">
+      <c r="E28" s="54">
         <v>-4.9964914599999997</v>
       </c>
     </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B29" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="202">
+        <f>MAX(C23:C28)-MIN(C23:C28)</f>
+        <v>2.8999999999994586E-3</v>
+      </c>
+      <c r="D29" s="203">
+        <f>MAX(D23:D28)-MIN(D23:D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="204">
+        <f>MAX(E23:E28)-MIN(E23:E28)</f>
+        <v>5.7865000000045796E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B30" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C30" s="205">
+        <f>STDEV(C23:C28)</f>
+        <v>9.584710046038515E-4</v>
+      </c>
+      <c r="D30" s="52">
+        <f>STDEV(D23:D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="58">
+        <f>STDEV(E23:E28)</f>
+        <v>2.1331544272908644E-4</v>
+      </c>
+    </row>
     <row r="31" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="104" t="s">
+      <c r="B31" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" s="206">
+        <f>MAX(C29:E29)</f>
+        <v>2.8999999999994586E-3</v>
+      </c>
+      <c r="D31" s="56"/>
+      <c r="E31" s="54"/>
+    </row>
+    <row r="33" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="105" t="s">
+      <c r="C33" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="104" t="s">
+      <c r="D33" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="J31" s="104"/>
-    </row>
-    <row r="32" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="70" t="s">
+      <c r="J33" s="104"/>
+    </row>
+    <row r="34" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D32" s="187" t="s">
+      <c r="C34" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="188" t="s">
+      <c r="E34" s="188" t="s">
         <v>51</v>
       </c>
-      <c r="J32" s="105"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="184">
+      <c r="J34" s="105"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="184">
         <v>1</v>
       </c>
-      <c r="C33" s="189">
+      <c r="C35" s="189">
         <v>1.7299999999999999E-2</v>
       </c>
-      <c r="D33" s="190">
+      <c r="D35" s="190">
         <v>-8.1487286000000003E-3</v>
       </c>
-      <c r="E33" s="191">
+      <c r="E35" s="191">
         <v>-1.00126533E-2</v>
-      </c>
-      <c r="J33" s="104"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="185">
-        <v>2</v>
-      </c>
-      <c r="C34" s="192">
-        <v>1.7100000000000001E-2</v>
-      </c>
-      <c r="D34" s="52">
-        <v>-8.1492985000000007E-3</v>
-      </c>
-      <c r="E34" s="58">
-        <v>-1.03242331E-2</v>
-      </c>
-      <c r="J34" s="104"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="185">
-        <v>3</v>
-      </c>
-      <c r="C35" s="192">
-        <v>1.7299999999999999E-2</v>
-      </c>
-      <c r="D35" s="52">
-        <v>-8.1492985000000007E-3</v>
-      </c>
-      <c r="E35" s="58">
-        <v>-1.01906989E-2</v>
       </c>
       <c r="J35" s="104"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="185">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C36" s="192">
-        <v>1.66E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="D36" s="52">
         <v>-8.1492985000000007E-3</v>
       </c>
       <c r="E36" s="58">
-        <v>-1.06803243E-2</v>
+        <v>-1.03242331E-2</v>
       </c>
       <c r="J36" s="104"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="185">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C37" s="192">
-        <v>1.6400000000000001E-2</v>
+        <v>1.7299999999999999E-2</v>
       </c>
       <c r="D37" s="52">
         <v>-8.1492985000000007E-3</v>
       </c>
       <c r="E37" s="58">
+        <v>-1.01906989E-2</v>
+      </c>
+      <c r="J37" s="104"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="185">
+        <v>4</v>
+      </c>
+      <c r="C38" s="192">
+        <v>1.66E-2</v>
+      </c>
+      <c r="D38" s="52">
+        <v>-8.1492985000000007E-3</v>
+      </c>
+      <c r="E38" s="58">
+        <v>-1.06803243E-2</v>
+      </c>
+      <c r="J38" s="104"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="185">
+        <v>5</v>
+      </c>
+      <c r="C39" s="192">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="D39" s="52">
+        <v>-8.1492985000000007E-3</v>
+      </c>
+      <c r="E39" s="58">
         <v>-1.0502278699999999E-2</v>
       </c>
-      <c r="J37" s="104"/>
-    </row>
-    <row r="38" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="186">
+      <c r="J39" s="104"/>
+    </row>
+    <row r="40" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="186">
         <v>6</v>
       </c>
-      <c r="C38" s="193">
+      <c r="C40" s="193">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D38" s="56">
+      <c r="D40" s="56">
         <v>-8.1487286000000003E-3</v>
       </c>
-      <c r="E38" s="54">
+      <c r="E40" s="54">
         <v>-1.08583699E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="104" t="s">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="202">
+        <f>MAX(C35:C40)-MIN(C35:C40)</f>
+        <v>8.9999999999999802E-4</v>
+      </c>
+      <c r="D41" s="203">
+        <f>MAX(D35:D40)-MIN(D35:D40)</f>
+        <v>5.6990000000048391E-7</v>
+      </c>
+      <c r="E41" s="204">
+        <f>MAX(E35:E40)-MIN(E35:E40)</f>
+        <v>8.4571659999999917E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C42" s="205">
+        <f>STDEV(C35:C40)</f>
+        <v>3.7282703764614445E-4</v>
+      </c>
+      <c r="D42" s="52">
+        <f>STDEV(D35:D40)</f>
+        <v>2.9429509453406415E-7</v>
+      </c>
+      <c r="E42" s="58">
+        <f>STDEV(E35:E40)</f>
+        <v>3.1432319015201309E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="206">
+        <f>MAX(C41:E41)</f>
+        <v>8.9999999999999802E-4</v>
+      </c>
+      <c r="D43" s="56"/>
+      <c r="E43" s="54"/>
+    </row>
+    <row r="45" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="105" t="s">
+      <c r="C45" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="D42" s="104" t="s">
+      <c r="D45" s="104" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="70" t="s">
+    <row r="46" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D43" s="187" t="s">
+      <c r="C46" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="188" t="s">
+      <c r="E46" s="188" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B44" s="184">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="184">
         <v>1</v>
       </c>
-      <c r="C44" s="189">
+      <c r="C47" s="189">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="D44" s="190">
+      <c r="D47" s="190">
         <v>-8.141321E-3</v>
       </c>
-      <c r="E44" s="191">
+      <c r="E47" s="191">
         <v>7.0797249199999997E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="185">
-        <v>2</v>
-      </c>
-      <c r="C45" s="192">
-        <v>1.5E-3</v>
-      </c>
-      <c r="D45" s="52">
-        <v>-8.1418900000000006E-3</v>
-      </c>
-      <c r="E45" s="58">
-        <v>5.8779170699999996E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="185">
-        <v>3</v>
-      </c>
-      <c r="C46" s="192">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="D46" s="52">
-        <v>-8.141321E-3</v>
-      </c>
-      <c r="E46" s="58">
-        <v>6.3675424900000001E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="185">
-        <v>4</v>
-      </c>
-      <c r="C47" s="192">
-        <v>1E-4</v>
-      </c>
-      <c r="D47" s="52">
-        <v>-8.1418900000000006E-3</v>
-      </c>
-      <c r="E47" s="58">
-        <v>6.4120538899999999E-3</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="185">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C48" s="192">
-        <v>2.0000000000000001E-4</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D48" s="52">
         <v>-8.1418900000000006E-3</v>
       </c>
       <c r="E48" s="58">
+        <v>5.8779170699999996E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B49" s="185">
+        <v>3</v>
+      </c>
+      <c r="C49" s="192">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D49" s="52">
+        <v>-8.141321E-3</v>
+      </c>
+      <c r="E49" s="58">
+        <v>6.3675424900000001E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B50" s="185">
+        <v>4</v>
+      </c>
+      <c r="C50" s="192">
+        <v>1E-4</v>
+      </c>
+      <c r="D50" s="52">
+        <v>-8.1418900000000006E-3</v>
+      </c>
+      <c r="E50" s="58">
+        <v>6.4120538899999999E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B51" s="185">
+        <v>5</v>
+      </c>
+      <c r="C51" s="192">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="D51" s="52">
+        <v>-8.1418900000000006E-3</v>
+      </c>
+      <c r="E51" s="58">
         <v>6.5900995E-3</v>
       </c>
     </row>
-    <row r="49" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="186">
+    <row r="52" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="186">
         <v>6</v>
       </c>
-      <c r="C49" s="193">
+      <c r="C52" s="193">
         <v>1E-3</v>
       </c>
-      <c r="D49" s="56">
+      <c r="D52" s="56">
         <v>-8.141321E-3</v>
       </c>
-      <c r="E49" s="54">
+      <c r="E52" s="54">
         <v>6.7681451100000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="104" t="s">
+    <row r="53" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B53" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="202">
+        <f>MAX(C47:C52)-MIN(C47:C52)</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="D53" s="203">
+        <f>MAX(D47:D52)-MIN(D47:D52)</f>
+        <v>5.6900000000061068E-7</v>
+      </c>
+      <c r="E53" s="204">
+        <f>MAX(E47:E52)-MIN(E47:E52)</f>
+        <v>1.2018078500000001E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B54" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="205">
+        <f>STDEV(C47:C52)</f>
+        <v>5.4680892457969262E-4</v>
+      </c>
+      <c r="D54" s="52">
+        <f>STDEV(D47:D52)</f>
+        <v>3.1165413522077398E-7</v>
+      </c>
+      <c r="E54" s="58">
+        <f>STDEV(E47:E52)</f>
+        <v>4.0665658359148019E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="206">
+        <f>MAX(C53:E53)</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="D55" s="56"/>
+      <c r="E55" s="54"/>
+    </row>
+    <row r="57" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="105" t="s">
+      <c r="C57" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="D53" s="104" t="s">
+      <c r="D57" s="104" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="70" t="s">
+    <row r="58" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D54" s="187" t="s">
+      <c r="C58" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D58" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="E54" s="188" t="s">
+      <c r="E58" s="188" t="s">
         <v>51</v>
-      </c>
-      <c r="I54" s="104"/>
-      <c r="Q54" s="106"/>
-      <c r="V54" s="103"/>
-      <c r="W54" s="103"/>
-      <c r="X54" s="103"/>
-    </row>
-    <row r="55" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B55" s="184">
-        <v>1</v>
-      </c>
-      <c r="C55" s="189">
-        <v>9.9903999999999993</v>
-      </c>
-      <c r="D55" s="190">
-        <v>9.9949074249999992</v>
-      </c>
-      <c r="E55" s="191">
-        <v>9.9993552900000005</v>
-      </c>
-      <c r="I55" s="105"/>
-      <c r="Q55" s="106"/>
-      <c r="V55" s="103"/>
-      <c r="W55" s="103"/>
-      <c r="X55" s="103"/>
-    </row>
-    <row r="56" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B56" s="185">
-        <v>2</v>
-      </c>
-      <c r="C56" s="192">
-        <v>9.99</v>
-      </c>
-      <c r="D56" s="52">
-        <v>9.9949074249999992</v>
-      </c>
-      <c r="E56" s="58">
-        <v>9.9990437100000005</v>
-      </c>
-      <c r="I56" s="104"/>
-      <c r="Q56" s="106"/>
-      <c r="V56" s="103"/>
-      <c r="W56" s="103"/>
-      <c r="X56" s="103"/>
-    </row>
-    <row r="57" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B57" s="185">
-        <v>3</v>
-      </c>
-      <c r="C57" s="192">
-        <v>9.9895999999999994</v>
-      </c>
-      <c r="D57" s="52">
-        <v>9.9949074249999992</v>
-      </c>
-      <c r="E57" s="58">
-        <v>9.9988211499999995</v>
-      </c>
-      <c r="I57" s="104"/>
-      <c r="Q57" s="106"/>
-      <c r="V57" s="103"/>
-      <c r="W57" s="103"/>
-      <c r="X57" s="103"/>
-    </row>
-    <row r="58" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B58" s="185">
-        <v>4</v>
-      </c>
-      <c r="C58" s="192">
-        <v>9.9986999999999995</v>
-      </c>
-      <c r="D58" s="52">
-        <v>9.9949074249999992</v>
-      </c>
-      <c r="E58" s="58">
-        <v>9.9985095699999995</v>
       </c>
       <c r="I58" s="104"/>
       <c r="Q58" s="106"/>
@@ -6973,36 +7138,36 @@
       <c r="X58" s="103"/>
     </row>
     <row r="59" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B59" s="185">
-        <v>5</v>
-      </c>
-      <c r="C59" s="192">
-        <v>9.9890000000000008</v>
-      </c>
-      <c r="D59" s="52">
-        <v>9.9949079919999999</v>
-      </c>
-      <c r="E59" s="58">
-        <v>9.9984650599999991</v>
-      </c>
-      <c r="I59" s="104"/>
+      <c r="B59" s="184">
+        <v>1</v>
+      </c>
+      <c r="C59" s="189">
+        <v>9.9903999999999993</v>
+      </c>
+      <c r="D59" s="190">
+        <v>9.9949074249999992</v>
+      </c>
+      <c r="E59" s="191">
+        <v>9.9993552900000005</v>
+      </c>
+      <c r="I59" s="105"/>
       <c r="Q59" s="106"/>
       <c r="V59" s="103"/>
       <c r="W59" s="103"/>
       <c r="X59" s="103"/>
     </row>
-    <row r="60" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="186">
-        <v>6</v>
-      </c>
-      <c r="C60" s="193">
-        <v>9.9885999999999999</v>
-      </c>
-      <c r="D60" s="56">
+    <row r="60" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B60" s="185">
+        <v>2</v>
+      </c>
+      <c r="C60" s="209">
+        <v>9.99</v>
+      </c>
+      <c r="D60" s="210">
         <v>9.9949074249999992</v>
       </c>
-      <c r="E60" s="54">
-        <v>9.9982870100000003</v>
+      <c r="E60" s="211">
+        <v>9.9990437100000005</v>
       </c>
       <c r="I60" s="104"/>
       <c r="Q60" s="106"/>
@@ -7010,850 +7175,1280 @@
       <c r="W60" s="103"/>
       <c r="X60" s="103"/>
     </row>
+    <row r="61" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B61" s="185">
+        <v>3</v>
+      </c>
+      <c r="C61" s="192">
+        <v>9.9895999999999994</v>
+      </c>
+      <c r="D61" s="52">
+        <v>9.9949074249999992</v>
+      </c>
+      <c r="E61" s="58">
+        <v>9.9988211499999995</v>
+      </c>
+      <c r="I61" s="104"/>
+      <c r="Q61" s="106"/>
+      <c r="V61" s="103"/>
+      <c r="W61" s="103"/>
+      <c r="X61" s="103"/>
+    </row>
+    <row r="62" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B62" s="185">
+        <v>4</v>
+      </c>
+      <c r="C62" s="192">
+        <v>9.9986999999999995</v>
+      </c>
+      <c r="D62" s="52">
+        <v>9.9949074249999992</v>
+      </c>
+      <c r="E62" s="58">
+        <v>9.9985095699999995</v>
+      </c>
+      <c r="I62" s="104"/>
+      <c r="Q62" s="106"/>
+      <c r="V62" s="103"/>
+      <c r="W62" s="103"/>
+      <c r="X62" s="103"/>
+    </row>
+    <row r="63" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B63" s="185">
+        <v>5</v>
+      </c>
+      <c r="C63" s="192">
+        <v>9.9890000000000008</v>
+      </c>
+      <c r="D63" s="52">
+        <v>9.9949079919999999</v>
+      </c>
+      <c r="E63" s="58">
+        <v>9.9984650599999991</v>
+      </c>
+      <c r="I63" s="104"/>
+      <c r="Q63" s="106"/>
+      <c r="V63" s="103"/>
+      <c r="W63" s="103"/>
+      <c r="X63" s="103"/>
+    </row>
     <row r="64" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="104" t="s">
+      <c r="B64" s="186">
+        <v>6</v>
+      </c>
+      <c r="C64" s="193">
+        <v>9.9885999999999999</v>
+      </c>
+      <c r="D64" s="56">
+        <v>9.9949074249999992</v>
+      </c>
+      <c r="E64" s="54">
+        <v>9.9982870100000003</v>
+      </c>
+      <c r="I64" s="104"/>
+      <c r="Q64" s="106"/>
+      <c r="V64" s="103"/>
+      <c r="W64" s="103"/>
+      <c r="X64" s="103"/>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B65" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="202">
+        <f>MAX(C59:C64)-MIN(C59:C64)</f>
+        <v>1.0099999999999554E-2</v>
+      </c>
+      <c r="D65" s="203">
+        <f>MAX(D59:D64)-MIN(D59:D64)</f>
+        <v>5.6700000072851253E-7</v>
+      </c>
+      <c r="E65" s="204">
+        <f>MAX(E59:E64)-MIN(E59:E64)</f>
+        <v>1.0682800000001436E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B66" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C66" s="205">
+        <f>STDEV(C59:C64)</f>
+        <v>3.8040767605291969E-3</v>
+      </c>
+      <c r="D66" s="52">
+        <f>STDEV(D59:D64)</f>
+        <v>2.3147678099042435E-7</v>
+      </c>
+      <c r="E66" s="58">
+        <f>STDEV(E59:E64)</f>
+        <v>4.0274203454598444E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C67" s="206">
+        <f>MAX(C65:E65)</f>
+        <v>1.0099999999999554E-2</v>
+      </c>
+      <c r="D67" s="56"/>
+      <c r="E67" s="54"/>
+    </row>
+    <row r="69" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="105" t="s">
+      <c r="C69" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="D64" s="104" t="s">
+      <c r="D69" s="104" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="70" t="s">
+    <row r="70" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D65" s="187" t="s">
+      <c r="C70" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D70" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="E65" s="188" t="s">
+      <c r="E70" s="188" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B66" s="184">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B71" s="184">
         <v>1</v>
       </c>
-      <c r="C66" s="189">
+      <c r="C71" s="189">
         <v>10.0046</v>
       </c>
-      <c r="D66" s="190">
+      <c r="D71" s="190">
         <v>9.9949148319999992</v>
       </c>
-      <c r="E66" s="191">
+      <c r="E71" s="191">
         <v>10.01524586</v>
       </c>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B67" s="185">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B72" s="185">
         <v>2</v>
       </c>
-      <c r="C67" s="192">
+      <c r="C72" s="192">
         <v>10.0047</v>
       </c>
-      <c r="D67" s="52">
+      <c r="D72" s="52">
         <v>9.9949148319999992</v>
       </c>
-      <c r="E67" s="58">
+      <c r="E72" s="58">
         <v>10.014355630000001</v>
       </c>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B68" s="185">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B73" s="185">
         <v>3</v>
       </c>
-      <c r="C68" s="192">
+      <c r="C73" s="192">
         <v>10.005100000000001</v>
       </c>
-      <c r="D68" s="52">
+      <c r="D73" s="52">
         <v>9.9949148319999992</v>
       </c>
-      <c r="E68" s="58">
+      <c r="E73" s="58">
         <v>10.014667210000001</v>
       </c>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B69" s="185">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B74" s="185">
         <v>4</v>
       </c>
-      <c r="C69" s="192">
+      <c r="C74" s="192">
         <v>10.0046</v>
       </c>
-      <c r="D69" s="52">
+      <c r="D74" s="52">
         <v>9.9949148319999992</v>
       </c>
-      <c r="E69" s="58">
+      <c r="E74" s="58">
         <v>10.01484526</v>
       </c>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B70" s="185">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B75" s="185">
         <v>5</v>
       </c>
-      <c r="C70" s="192">
+      <c r="C75" s="192">
         <v>10.004799999999999</v>
       </c>
-      <c r="D70" s="52">
+      <c r="D75" s="52">
         <v>9.9949142650000002</v>
       </c>
-      <c r="E70" s="58">
+      <c r="E75" s="58">
         <v>10.015023299999999</v>
       </c>
     </row>
-    <row r="71" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="186">
+    <row r="76" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="186">
         <v>6</v>
       </c>
-      <c r="C71" s="193">
+      <c r="C76" s="193">
         <v>10.0054</v>
       </c>
-      <c r="D71" s="56">
+      <c r="D76" s="56">
         <v>9.9949148319999992</v>
       </c>
-      <c r="E71" s="54">
+      <c r="E76" s="54">
         <v>10.01520135</v>
       </c>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="Q72" s="106"/>
-    </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="Q73" s="106"/>
-    </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="Q74" s="106"/>
-    </row>
-    <row r="75" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="106" t="s">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B77" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" s="202">
+        <f>MAX(C71:C76)-MIN(C71:C76)</f>
+        <v>7.9999999999991189E-4</v>
+      </c>
+      <c r="D77" s="203">
+        <f>MAX(D71:D76)-MIN(D71:D76)</f>
+        <v>5.6699999895215569E-7</v>
+      </c>
+      <c r="E77" s="204">
+        <f>MAX(E71:E76)-MIN(E71:E76)</f>
+        <v>8.9022999999954777E-4</v>
+      </c>
+      <c r="Q77" s="106"/>
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B78" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C78" s="205">
+        <f>STDEV(C71:C76)</f>
+        <v>3.2041639575204774E-4</v>
+      </c>
+      <c r="D78" s="52">
+        <f>STDEV(D71:D76)</f>
+        <v>2.3147678026522968E-7</v>
+      </c>
+      <c r="E78" s="58">
+        <f>STDEV(E71:E76)</f>
+        <v>3.4015645773150411E-4</v>
+      </c>
+      <c r="Q78" s="106"/>
+    </row>
+    <row r="79" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" s="206">
+        <f>MAX(C77:E77)</f>
+        <v>8.9022999999954777E-4</v>
+      </c>
+      <c r="D79" s="56"/>
+      <c r="E79" s="54"/>
+      <c r="Q79" s="106"/>
+    </row>
+    <row r="80" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="Q80" s="106"/>
+    </row>
+    <row r="81" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="C75" s="106" t="s">
+      <c r="C81" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="D75" s="106" t="s">
+      <c r="D81" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="Q75" s="106"/>
-    </row>
-    <row r="76" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="70" t="s">
+      <c r="Q81" s="106"/>
+    </row>
+    <row r="82" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="C76" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D76" s="187" t="s">
+      <c r="C82" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D82" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="E76" s="188" t="s">
+      <c r="E82" s="188" t="s">
         <v>51</v>
       </c>
-      <c r="Q76" s="106"/>
-    </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B77" s="184">
+      <c r="Q82" s="106"/>
+    </row>
+    <row r="83" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B83" s="184">
         <v>1</v>
       </c>
-      <c r="C77" s="189">
+      <c r="C83" s="189">
         <v>19.9969</v>
       </c>
-      <c r="D77" s="190">
+      <c r="D83" s="190">
         <v>19.997963500000001</v>
       </c>
-      <c r="E77" s="191">
+      <c r="E83" s="191">
         <v>19.999108769999999</v>
       </c>
-      <c r="Q77" s="106"/>
-    </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B78" s="185">
+      <c r="Q83" s="106"/>
+    </row>
+    <row r="84" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B84" s="185">
         <v>2</v>
       </c>
-      <c r="C78" s="192">
+      <c r="C84" s="192">
         <v>19.9954</v>
       </c>
-      <c r="D78" s="52">
+      <c r="D84" s="52">
         <v>19.997963500000001</v>
       </c>
-      <c r="E78" s="58">
+      <c r="E84" s="58">
         <v>19.998619139999999</v>
       </c>
-      <c r="Q78" s="106"/>
-    </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B79" s="185">
+      <c r="Q84" s="106"/>
+    </row>
+    <row r="85" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B85" s="185">
         <v>3</v>
       </c>
-      <c r="C79" s="192">
+      <c r="C85" s="192">
         <v>19.994800000000001</v>
       </c>
-      <c r="D79" s="52">
+      <c r="D85" s="52">
         <v>19.997963500000001</v>
       </c>
-      <c r="E79" s="58">
+      <c r="E85" s="58">
         <v>19.998441100000001</v>
       </c>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B80" s="185">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B86" s="185">
         <v>4</v>
       </c>
-      <c r="C80" s="192">
+      <c r="C86" s="192">
         <v>19.994800000000001</v>
       </c>
-      <c r="D80" s="52">
+      <c r="D86" s="52">
         <v>19.997963500000001</v>
       </c>
-      <c r="E80" s="58">
+      <c r="E86" s="58">
         <v>19.998263049999998</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B81" s="185">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B87" s="185">
         <v>5</v>
       </c>
-      <c r="C81" s="192">
+      <c r="C87" s="192">
         <v>19.995000000000001</v>
       </c>
-      <c r="D81" s="52">
+      <c r="D87" s="52">
         <v>19.997963500000001</v>
       </c>
-      <c r="E81" s="58">
+      <c r="E87" s="58">
         <v>19.998040499999998</v>
       </c>
     </row>
-    <row r="82" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="186">
+    <row r="88" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="186">
         <v>6</v>
       </c>
-      <c r="C82" s="193">
+      <c r="C88" s="193">
         <v>19.994900000000001</v>
       </c>
-      <c r="D82" s="56">
+      <c r="D88" s="56">
         <v>19.997963500000001</v>
       </c>
-      <c r="E82" s="54">
+      <c r="E88" s="54">
         <v>19.997906960000002</v>
       </c>
     </row>
-    <row r="86" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="106" t="s">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B89" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C89" s="202">
+        <f>MAX(C83:C88)-MIN(C83:C88)</f>
+        <v>2.0999999999986585E-3</v>
+      </c>
+      <c r="D89" s="203">
+        <f>MAX(D83:D88)-MIN(D83:D88)</f>
+        <v>0</v>
+      </c>
+      <c r="E89" s="204">
+        <f>MAX(E83:E88)-MIN(E83:E88)</f>
+        <v>1.2018099999977494E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B90" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C90" s="205">
+        <f>STDEV(C83:C88)</f>
+        <v>8.148619514980306E-4</v>
+      </c>
+      <c r="D90" s="52">
+        <f>STDEV(D83:D88)</f>
+        <v>0</v>
+      </c>
+      <c r="E90" s="58">
+        <f>STDEV(E83:E88)</f>
+        <v>4.3429956286692947E-4</v>
+      </c>
+    </row>
+    <row r="91" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C91" s="206">
+        <f>MAX(C89:E89)</f>
+        <v>2.0999999999986585E-3</v>
+      </c>
+      <c r="D91" s="56"/>
+      <c r="E91" s="54"/>
+    </row>
+    <row r="93" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="C86" s="106" t="s">
+      <c r="C93" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="D86" s="106" t="s">
+      <c r="D93" s="106" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="87" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="70" t="s">
+    <row r="94" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="C87" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D87" s="187" t="s">
+      <c r="C94" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D94" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="E87" s="188" t="s">
+      <c r="E94" s="188" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B88" s="184">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B95" s="184">
         <v>1</v>
       </c>
-      <c r="C88" s="189">
+      <c r="C95" s="189">
         <v>20.015999999999998</v>
       </c>
-      <c r="D88" s="190">
+      <c r="D95" s="190">
         <v>19.997970980000002</v>
       </c>
-      <c r="E88" s="191">
+      <c r="E95" s="191">
         <v>20.012996300000001</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B89" s="185">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B96" s="185">
         <v>2</v>
       </c>
-      <c r="C89" s="192">
+      <c r="C96" s="192">
         <v>20.010999999999999</v>
       </c>
-      <c r="D89" s="52">
+      <c r="D96" s="52">
         <v>19.997970980000002</v>
       </c>
-      <c r="E89" s="58">
+      <c r="E96" s="58">
         <v>20.013218800000001</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B90" s="185">
+    <row r="97" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B97" s="185">
         <v>3</v>
       </c>
-      <c r="C90" s="192">
+      <c r="C97" s="192">
         <v>20.011299999999999</v>
       </c>
-      <c r="D90" s="52">
+      <c r="D97" s="52">
         <v>19.997970980000002</v>
       </c>
-      <c r="E90" s="58">
+      <c r="E97" s="58">
         <v>20.0133969</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B91" s="185">
+    <row r="98" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B98" s="185">
         <v>4</v>
       </c>
-      <c r="C91" s="192">
+      <c r="C98" s="192">
         <v>20.011700000000001</v>
       </c>
-      <c r="D91" s="52">
+      <c r="D98" s="52">
         <v>19.997970980000002</v>
       </c>
-      <c r="E91" s="58">
+      <c r="E98" s="58">
         <v>20.013574899999998</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B92" s="185">
+    <row r="99" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B99" s="185">
         <v>5</v>
       </c>
-      <c r="C92" s="192">
+      <c r="C99" s="192">
         <v>20.011399999999998</v>
       </c>
-      <c r="D92" s="52">
+      <c r="D99" s="52">
         <v>19.997970980000002</v>
       </c>
-      <c r="E92" s="58">
+      <c r="E99" s="58">
         <v>20.013753000000001</v>
       </c>
     </row>
-    <row r="93" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="186">
+    <row r="100" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="186">
         <v>6</v>
       </c>
-      <c r="C93" s="193">
+      <c r="C100" s="193">
         <v>20.011500000000002</v>
       </c>
-      <c r="D93" s="56">
+      <c r="D100" s="56">
         <v>19.997970980000002</v>
       </c>
-      <c r="E93" s="54">
+      <c r="E100" s="54">
         <v>20.013040799999999</v>
       </c>
     </row>
-    <row r="97" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="106" t="s">
+    <row r="101" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B101" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C101" s="202">
+        <f>MAX(C95:C100)-MIN(C95:C100)</f>
+        <v>4.9999999999990052E-3</v>
+      </c>
+      <c r="D101" s="203">
+        <f>MAX(D95:D100)-MIN(D95:D100)</f>
+        <v>0</v>
+      </c>
+      <c r="E101" s="204">
+        <f>MAX(E95:E100)-MIN(E95:E100)</f>
+        <v>7.5670000000016557E-4</v>
+      </c>
+    </row>
+    <row r="102" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B102" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" s="205">
+        <f>STDEV(C95:C100)</f>
+        <v>1.9002631396725085E-3</v>
+      </c>
+      <c r="D102" s="52">
+        <f>STDEV(D95:D100)</f>
+        <v>0</v>
+      </c>
+      <c r="E102" s="58">
+        <f>STDEV(E95:E100)</f>
+        <v>3.0024600191621165E-4</v>
+      </c>
+    </row>
+    <row r="103" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C103" s="206">
+        <f>MAX(C101:E101)</f>
+        <v>4.9999999999990052E-3</v>
+      </c>
+      <c r="D103" s="56"/>
+      <c r="E103" s="54"/>
+    </row>
+    <row r="105" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="C97" s="106" t="s">
+      <c r="C105" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="D97" s="106" t="s">
+      <c r="D105" s="106" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="70" t="s">
+    <row r="106" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="C98" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D98" s="187" t="s">
+      <c r="C106" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D106" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="E98" s="188" t="s">
+      <c r="E106" s="188" t="s">
         <v>51</v>
       </c>
-      <c r="F98" s="103"/>
-      <c r="G98" s="103"/>
-      <c r="H98" s="103"/>
-      <c r="I98" s="106"/>
-      <c r="Q98" s="106"/>
-      <c r="V98" s="103"/>
-      <c r="W98" s="103"/>
-      <c r="X98" s="103"/>
-    </row>
-    <row r="99" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B99" s="184">
+      <c r="F106" s="103"/>
+      <c r="G106" s="103"/>
+      <c r="H106" s="103"/>
+      <c r="I106" s="106"/>
+      <c r="Q106" s="106"/>
+      <c r="V106" s="103"/>
+      <c r="W106" s="103"/>
+      <c r="X106" s="103"/>
+    </row>
+    <row r="107" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B107" s="184">
         <v>1</v>
       </c>
-      <c r="C99" s="189">
+      <c r="C107" s="189">
         <v>29.996400000000001</v>
       </c>
-      <c r="D99" s="190">
+      <c r="D107" s="190">
         <v>30.001020302000001</v>
       </c>
-      <c r="E99" s="191">
+      <c r="E107" s="191">
         <v>29.996236079999999</v>
       </c>
-      <c r="F99" s="103"/>
-      <c r="G99" s="103"/>
-      <c r="H99" s="103"/>
-      <c r="I99" s="106"/>
-      <c r="Q99" s="106"/>
-      <c r="V99" s="103"/>
-      <c r="W99" s="103"/>
-      <c r="X99" s="103"/>
-    </row>
-    <row r="100" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B100" s="185">
+      <c r="F107" s="103"/>
+      <c r="G107" s="103"/>
+      <c r="H107" s="103"/>
+      <c r="I107" s="106"/>
+      <c r="Q107" s="106"/>
+      <c r="V107" s="103"/>
+      <c r="W107" s="103"/>
+      <c r="X107" s="103"/>
+    </row>
+    <row r="108" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B108" s="185">
         <v>2</v>
       </c>
-      <c r="C100" s="192">
+      <c r="C108" s="192">
         <v>29.9968</v>
       </c>
-      <c r="D100" s="52">
+      <c r="D108" s="52">
         <v>30.001019735</v>
       </c>
-      <c r="E100" s="58">
+      <c r="E108" s="58">
         <v>29.99659217</v>
       </c>
-      <c r="F100" s="103"/>
-      <c r="G100" s="103"/>
-      <c r="H100" s="103"/>
-      <c r="I100" s="106"/>
-      <c r="Q100" s="106"/>
-      <c r="V100" s="103"/>
-      <c r="W100" s="103"/>
-      <c r="X100" s="103"/>
-    </row>
-    <row r="101" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B101" s="185">
+      <c r="F108" s="103"/>
+      <c r="G108" s="103"/>
+      <c r="H108" s="103"/>
+      <c r="I108" s="106"/>
+      <c r="Q108" s="106"/>
+      <c r="V108" s="103"/>
+      <c r="W108" s="103"/>
+      <c r="X108" s="103"/>
+    </row>
+    <row r="109" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B109" s="185">
         <v>3</v>
       </c>
-      <c r="C101" s="192">
+      <c r="C109" s="192">
         <v>29.997399999999999</v>
       </c>
-      <c r="D101" s="52">
+      <c r="D109" s="52">
         <v>30.001020302000001</v>
       </c>
-      <c r="E101" s="58">
+      <c r="E109" s="58">
         <v>29.996414130000002</v>
       </c>
-      <c r="F101" s="103"/>
-      <c r="G101" s="103"/>
-      <c r="H101" s="103"/>
-      <c r="I101" s="106"/>
-      <c r="Q101" s="106"/>
-      <c r="V101" s="103"/>
-      <c r="W101" s="103"/>
-      <c r="X101" s="103"/>
-    </row>
-    <row r="102" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B102" s="185">
+      <c r="F109" s="103"/>
+      <c r="G109" s="103"/>
+      <c r="H109" s="103"/>
+      <c r="I109" s="106"/>
+      <c r="Q109" s="106"/>
+      <c r="V109" s="103"/>
+      <c r="W109" s="103"/>
+      <c r="X109" s="103"/>
+    </row>
+    <row r="110" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B110" s="185">
         <v>4</v>
       </c>
-      <c r="C102" s="192">
+      <c r="C110" s="192">
         <v>29.9969</v>
       </c>
-      <c r="D102" s="52">
+      <c r="D110" s="52">
         <v>30.001019735</v>
       </c>
-      <c r="E102" s="58">
+      <c r="E110" s="58">
         <v>29.996236079999999</v>
       </c>
-      <c r="F102" s="103"/>
-      <c r="G102" s="103"/>
-      <c r="H102" s="103"/>
-      <c r="I102" s="106"/>
-      <c r="Q102" s="106"/>
-      <c r="V102" s="103"/>
-      <c r="W102" s="103"/>
-      <c r="X102" s="103"/>
-    </row>
-    <row r="103" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B103" s="185">
-        <v>5</v>
-      </c>
-      <c r="C103" s="192">
-        <v>29.996300000000002</v>
-      </c>
-      <c r="D103" s="52">
-        <v>30.001019735</v>
-      </c>
-      <c r="E103" s="58">
-        <v>29.99605803</v>
-      </c>
-      <c r="F103" s="103"/>
-      <c r="G103" s="103"/>
-      <c r="H103" s="103"/>
-      <c r="I103" s="106"/>
-      <c r="Q103" s="106"/>
-      <c r="V103" s="103"/>
-      <c r="W103" s="103"/>
-      <c r="X103" s="103"/>
-    </row>
-    <row r="104" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="186">
-        <v>6</v>
-      </c>
-      <c r="C104" s="193">
-        <v>29.996400000000001</v>
-      </c>
-      <c r="D104" s="56">
-        <v>30.001019735</v>
-      </c>
-      <c r="E104" s="54">
-        <v>29.996013520000002</v>
-      </c>
-      <c r="F104" s="103"/>
-      <c r="G104" s="103"/>
-      <c r="H104" s="103"/>
-      <c r="I104" s="106"/>
-      <c r="Q104" s="106"/>
-      <c r="V104" s="103"/>
-      <c r="W104" s="103"/>
-      <c r="X104" s="103"/>
-    </row>
-    <row r="108" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="106" t="s">
-        <v>61</v>
-      </c>
-      <c r="C108" s="106" t="s">
-        <v>116</v>
-      </c>
-      <c r="D108" s="106" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="109" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="C109" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D109" s="187" t="s">
-        <v>52</v>
-      </c>
-      <c r="E109" s="188" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="110" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B110" s="184">
-        <v>1</v>
-      </c>
-      <c r="C110" s="189">
-        <v>30.016200000000001</v>
-      </c>
-      <c r="D110" s="190">
-        <v>30.001027709999999</v>
-      </c>
-      <c r="E110" s="191">
-        <v>30.016310699999998</v>
-      </c>
+      <c r="F110" s="103"/>
+      <c r="G110" s="103"/>
+      <c r="H110" s="103"/>
+      <c r="I110" s="106"/>
+      <c r="Q110" s="106"/>
+      <c r="V110" s="103"/>
+      <c r="W110" s="103"/>
+      <c r="X110" s="103"/>
     </row>
     <row r="111" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B111" s="185">
+        <v>5</v>
+      </c>
+      <c r="C111" s="192">
+        <v>29.996300000000002</v>
+      </c>
+      <c r="D111" s="52">
+        <v>30.001019735</v>
+      </c>
+      <c r="E111" s="58">
+        <v>29.99605803</v>
+      </c>
+      <c r="F111" s="103"/>
+      <c r="G111" s="103"/>
+      <c r="H111" s="103"/>
+      <c r="I111" s="106"/>
+      <c r="Q111" s="106"/>
+      <c r="V111" s="103"/>
+      <c r="W111" s="103"/>
+      <c r="X111" s="103"/>
+    </row>
+    <row r="112" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="186">
+        <v>6</v>
+      </c>
+      <c r="C112" s="193">
+        <v>29.996400000000001</v>
+      </c>
+      <c r="D112" s="56">
+        <v>30.001019735</v>
+      </c>
+      <c r="E112" s="54">
+        <v>29.996013520000002</v>
+      </c>
+      <c r="F112" s="103"/>
+      <c r="G112" s="103"/>
+      <c r="H112" s="103"/>
+      <c r="I112" s="106"/>
+      <c r="Q112" s="106"/>
+      <c r="V112" s="103"/>
+      <c r="W112" s="103"/>
+      <c r="X112" s="103"/>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B113" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C113" s="202">
+        <f>MAX(C107:C112)-MIN(C107:C112)</f>
+        <v>1.0999999999974364E-3</v>
+      </c>
+      <c r="D113" s="203">
+        <f>MAX(D107:D112)-MIN(D107:D112)</f>
+        <v>5.6700000072851253E-7</v>
+      </c>
+      <c r="E113" s="204">
+        <f>MAX(E107:E112)-MIN(E107:E112)</f>
+        <v>5.7864999999779343E-4</v>
+      </c>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B114" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C114" s="205">
+        <f>STDEV(C107:C112)</f>
+        <v>4.1952353926708291E-4</v>
+      </c>
+      <c r="D114" s="52">
+        <f>STDEV(D107:D112)</f>
+        <v>2.9279754134948294E-7</v>
+      </c>
+      <c r="E114" s="58">
+        <f>STDEV(E107:E112)</f>
+        <v>2.1760741556723227E-4</v>
+      </c>
+    </row>
+    <row r="115" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C115" s="206">
+        <f>MAX(C113:E113)</f>
+        <v>1.0999999999974364E-3</v>
+      </c>
+      <c r="D115" s="56"/>
+      <c r="E115" s="54"/>
+    </row>
+    <row r="117" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="106" t="s">
+        <v>61</v>
+      </c>
+      <c r="C117" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="D117" s="106" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="118" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="C118" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D118" s="187" t="s">
+        <v>52</v>
+      </c>
+      <c r="E118" s="188" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="119" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B119" s="184">
+        <v>1</v>
+      </c>
+      <c r="C119" s="189">
+        <v>30.016200000000001</v>
+      </c>
+      <c r="D119" s="190">
+        <v>30.001027709999999</v>
+      </c>
+      <c r="E119" s="191">
+        <v>30.016310699999998</v>
+      </c>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B120" s="185">
         <v>2</v>
       </c>
-      <c r="C111" s="192">
+      <c r="C120" s="192">
         <v>30.0168</v>
       </c>
-      <c r="D111" s="52">
+      <c r="D120" s="52">
         <v>30.001027140000001</v>
       </c>
-      <c r="E111" s="58">
+      <c r="E120" s="58">
         <v>30.016666799999999</v>
       </c>
     </row>
-    <row r="112" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B112" s="185">
+    <row r="121" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B121" s="185">
         <v>3</v>
       </c>
-      <c r="C112" s="192">
+      <c r="C121" s="192">
         <v>30.0167</v>
       </c>
-      <c r="D112" s="52">
+      <c r="D121" s="52">
         <v>30.001027140000001</v>
       </c>
-      <c r="E112" s="58">
+      <c r="E121" s="58">
         <v>30.016889299999999</v>
       </c>
-    </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B113" s="185">
-        <v>4</v>
-      </c>
-      <c r="C113" s="192">
-        <v>30.0167</v>
-      </c>
-      <c r="D113" s="52">
-        <v>30.001027140000001</v>
-      </c>
-      <c r="E113" s="58">
-        <v>30.017200899999999</v>
-      </c>
-    </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B114" s="185">
-        <v>5</v>
-      </c>
-      <c r="C114" s="192">
-        <v>30.016999999999999</v>
-      </c>
-      <c r="D114" s="52">
-        <v>30.001027709999999</v>
-      </c>
-      <c r="E114" s="58">
-        <v>30.017378999999998</v>
-      </c>
-    </row>
-    <row r="115" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="186">
-        <v>6</v>
-      </c>
-      <c r="C115" s="193">
-        <v>30.017399999999999</v>
-      </c>
-      <c r="D115" s="56">
-        <v>30.001027709999999</v>
-      </c>
-      <c r="E115" s="54">
-        <v>30.017601500000001</v>
-      </c>
-      <c r="K115" s="106"/>
-    </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="K116" s="106"/>
-    </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="K117" s="106"/>
-    </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="K118" s="106"/>
-    </row>
-    <row r="119" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="106" t="s">
-        <v>61</v>
-      </c>
-      <c r="C119" s="106" t="s">
-        <v>117</v>
-      </c>
-      <c r="D119" s="106" t="s">
-        <v>111</v>
-      </c>
-      <c r="K119" s="106"/>
-    </row>
-    <row r="120" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="C120" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D120" s="187" t="s">
-        <v>52</v>
-      </c>
-      <c r="E120" s="188" t="s">
-        <v>51</v>
-      </c>
-      <c r="K120" s="106"/>
-    </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B121" s="184">
-        <v>1</v>
-      </c>
-      <c r="C121" s="189">
-        <v>40.013199999999998</v>
-      </c>
-      <c r="D121" s="190">
-        <v>40.004076449999999</v>
-      </c>
-      <c r="E121" s="191">
-        <v>40.005915600000002</v>
-      </c>
-      <c r="K121" s="106"/>
     </row>
     <row r="122" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B122" s="185">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C122" s="192">
-        <v>40.007800000000003</v>
+        <v>30.0167</v>
       </c>
       <c r="D122" s="52">
-        <v>40.004076449999999</v>
+        <v>30.001027140000001</v>
       </c>
       <c r="E122" s="58">
-        <v>40.006672299999998</v>
+        <v>30.017200899999999</v>
       </c>
     </row>
     <row r="123" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B123" s="185">
+        <v>5</v>
+      </c>
+      <c r="C123" s="192">
+        <v>30.016999999999999</v>
+      </c>
+      <c r="D123" s="52">
+        <v>30.001027709999999</v>
+      </c>
+      <c r="E123" s="58">
+        <v>30.017378999999998</v>
+      </c>
+    </row>
+    <row r="124" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="186">
+        <v>6</v>
+      </c>
+      <c r="C124" s="193">
+        <v>30.017399999999999</v>
+      </c>
+      <c r="D124" s="56">
+        <v>30.001027709999999</v>
+      </c>
+      <c r="E124" s="54">
+        <v>30.017601500000001</v>
+      </c>
+      <c r="K124" s="106"/>
+    </row>
+    <row r="125" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B125" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C125" s="202">
+        <f>MAX(C119:C124)-MIN(C119:C124)</f>
+        <v>1.1999999999972033E-3</v>
+      </c>
+      <c r="D125" s="203">
+        <f>MAX(D119:D124)-MIN(D119:D124)</f>
+        <v>5.6999999742401997E-7</v>
+      </c>
+      <c r="E125" s="204">
+        <f>MAX(E119:E124)-MIN(E119:E124)</f>
+        <v>1.290800000003145E-3</v>
+      </c>
+      <c r="K125" s="106"/>
+    </row>
+    <row r="126" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B126" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C126" s="205">
+        <f>STDEV(C119:C124)</f>
+        <v>3.9496835316170945E-4</v>
+      </c>
+      <c r="D126" s="52">
+        <f>STDEV(D119:D124)</f>
+        <v>3.122018563670223E-7</v>
+      </c>
+      <c r="E126" s="58">
+        <f>STDEV(E119:E124)</f>
+        <v>4.7829448529882238E-4</v>
+      </c>
+      <c r="K126" s="106"/>
+    </row>
+    <row r="127" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C127" s="206">
+        <f>MAX(C125:E125)</f>
+        <v>1.290800000003145E-3</v>
+      </c>
+      <c r="D127" s="56"/>
+      <c r="E127" s="54"/>
+      <c r="K127" s="106"/>
+    </row>
+    <row r="128" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K128" s="106"/>
+    </row>
+    <row r="129" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="106" t="s">
+        <v>61</v>
+      </c>
+      <c r="C129" s="106" t="s">
+        <v>117</v>
+      </c>
+      <c r="D129" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="K129" s="106"/>
+    </row>
+    <row r="130" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="C130" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D130" s="187" t="s">
+        <v>52</v>
+      </c>
+      <c r="E130" s="188" t="s">
+        <v>51</v>
+      </c>
+      <c r="K130" s="106"/>
+    </row>
+    <row r="131" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B131" s="184">
+        <v>1</v>
+      </c>
+      <c r="C131" s="189">
+        <v>40.013199999999998</v>
+      </c>
+      <c r="D131" s="190">
+        <v>40.004076449999999</v>
+      </c>
+      <c r="E131" s="191">
+        <v>40.005915600000002</v>
+      </c>
+      <c r="K131" s="106"/>
+    </row>
+    <row r="132" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B132" s="185">
+        <v>2</v>
+      </c>
+      <c r="C132" s="192">
+        <v>40.007800000000003</v>
+      </c>
+      <c r="D132" s="52">
+        <v>40.004076449999999</v>
+      </c>
+      <c r="E132" s="58">
+        <v>40.006672299999998</v>
+      </c>
+    </row>
+    <row r="133" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B133" s="185">
         <v>3</v>
       </c>
-      <c r="C123" s="192">
+      <c r="C133" s="192">
         <v>40.007800000000003</v>
       </c>
-      <c r="D123" s="52">
+      <c r="D133" s="52">
         <v>40.004077019999997</v>
       </c>
-      <c r="E123" s="58">
+      <c r="E133" s="58">
         <v>40.006494199999999</v>
       </c>
     </row>
-    <row r="124" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B124" s="185">
+    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B134" s="185">
         <v>4</v>
       </c>
-      <c r="C124" s="192">
+      <c r="C134" s="192">
         <v>40.004399999999997</v>
       </c>
-      <c r="D124" s="52">
+      <c r="D134" s="52">
         <v>40.004076449999999</v>
       </c>
-      <c r="E124" s="58">
+      <c r="E134" s="58">
         <v>40.006316200000001</v>
       </c>
     </row>
-    <row r="125" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B125" s="185">
+    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B135" s="185">
         <v>5</v>
       </c>
-      <c r="C125" s="192">
+      <c r="C135" s="192">
         <v>40.006900000000002</v>
       </c>
-      <c r="D125" s="52">
+      <c r="D135" s="52">
         <v>40.004077019999997</v>
       </c>
-      <c r="E125" s="58">
+      <c r="E135" s="58">
         <v>40.0060936</v>
       </c>
     </row>
-    <row r="126" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="186">
+    <row r="136" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="186">
         <v>6</v>
       </c>
-      <c r="C126" s="193">
+      <c r="C136" s="193">
         <v>40.005499999999998</v>
       </c>
-      <c r="D126" s="56">
+      <c r="D136" s="56">
         <v>40.004077019999997</v>
       </c>
-      <c r="E126" s="54">
+      <c r="E136" s="54">
         <v>40.005960100000003</v>
       </c>
     </row>
-    <row r="131" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="106" t="s">
+    <row r="137" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B137" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C137" s="202">
+        <f>MAX(C131:C136)-MIN(C131:C136)</f>
+        <v>8.8000000000008072E-3</v>
+      </c>
+      <c r="D137" s="203">
+        <f>MAX(D131:D136)-MIN(D131:D136)</f>
+        <v>5.6999999742401997E-7</v>
+      </c>
+      <c r="E137" s="204">
+        <f>MAX(E131:E136)-MIN(E131:E136)</f>
+        <v>7.5669999999661286E-4</v>
+      </c>
+    </row>
+    <row r="138" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B138" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C138" s="205">
+        <f>STDEV(C131:C136)</f>
+        <v>3.0522123124056477E-3</v>
+      </c>
+      <c r="D138" s="52">
+        <f>STDEV(D131:D136)</f>
+        <v>3.1220185636702241E-7</v>
+      </c>
+      <c r="E138" s="58">
+        <f>STDEV(E131:E136)</f>
+        <v>3.0407094566738731E-4</v>
+      </c>
+    </row>
+    <row r="139" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C139" s="206">
+        <f>MAX(C137:E137)</f>
+        <v>8.8000000000008072E-3</v>
+      </c>
+      <c r="D139" s="56"/>
+      <c r="E139" s="54"/>
+    </row>
+    <row r="141" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="C131" s="106" t="s">
+      <c r="C141" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="D131" s="106" t="s">
+      <c r="D141" s="106" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="132" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="70" t="s">
+    <row r="142" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="C132" s="187" t="s">
-        <v>187</v>
-      </c>
-      <c r="D132" s="187" t="s">
+      <c r="C142" s="187" t="s">
+        <v>176</v>
+      </c>
+      <c r="D142" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="E132" s="188" t="s">
+      <c r="E142" s="188" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B133" s="184">
+    <row r="143" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B143" s="184">
         <v>1</v>
       </c>
-      <c r="C133" s="189">
+      <c r="C143" s="189">
         <v>40.017200000000003</v>
       </c>
-      <c r="D133" s="190">
+      <c r="D143" s="190">
         <v>40.004083860000001</v>
       </c>
-      <c r="E133" s="191">
+      <c r="E143" s="191">
         <v>40.019313539999999</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B134" s="185">
+    <row r="144" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B144" s="185">
         <v>2</v>
       </c>
-      <c r="C134" s="192">
+      <c r="C144" s="192">
         <v>40.022100000000002</v>
       </c>
-      <c r="D134" s="52">
+      <c r="D144" s="52">
         <v>40.004083860000001</v>
       </c>
-      <c r="E134" s="58">
+      <c r="E144" s="58">
         <v>40.01949158</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B135" s="185">
+    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B145" s="185">
         <v>3</v>
       </c>
-      <c r="C135" s="192">
+      <c r="C145" s="192">
         <v>40.017600000000002</v>
       </c>
-      <c r="D135" s="52">
+      <c r="D145" s="52">
         <v>40.004083289999997</v>
       </c>
-      <c r="E135" s="58">
+      <c r="E145" s="58">
         <v>40.019669630000003</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B136" s="185">
+    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B146" s="185">
         <v>4</v>
       </c>
-      <c r="C136" s="192">
+      <c r="C146" s="192">
         <v>40.022399999999998</v>
       </c>
-      <c r="D136" s="52">
+      <c r="D146" s="52">
         <v>40.004083860000001</v>
       </c>
-      <c r="E136" s="58">
+      <c r="E146" s="58">
         <v>40.019847669999997</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B137" s="185">
+    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B147" s="185">
         <v>5</v>
       </c>
-      <c r="C137" s="192">
+      <c r="C147" s="192">
         <v>40.018599999999999</v>
       </c>
-      <c r="D137" s="52">
+      <c r="D147" s="52">
         <v>40.004083860000001</v>
       </c>
-      <c r="E137" s="58">
+      <c r="E147" s="58">
         <v>40.019981209999997</v>
       </c>
     </row>
-    <row r="138" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="186">
+    <row r="148" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="186">
         <v>6</v>
       </c>
-      <c r="C138" s="193">
+      <c r="C148" s="193">
         <v>40.024900000000002</v>
       </c>
-      <c r="D138" s="56">
+      <c r="D148" s="56">
         <v>40.004083860000001</v>
       </c>
-      <c r="E138" s="54">
+      <c r="E148" s="54">
         <v>40.020159249999999</v>
       </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B149" s="198" t="s">
+        <v>177</v>
+      </c>
+      <c r="C149" s="202">
+        <f>MAX(C143:C148)-MIN(C143:C148)</f>
+        <v>7.6999999999998181E-3</v>
+      </c>
+      <c r="D149" s="203">
+        <f>MAX(D143:D148)-MIN(D143:D148)</f>
+        <v>5.7000000452944732E-7</v>
+      </c>
+      <c r="E149" s="204">
+        <f>MAX(E143:E148)-MIN(E143:E148)</f>
+        <v>8.4571000000011054E-4</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B150" s="185" t="s">
+        <v>179</v>
+      </c>
+      <c r="C150" s="205">
+        <f>STDEV(C143:C148)</f>
+        <v>3.1123410267297948E-3</v>
+      </c>
+      <c r="D150" s="52">
+        <f>STDEV(D143:D148)</f>
+        <v>2.3270152741354107E-7</v>
+      </c>
+      <c r="E150" s="58">
+        <f>STDEV(E143:E148)</f>
+        <v>3.1432180049466578E-4</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C151" s="206">
+        <f>MAX(C149:E149)</f>
+        <v>7.6999999999998181E-3</v>
+      </c>
+      <c r="D151" s="56"/>
+      <c r="E151" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add more accuracy calcs
</commit_message>
<xml_diff>
--- a/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
+++ b/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anderssandstrom/ecmc_bifrost_vac_tank_sat/docs/testplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC34FF3B-7E19-244A-8F90-41190A323782}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2706F7FF-AE27-0341-8B5E-BA64168BEBE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="16520" activeTab="5" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
+    <workbookView xWindow="1360" yWindow="3120" windowWidth="27800" windowHeight="16520" activeTab="5" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="15" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="186">
   <si>
     <t>General Inspection</t>
   </si>
@@ -689,6 +689,12 @@
   <si>
     <t>BELOW Before COLLISION reduced datapoints</t>
   </si>
+  <si>
+    <t>BELOW Before COLLISION without 0 outlier</t>
+  </si>
+  <si>
+    <t>Excluded </t>
+  </si>
 </sst>
 </file>
 
@@ -699,7 +705,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -828,6 +834,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1657,7 +1669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1962,6 +1974,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4637,10 +4651,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CEB521-8DC8-0C48-A601-3238D1EFF0A3}">
-  <dimension ref="B2:Z86"/>
+  <dimension ref="B2:Z123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6133,231 +6147,279 @@
         <v>1.0001512578738871</v>
       </c>
     </row>
-    <row r="70" spans="2:25" s="125" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="129"/>
-      <c r="D70" s="129"/>
-      <c r="E70" s="129" t="s">
-        <v>183</v>
-      </c>
-      <c r="R70" s="126"/>
-      <c r="S70" s="127"/>
-      <c r="T70" s="127"/>
-      <c r="U70" s="127"/>
-      <c r="V70" s="127"/>
-      <c r="W70" s="127"/>
-      <c r="X70" s="127"/>
-      <c r="Y70" s="128"/>
-    </row>
-    <row r="72" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:25" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="129"/>
+      <c r="D68" s="129"/>
+      <c r="E68" s="129" t="s">
+        <v>184</v>
+      </c>
+      <c r="R68" s="126"/>
+      <c r="S68" s="127"/>
+      <c r="T68" s="127"/>
+      <c r="U68" s="127"/>
+      <c r="V68" s="127"/>
+      <c r="W68" s="127"/>
+      <c r="X68" s="127"/>
+      <c r="Y68" s="128"/>
+    </row>
+    <row r="70" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71" s="95" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="E71" s="113" t="s">
+        <v>160</v>
+      </c>
+      <c r="F71" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="G71" s="94" t="s">
+        <v>159</v>
+      </c>
+      <c r="H71" s="112"/>
+      <c r="I71" s="112"/>
+      <c r="J71" s="112"/>
+      <c r="K71" s="112"/>
+      <c r="L71" s="114"/>
+      <c r="M71" s="114"/>
+      <c r="N71" s="114"/>
+      <c r="O71" s="114"/>
+    </row>
+    <row r="72" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B72" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" s="108"/>
+      <c r="D72" s="108"/>
+      <c r="E72" s="108"/>
+      <c r="F72" s="108"/>
+      <c r="G72" s="109"/>
+      <c r="H72" s="112"/>
+      <c r="I72" s="112"/>
+      <c r="J72" s="112"/>
+      <c r="K72" s="112"/>
+      <c r="L72" s="112"/>
+      <c r="M72" s="112"/>
+      <c r="N72" s="112"/>
+      <c r="O72" s="112"/>
+    </row>
     <row r="73" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="C73" s="95" t="s">
-        <v>106</v>
-      </c>
-      <c r="D73" s="93" t="s">
-        <v>107</v>
-      </c>
-      <c r="E73" s="113" t="s">
-        <v>160</v>
-      </c>
-      <c r="F73" s="94" t="s">
-        <v>108</v>
-      </c>
-      <c r="G73" s="94" t="s">
-        <v>159</v>
-      </c>
-      <c r="H73" s="112"/>
-      <c r="I73" s="112"/>
-      <c r="J73" s="112"/>
-      <c r="K73" s="112"/>
-      <c r="L73" s="114"/>
-      <c r="M73" s="114"/>
-      <c r="N73" s="114"/>
-      <c r="O73" s="114"/>
-    </row>
-    <row r="74" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B74" s="107" t="s">
-        <v>141</v>
-      </c>
-      <c r="C74" s="108">
-        <v>-10.98</v>
-      </c>
-      <c r="D74" s="108">
-        <v>-10.978210375023499</v>
-      </c>
-      <c r="E74" s="108">
-        <f>ABS(C74-D74)</f>
-        <v>1.7896249765012584E-3</v>
-      </c>
-      <c r="F74" s="108">
-        <v>-10.974417235955199</v>
-      </c>
-      <c r="G74" s="109">
-        <f>ABS(C74-F74)</f>
-        <v>5.5827640448011806E-3</v>
-      </c>
-      <c r="H74" s="112"/>
-      <c r="I74" s="112"/>
-      <c r="J74" s="112"/>
-      <c r="K74" s="112"/>
-      <c r="L74" s="112"/>
-      <c r="M74" s="112"/>
-      <c r="N74" s="112"/>
-      <c r="O74" s="112"/>
-    </row>
-    <row r="75" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="106">
+      <c r="B73" s="106">
         <v>-5</v>
       </c>
-      <c r="C75" s="171" t="s">
-        <v>144</v>
-      </c>
-      <c r="D75" s="171">
-        <v>-5.0096773753587298</v>
+      <c r="C73" s="171">
+        <v>-5.0176999999999996</v>
+      </c>
+      <c r="D73" s="171">
+        <v>-5.0194000000000001</v>
+      </c>
+      <c r="E73" s="172">
+        <f t="shared" ref="E73:E83" si="4">ABS(C73-D73)</f>
+        <v>1.7000000000004789E-3</v>
+      </c>
+      <c r="F73" s="171">
+        <v>-5.0212500000000002</v>
+      </c>
+      <c r="G73" s="176">
+        <f t="shared" ref="G73:G83" si="5">ABS(C73-F73)</f>
+        <v>3.5500000000006082E-3</v>
+      </c>
+      <c r="H73" s="110"/>
+      <c r="I73" s="110"/>
+      <c r="J73" s="111"/>
+      <c r="K73" s="111"/>
+      <c r="L73" s="115"/>
+      <c r="M73" s="116"/>
+      <c r="N73" s="116"/>
+      <c r="O73" s="116"/>
+    </row>
+    <row r="74" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="80">
+        <v>0</v>
+      </c>
+      <c r="C74" s="173"/>
+      <c r="D74" s="173" t="s">
+        <v>185</v>
+      </c>
+      <c r="E74" s="172"/>
+      <c r="F74" s="173" t="s">
+        <v>185</v>
+      </c>
+      <c r="G74" s="176"/>
+      <c r="H74" s="110"/>
+      <c r="I74" s="110"/>
+      <c r="J74" s="111"/>
+      <c r="K74" s="122"/>
+      <c r="L74" s="121" t="s">
+        <v>158</v>
+      </c>
+      <c r="M74" s="119" t="s">
+        <v>151</v>
+      </c>
+      <c r="N74" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="O74" s="111"/>
+    </row>
+    <row r="75" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B75" s="80">
+        <v>5</v>
+      </c>
+      <c r="C75" s="173">
+        <v>4.9862000000000002</v>
+      </c>
+      <c r="D75" s="173">
+        <v>4.9862000000000002</v>
       </c>
       <c r="E75" s="172">
-        <f t="shared" ref="E75:E85" si="4">ABS(C75-D75)</f>
-        <v>8.0226246412697932E-3</v>
-      </c>
-      <c r="F75" s="171">
-        <v>-5.0102009745677902</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F75" s="173">
+        <v>4.9874999999999998</v>
       </c>
       <c r="G75" s="176">
-        <f t="shared" ref="G75:G85" si="5">ABS(C75-F75)</f>
-        <v>7.4990254322093719E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.2999999999996348E-3</v>
       </c>
       <c r="H75" s="110"/>
       <c r="I75" s="110"/>
       <c r="J75" s="111"/>
-      <c r="K75" s="111"/>
-      <c r="L75" s="115"/>
-      <c r="M75" s="116"/>
-      <c r="N75" s="116"/>
-      <c r="O75" s="116"/>
+      <c r="K75" s="123" t="s">
+        <v>156</v>
+      </c>
+      <c r="L75" s="166">
+        <v>8.1062000000000004E-5</v>
+      </c>
+      <c r="M75" s="166">
+        <v>-1.66E-2</v>
+      </c>
+      <c r="N75" s="166">
+        <f>MAX(E73:E83)</f>
+        <v>3.8999999999980162E-3</v>
+      </c>
+      <c r="O75" s="111"/>
     </row>
     <row r="76" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="80">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C76" s="173">
-        <v>1.9199999999999998E-2</v>
+        <v>9.9887999999999995</v>
       </c>
       <c r="D76" s="173">
-        <v>-8.1487286875825005E-3</v>
+        <v>9.9890000000000008</v>
       </c>
       <c r="E76" s="172">
         <f t="shared" si="4"/>
-        <v>2.7348728687582501E-2</v>
+        <v>2.0000000000131024E-4</v>
       </c>
       <c r="F76" s="173">
-        <v>-1.17485980349982E-2</v>
+        <v>9.9920000000000009</v>
       </c>
       <c r="G76" s="176">
         <f t="shared" si="5"/>
-        <v>3.09485980349982E-2</v>
+        <v>3.2000000000014239E-3</v>
       </c>
       <c r="H76" s="110"/>
       <c r="I76" s="110"/>
       <c r="J76" s="111"/>
-      <c r="K76" s="122"/>
-      <c r="L76" s="121" t="s">
-        <v>158</v>
-      </c>
-      <c r="M76" s="119" t="s">
-        <v>151</v>
-      </c>
-      <c r="N76" s="120" t="s">
-        <v>24</v>
+      <c r="K76" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="L76" s="166">
+        <v>-4.4524999999999998E-5</v>
+      </c>
+      <c r="M76" s="166">
+        <v>30.726199999999999</v>
+      </c>
+      <c r="N76" s="167">
+        <f>MAX(G73:G83)</f>
+        <v>6.7000000000003723E-3</v>
       </c>
       <c r="O76" s="111"/>
     </row>
     <row r="77" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B77" s="80">
-        <v>5</v>
-      </c>
+      <c r="B77" s="80"/>
       <c r="C77" s="173">
-        <v>4.9862000000000002</v>
+        <v>14.989699999999999</v>
       </c>
       <c r="D77" s="173">
-        <v>4.9933787789488502</v>
+        <v>14.991899999999999</v>
       </c>
       <c r="E77" s="172">
         <f t="shared" si="4"/>
-        <v>7.1787789488499953E-3</v>
+        <v>2.2000000000002018E-3</v>
       </c>
       <c r="F77" s="173">
-        <v>4.9956060588578</v>
+        <v>14.9964</v>
       </c>
       <c r="G77" s="176">
         <f t="shared" si="5"/>
-        <v>9.4060588577997706E-3</v>
+        <v>6.7000000000003723E-3</v>
       </c>
       <c r="H77" s="110"/>
       <c r="I77" s="110"/>
       <c r="J77" s="111"/>
-      <c r="K77" s="123" t="s">
-        <v>156</v>
-      </c>
-      <c r="L77" s="96">
-        <v>8.1041246399999998E-5</v>
-      </c>
-      <c r="M77" s="168">
-        <v>-8.1453097600000003E-3</v>
-      </c>
-      <c r="N77" s="166">
-        <f>MAX(E75:E85)</f>
-        <v>2.7348728687582501E-2</v>
-      </c>
+      <c r="K77" s="111"/>
+      <c r="L77" s="111"/>
+      <c r="M77" s="111"/>
+      <c r="N77" s="111"/>
       <c r="O77" s="111"/>
     </row>
-    <row r="78" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="80">
-        <v>10</v>
-      </c>
-      <c r="C78" s="173">
-        <v>9.9887999999999995</v>
-      </c>
-      <c r="D78" s="173">
-        <v>9.9949074254174004</v>
+    <row r="78" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B78" s="80"/>
+      <c r="C78" s="174">
+        <v>19.995100000000001</v>
+      </c>
+      <c r="D78" s="174">
+        <v>19.994700000000002</v>
       </c>
       <c r="E78" s="172">
         <f t="shared" si="4"/>
-        <v>6.1074254174009468E-3</v>
-      </c>
-      <c r="F78" s="173">
-        <v>9.9986431097759993</v>
+        <v>3.9999999999906777E-4</v>
+      </c>
+      <c r="F78" s="174">
+        <v>19.994199999999999</v>
       </c>
       <c r="G78" s="176">
         <f t="shared" si="5"/>
-        <v>9.843109775999892E-3</v>
+        <v>9.0000000000145519E-4</v>
       </c>
       <c r="H78" s="110"/>
       <c r="I78" s="110"/>
       <c r="J78" s="111"/>
-      <c r="K78" s="124" t="s">
-        <v>157</v>
-      </c>
-      <c r="L78" s="55">
-        <v>-4.4511401799999998E-5</v>
-      </c>
-      <c r="M78" s="170">
-        <v>30.7267127</v>
-      </c>
-      <c r="N78" s="167">
-        <f>MAX(G75:G85)</f>
-        <v>3.09485980349982E-2</v>
-      </c>
+      <c r="K78" s="111"/>
+      <c r="L78" s="111"/>
+      <c r="M78" s="111"/>
+      <c r="N78" s="111"/>
       <c r="O78" s="111"/>
     </row>
     <row r="79" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B79" s="80"/>
-      <c r="C79" s="173"/>
-      <c r="D79" s="173"/>
-      <c r="E79" s="172"/>
-      <c r="F79" s="173"/>
-      <c r="G79" s="176"/>
+      <c r="C79" s="173">
+        <v>24.9998</v>
+      </c>
+      <c r="D79" s="173">
+        <v>24.997499999999999</v>
+      </c>
+      <c r="E79" s="172">
+        <f t="shared" si="4"/>
+        <v>2.3000000000017451E-3</v>
+      </c>
+      <c r="F79" s="173">
+        <v>24.994900000000001</v>
+      </c>
+      <c r="G79" s="176">
+        <f t="shared" si="5"/>
+        <v>4.8999999999992383E-3</v>
+      </c>
       <c r="H79" s="110"/>
       <c r="I79" s="110"/>
       <c r="J79" s="111"/>
@@ -6369,11 +6431,23 @@
     </row>
     <row r="80" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B80" s="80"/>
-      <c r="C80" s="174"/>
-      <c r="D80" s="174"/>
-      <c r="E80" s="172"/>
-      <c r="F80" s="174"/>
-      <c r="G80" s="176"/>
+      <c r="C80" s="173">
+        <v>29.996500000000001</v>
+      </c>
+      <c r="D80" s="173">
+        <v>30.000399999999999</v>
+      </c>
+      <c r="E80" s="172">
+        <f t="shared" si="4"/>
+        <v>3.8999999999980162E-3</v>
+      </c>
+      <c r="F80" s="173">
+        <v>29.994399999999999</v>
+      </c>
+      <c r="G80" s="176">
+        <f t="shared" si="5"/>
+        <v>2.1000000000022112E-3</v>
+      </c>
       <c r="H80" s="110"/>
       <c r="I80" s="110"/>
       <c r="J80" s="111"/>
@@ -6383,13 +6457,27 @@
       <c r="N80" s="111"/>
       <c r="O80" s="111"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B81" s="80"/>
-      <c r="C81" s="173"/>
-      <c r="D81" s="173"/>
-      <c r="E81" s="172"/>
-      <c r="F81" s="173"/>
-      <c r="G81" s="176"/>
+    <row r="81" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B81" s="80">
+        <v>35</v>
+      </c>
+      <c r="C81" s="173">
+        <v>35.000500000000002</v>
+      </c>
+      <c r="D81" s="173">
+        <v>35.0032</v>
+      </c>
+      <c r="E81" s="172">
+        <f t="shared" si="4"/>
+        <v>2.6999999999972601E-3</v>
+      </c>
+      <c r="F81" s="173">
+        <v>34.998100000000001</v>
+      </c>
+      <c r="G81" s="176">
+        <f t="shared" si="5"/>
+        <v>2.400000000001512E-3</v>
+      </c>
       <c r="H81" s="110"/>
       <c r="I81" s="110"/>
       <c r="J81" s="111"/>
@@ -6399,42 +6487,53 @@
       <c r="N81" s="111"/>
       <c r="O81" s="111"/>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B82" s="80"/>
-      <c r="C82" s="173"/>
-      <c r="D82" s="173"/>
-      <c r="E82" s="172"/>
-      <c r="F82" s="173"/>
-      <c r="G82" s="176"/>
+    <row r="82" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B82" s="83"/>
+      <c r="C82" s="175">
+        <v>40.009500000000003</v>
+      </c>
+      <c r="D82" s="175">
+        <v>40.006</v>
+      </c>
+      <c r="E82" s="172">
+        <f t="shared" si="4"/>
+        <v>3.5000000000025011E-3</v>
+      </c>
+      <c r="F82" s="175">
+        <v>40.007100000000001</v>
+      </c>
+      <c r="G82" s="176">
+        <f t="shared" si="5"/>
+        <v>2.400000000001512E-3</v>
+      </c>
       <c r="H82" s="110"/>
       <c r="I82" s="110"/>
-      <c r="J82" s="111"/>
       <c r="K82" s="111"/>
       <c r="L82" s="111"/>
       <c r="M82" s="111"/>
       <c r="N82" s="111"/>
       <c r="O82" s="111"/>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B83" s="80">
-        <v>35</v>
-      </c>
-      <c r="C83" s="173">
-        <v>35.000500000000002</v>
-      </c>
-      <c r="D83" s="173">
-        <v>35.002548380501104</v>
+    <row r="83" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B83" s="83">
+        <v>45</v>
+      </c>
+      <c r="C83" s="175">
+        <v>45.012700000000002</v>
+      </c>
+      <c r="D83" s="175">
+        <v>45.008899999999997</v>
       </c>
       <c r="E83" s="172">
         <f t="shared" si="4"/>
-        <v>2.0483805011011214E-3</v>
-      </c>
-      <c r="F83" s="173">
-        <v>34.997359145700898</v>
+        <v>3.8000000000053547E-3</v>
+      </c>
+      <c r="F83" s="175">
+        <v>45.015000000000001</v>
       </c>
       <c r="G83" s="176">
         <f t="shared" si="5"/>
-        <v>3.1408542991044897E-3</v>
+        <v>2.2999999999981924E-3</v>
       </c>
       <c r="H83" s="110"/>
       <c r="I83" s="110"/>
@@ -6445,70 +6544,417 @@
       <c r="N83" s="111"/>
       <c r="O83" s="111"/>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B84" s="83"/>
-      <c r="C84" s="175"/>
-      <c r="D84" s="175"/>
-      <c r="E84" s="172"/>
-      <c r="F84" s="175"/>
-      <c r="G84" s="176"/>
-      <c r="H84" s="110"/>
-      <c r="I84" s="110"/>
+    <row r="84" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="81" t="s">
+        <v>142</v>
+      </c>
+      <c r="C84" s="169"/>
+      <c r="D84" s="169"/>
+      <c r="E84" s="177"/>
+      <c r="F84" s="169"/>
+      <c r="G84" s="178"/>
+      <c r="H84" s="111"/>
+      <c r="I84" s="111"/>
+      <c r="J84" s="111"/>
       <c r="K84" s="111"/>
       <c r="L84" s="111"/>
       <c r="M84" s="111"/>
       <c r="N84" s="111"/>
       <c r="O84" s="111"/>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B85" s="83">
+    <row r="87" spans="2:25" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="129"/>
+      <c r="D87" s="129"/>
+      <c r="E87" s="129" t="s">
+        <v>183</v>
+      </c>
+      <c r="R87" s="126"/>
+      <c r="S87" s="127"/>
+      <c r="T87" s="127"/>
+      <c r="U87" s="127"/>
+      <c r="V87" s="127"/>
+      <c r="W87" s="127"/>
+      <c r="X87" s="127"/>
+      <c r="Y87" s="128"/>
+    </row>
+    <row r="89" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="C90" s="95" t="s">
+        <v>106</v>
+      </c>
+      <c r="D90" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="E90" s="113" t="s">
+        <v>160</v>
+      </c>
+      <c r="F90" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="G90" s="94" t="s">
+        <v>159</v>
+      </c>
+      <c r="H90" s="112"/>
+      <c r="I90" s="112"/>
+      <c r="J90" s="112"/>
+      <c r="K90" s="112"/>
+      <c r="L90" s="114"/>
+      <c r="M90" s="114"/>
+      <c r="N90" s="114"/>
+      <c r="O90" s="114"/>
+    </row>
+    <row r="91" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B91" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="C91" s="108"/>
+      <c r="D91" s="108"/>
+      <c r="E91" s="108"/>
+      <c r="F91" s="108"/>
+      <c r="G91" s="109"/>
+      <c r="H91" s="112"/>
+      <c r="I91" s="112"/>
+      <c r="J91" s="112"/>
+      <c r="K91" s="112"/>
+      <c r="L91" s="112"/>
+      <c r="M91" s="112"/>
+      <c r="N91" s="112"/>
+      <c r="O91" s="112"/>
+    </row>
+    <row r="92" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="106">
+        <v>-5</v>
+      </c>
+      <c r="C92" s="171" t="s">
+        <v>144</v>
+      </c>
+      <c r="D92" s="171">
+        <v>-5.0187746972428604</v>
+      </c>
+      <c r="E92" s="172">
+        <f t="shared" ref="E92:E102" si="6">ABS(C92-D92)</f>
+        <v>1.0746972428608004E-3</v>
+      </c>
+      <c r="F92" s="171">
+        <v>-5.0202362811728003</v>
+      </c>
+      <c r="G92" s="176">
+        <f t="shared" ref="G92:G102" si="7">ABS(C92-F92)</f>
+        <v>2.5362811728006918E-3</v>
+      </c>
+      <c r="H92" s="110"/>
+      <c r="I92" s="110"/>
+      <c r="J92" s="111"/>
+      <c r="K92" s="111"/>
+      <c r="L92" s="115"/>
+      <c r="M92" s="116"/>
+      <c r="N92" s="116"/>
+      <c r="O92" s="116"/>
+    </row>
+    <row r="93" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="80"/>
+      <c r="C93" s="173"/>
+      <c r="D93" s="171"/>
+      <c r="E93" s="172"/>
+      <c r="F93" s="171"/>
+      <c r="G93" s="176"/>
+      <c r="H93" s="110"/>
+      <c r="I93" s="110"/>
+      <c r="J93" s="111"/>
+      <c r="K93" s="122"/>
+      <c r="L93" s="121" t="s">
+        <v>158</v>
+      </c>
+      <c r="M93" s="119" t="s">
+        <v>151</v>
+      </c>
+      <c r="N93" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="O93" s="111"/>
+    </row>
+    <row r="94" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B94" s="80">
+        <v>5</v>
+      </c>
+      <c r="C94" s="173">
+        <v>4.9862000000000002</v>
+      </c>
+      <c r="D94" s="171">
+        <v>4.98658796291366</v>
+      </c>
+      <c r="E94" s="172">
+        <f t="shared" si="6"/>
+        <v>3.8796291365983393E-4</v>
+      </c>
+      <c r="F94" s="171">
+        <v>4.9877635982127897</v>
+      </c>
+      <c r="G94" s="176">
+        <f t="shared" si="7"/>
+        <v>1.5635982127895076E-3</v>
+      </c>
+      <c r="H94" s="110"/>
+      <c r="I94" s="110"/>
+      <c r="J94" s="111"/>
+      <c r="K94" s="123" t="s">
+        <v>156</v>
+      </c>
+      <c r="L94" s="96">
+        <v>8.1041246399999998E-5</v>
+      </c>
+      <c r="M94" s="168">
+        <v>-8.1453097600000003E-3</v>
+      </c>
+      <c r="N94" s="166">
+        <f>MAX(E92:E102)</f>
+        <v>4.6602567576030651E-3</v>
+      </c>
+      <c r="O94" s="111"/>
+    </row>
+    <row r="95" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="80">
+        <v>10</v>
+      </c>
+      <c r="C95" s="173">
+        <v>9.9887999999999995</v>
+      </c>
+      <c r="D95" s="171">
+        <v>9.9892698624379594</v>
+      </c>
+      <c r="E95" s="172">
+        <f t="shared" si="6"/>
+        <v>4.6986243795998917E-4</v>
+      </c>
+      <c r="F95" s="171">
+        <v>9.9918971013759901</v>
+      </c>
+      <c r="G95" s="176">
+        <f t="shared" si="7"/>
+        <v>3.0971013759906185E-3</v>
+      </c>
+      <c r="H95" s="110"/>
+      <c r="I95" s="110"/>
+      <c r="J95" s="111"/>
+      <c r="K95" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="L95" s="55">
+        <v>-4.4511401799999998E-5</v>
+      </c>
+      <c r="M95" s="170">
+        <v>30.7267127</v>
+      </c>
+      <c r="N95" s="167">
+        <f>MAX(G92:G102)</f>
+        <v>4.4082108241028095E-3</v>
+      </c>
+      <c r="O95" s="111"/>
+    </row>
+    <row r="96" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B96" s="80"/>
+      <c r="C96" s="173"/>
+      <c r="D96" s="171"/>
+      <c r="E96" s="172"/>
+      <c r="F96" s="173"/>
+      <c r="G96" s="176"/>
+      <c r="H96" s="110"/>
+      <c r="I96" s="110"/>
+      <c r="J96" s="111"/>
+      <c r="K96" s="111"/>
+      <c r="L96" s="111"/>
+      <c r="M96" s="111"/>
+      <c r="N96" s="111"/>
+      <c r="O96" s="111"/>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B97" s="80"/>
+      <c r="C97" s="174"/>
+      <c r="D97" s="171"/>
+      <c r="E97" s="172"/>
+      <c r="F97" s="174"/>
+      <c r="G97" s="176"/>
+      <c r="H97" s="110"/>
+      <c r="I97" s="110"/>
+      <c r="J97" s="111"/>
+      <c r="K97" s="111"/>
+      <c r="L97" s="111"/>
+      <c r="M97" s="111"/>
+      <c r="N97" s="111"/>
+      <c r="O97" s="111"/>
+    </row>
+    <row r="98" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B98" s="80"/>
+      <c r="C98" s="173"/>
+      <c r="D98" s="171"/>
+      <c r="E98" s="172"/>
+      <c r="F98" s="173"/>
+      <c r="G98" s="176"/>
+      <c r="H98" s="110"/>
+      <c r="I98" s="110"/>
+      <c r="J98" s="111"/>
+      <c r="K98" s="111"/>
+      <c r="L98" s="111"/>
+      <c r="M98" s="111"/>
+      <c r="N98" s="111"/>
+      <c r="O98" s="111"/>
+    </row>
+    <row r="99" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B99" s="80"/>
+      <c r="C99" s="173"/>
+      <c r="D99" s="173"/>
+      <c r="E99" s="172"/>
+      <c r="F99" s="173"/>
+      <c r="G99" s="176"/>
+      <c r="H99" s="110"/>
+      <c r="I99" s="110"/>
+      <c r="J99" s="111"/>
+      <c r="K99" s="111"/>
+      <c r="L99" s="111"/>
+      <c r="M99" s="111"/>
+      <c r="N99" s="111"/>
+      <c r="O99" s="111"/>
+    </row>
+    <row r="100" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B100" s="80">
+        <v>35</v>
+      </c>
+      <c r="C100" s="173">
+        <v>35.000500000000002</v>
+      </c>
+      <c r="D100" s="173">
+        <v>35.002677082275298</v>
+      </c>
+      <c r="E100" s="172">
+        <f t="shared" si="6"/>
+        <v>2.177082275295561E-3</v>
+      </c>
+      <c r="F100" s="173">
+        <v>34.9960917891759</v>
+      </c>
+      <c r="G100" s="176">
+        <f t="shared" si="7"/>
+        <v>4.4082108241028095E-3</v>
+      </c>
+      <c r="H100" s="110"/>
+      <c r="I100" s="110"/>
+      <c r="J100" s="111"/>
+      <c r="K100" s="111"/>
+      <c r="L100" s="111"/>
+      <c r="M100" s="111"/>
+      <c r="N100" s="111"/>
+      <c r="O100" s="111"/>
+    </row>
+    <row r="101" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B101" s="83"/>
+      <c r="C101" s="175"/>
+      <c r="D101" s="175"/>
+      <c r="E101" s="172"/>
+      <c r="F101" s="175"/>
+      <c r="G101" s="176"/>
+      <c r="H101" s="110"/>
+      <c r="I101" s="110"/>
+      <c r="K101" s="111"/>
+      <c r="L101" s="111"/>
+      <c r="M101" s="111"/>
+      <c r="N101" s="111"/>
+      <c r="O101" s="111"/>
+    </row>
+    <row r="102" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B102" s="83">
         <v>45</v>
       </c>
-      <c r="C85" s="175">
+      <c r="C102" s="175">
         <v>45.012700000000002</v>
       </c>
-      <c r="D85" s="175">
-        <v>45.005604535619099</v>
-      </c>
-      <c r="E85" s="172">
-        <f t="shared" si="4"/>
-        <v>7.0954643809031381E-3</v>
-      </c>
-      <c r="F85" s="175">
-        <v>45.0113562770578</v>
-      </c>
-      <c r="G85" s="176">
-        <f t="shared" si="5"/>
-        <v>1.3437229422024188E-3</v>
-      </c>
-      <c r="H85" s="110"/>
-      <c r="I85" s="110"/>
-      <c r="J85" s="111"/>
-      <c r="K85" s="111"/>
-      <c r="L85" s="111"/>
-      <c r="M85" s="111"/>
-      <c r="N85" s="111"/>
-      <c r="O85" s="111"/>
-    </row>
-    <row r="86" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="81" t="s">
+      <c r="D102" s="175">
+        <v>45.008039743242399</v>
+      </c>
+      <c r="E102" s="172">
+        <f t="shared" si="6"/>
+        <v>4.6602567576030651E-3</v>
+      </c>
+      <c r="F102" s="175">
+        <v>45.012283561412801</v>
+      </c>
+      <c r="G102" s="176">
+        <f t="shared" si="7"/>
+        <v>4.1643858720163962E-4</v>
+      </c>
+      <c r="H102" s="110"/>
+      <c r="I102" s="110"/>
+      <c r="J102" s="111"/>
+      <c r="K102" s="111"/>
+      <c r="L102" s="111"/>
+      <c r="M102" s="111"/>
+      <c r="N102" s="111"/>
+      <c r="O102" s="111"/>
+    </row>
+    <row r="103" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="C86" s="169">
-        <v>48.5</v>
-      </c>
-      <c r="D86" s="169"/>
-      <c r="E86" s="177"/>
-      <c r="F86" s="169"/>
-      <c r="G86" s="178"/>
-      <c r="H86" s="111"/>
-      <c r="I86" s="111"/>
-      <c r="J86" s="111"/>
-      <c r="K86" s="111"/>
-      <c r="L86" s="111"/>
-      <c r="M86" s="111"/>
-      <c r="N86" s="111"/>
-      <c r="O86" s="111"/>
+      <c r="C103" s="169"/>
+      <c r="D103" s="169"/>
+      <c r="E103" s="177"/>
+      <c r="F103" s="169"/>
+      <c r="G103" s="178"/>
+      <c r="H103" s="111"/>
+      <c r="I103" s="111"/>
+      <c r="J103" s="111"/>
+      <c r="K103" s="111"/>
+      <c r="L103" s="111"/>
+      <c r="M103" s="111"/>
+      <c r="N103" s="111"/>
+      <c r="O103" s="111"/>
+    </row>
+    <row r="109" spans="2:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="C109" s="218"/>
+    </row>
+    <row r="110" spans="2:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="C110" s="218"/>
+    </row>
+    <row r="111" spans="2:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="C111" s="218"/>
+    </row>
+    <row r="112" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C112" s="219"/>
+    </row>
+    <row r="113" spans="3:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C113" s="218"/>
+    </row>
+    <row r="114" spans="3:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C114" s="218"/>
+    </row>
+    <row r="115" spans="3:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C115" s="218"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C116" s="219"/>
+    </row>
+    <row r="117" spans="3:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C117" s="218"/>
+    </row>
+    <row r="118" spans="3:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C118" s="218"/>
+    </row>
+    <row r="119" spans="3:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C119" s="218"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C120" s="219"/>
+    </row>
+    <row r="121" spans="3:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C121" s="218"/>
+    </row>
+    <row r="122" spans="3:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C122" s="218"/>
+    </row>
+    <row r="123" spans="3:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C123" s="218"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add repeatability and accuracy cahpters
</commit_message>
<xml_diff>
--- a/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
+++ b/docs/testplan/SAT_TEMPLATE_v0_1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anderssandstrom/ecmc_bifrost_vac_tank_sat/docs/testplan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\federicorojas\Documents\FAT_SAT\ecmc_bifrost_vac_tank_sat\docs\testplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E63F49F-6F0E-6D46-95B4-5E7F7D4A7C76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="1220" windowWidth="27800" windowHeight="16520" activeTab="1" xr2:uid="{D3CCAE6E-ED0A-164C-8A50-F00EEBDAA32D}"/>
+    <workbookView xWindow="5724" yWindow="1224" windowWidth="27804" windowHeight="16524" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="15" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Accuracy" sheetId="12" r:id="rId6"/>
     <sheet name="Repeatability" sheetId="18" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="214">
   <si>
     <t>General Inspection</t>
   </si>
@@ -670,20 +669,23 @@
   </si>
   <si>
     <t>Dent on posital encoder housing. Encoder was concluded to work correct.</t>
+  </si>
+  <si>
+    <t>repeatabilty  no laser scanner and no -5 measuremnet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1654,7 +1656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1974,17 +1976,17 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2001,6 +2003,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2456,22 +2460,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CCFE59-F0B8-B348-A215-20650DA579DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:C25"/>
   <sheetViews>
     <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.1640625" customWidth="1"/>
+    <col min="3" max="3" width="53.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:3" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="16.2" thickBot="1"/>
+    <row r="6" spans="2:3" ht="18.600000000000001" thickBot="1">
       <c r="B6" s="57" t="s">
         <v>69</v>
       </c>
@@ -2479,7 +2483,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="18">
       <c r="B7" s="59" t="s">
         <v>53</v>
       </c>
@@ -2487,7 +2491,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="18">
       <c r="B8" s="60" t="s">
         <v>54</v>
       </c>
@@ -2495,7 +2499,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="18">
       <c r="B9" s="60" t="s">
         <v>55</v>
       </c>
@@ -2503,7 +2507,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="40" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="54">
       <c r="B10" s="60" t="s">
         <v>56</v>
       </c>
@@ -2511,7 +2515,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="18">
       <c r="B11" s="60" t="s">
         <v>57</v>
       </c>
@@ -2519,7 +2523,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="36">
       <c r="B12" s="60" t="s">
         <v>58</v>
       </c>
@@ -2527,7 +2531,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" ht="18">
       <c r="B13" s="60" t="s">
         <v>59</v>
       </c>
@@ -2535,7 +2539,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" ht="18">
       <c r="B14" s="60" t="s">
         <v>60</v>
       </c>
@@ -2543,31 +2547,31 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3">
       <c r="C15" s="55"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="54"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="54"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="54"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="54"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="54"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="54"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="54"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" s="54"/>
     </row>
   </sheetData>
@@ -2577,35 +2581,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91EDC4E-2031-9045-973C-F1B4515431EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="150" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="31"/>
-    <col min="2" max="2" width="10.83203125" style="31" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="31"/>
+    <col min="2" max="2" width="10.796875" style="31" customWidth="1"/>
+    <col min="3" max="3" width="21.796875" style="31" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" style="31" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="31" customWidth="1"/>
-    <col min="6" max="6" width="39.1640625" style="37" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="31"/>
+    <col min="6" max="6" width="39.19921875" style="37" customWidth="1"/>
+    <col min="7" max="16384" width="10.796875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:6">
       <c r="F1" s="32"/>
     </row>
-    <row r="2" spans="2:6" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" ht="12.6" thickBot="1">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="2:6" s="33" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" s="33" customFormat="1" ht="12.6" thickBot="1">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2622,7 +2626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" ht="12.6" thickBot="1">
       <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
@@ -2633,7 +2637,7 @@
       <c r="E4" s="11"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="2:6" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" ht="12.6" thickBot="1">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2644,7 +2648,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" ht="24.6" thickBot="1">
       <c r="B6" s="15" t="s">
         <v>5</v>
       </c>
@@ -2659,7 +2663,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" ht="12.6" thickBot="1">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2670,7 +2674,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="2:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:6">
       <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
@@ -2681,7 +2685,7 @@
       <c r="E8" s="235"/>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="2:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:6">
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -2694,7 +2698,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="2:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:6">
       <c r="B10" s="18" t="s">
         <v>8</v>
       </c>
@@ -2707,7 +2711,7 @@
       </c>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" spans="2:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:6">
       <c r="B11" s="18" t="s">
         <v>9</v>
       </c>
@@ -2720,7 +2724,7 @@
       </c>
       <c r="F11" s="20"/>
     </row>
-    <row r="12" spans="2:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:6">
       <c r="B12" s="18" t="s">
         <v>10</v>
       </c>
@@ -2733,7 +2737,7 @@
       </c>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="2:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:6">
       <c r="B13" s="18" t="s">
         <v>11</v>
       </c>
@@ -2746,7 +2750,7 @@
       </c>
       <c r="F13" s="20"/>
     </row>
-    <row r="14" spans="2:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:6">
       <c r="B14" s="18" t="s">
         <v>12</v>
       </c>
@@ -2761,7 +2765,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:6">
       <c r="B15" s="18" t="s">
         <v>21</v>
       </c>
@@ -2774,7 +2778,7 @@
       </c>
       <c r="F15" s="20"/>
     </row>
-    <row r="16" spans="2:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" ht="12.6" thickBot="1">
       <c r="B16" s="21" t="s">
         <v>21</v>
       </c>
@@ -2787,8 +2791,8 @@
       </c>
       <c r="F16" s="23"/>
     </row>
-    <row r="17" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="12.6" thickBot="1"/>
+    <row r="18" spans="1:18" ht="12.6" thickBot="1">
       <c r="B18" s="8" t="s">
         <v>16</v>
       </c>
@@ -2799,7 +2803,7 @@
       <c r="E18" s="11"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18">
       <c r="A19" s="34" t="s">
         <v>29</v>
       </c>
@@ -2817,7 +2821,7 @@
       </c>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" s="35" customFormat="1">
       <c r="A20" s="36"/>
       <c r="B20" s="15" t="s">
         <v>28</v>
@@ -2845,7 +2849,7 @@
       <c r="Q20" s="31"/>
       <c r="R20" s="31"/>
     </row>
-    <row r="21" spans="1:18" s="35" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" s="35" customFormat="1" ht="12.6" thickBot="1">
       <c r="A21" s="36"/>
       <c r="B21" s="15" t="s">
         <v>28</v>
@@ -2875,7 +2879,7 @@
       <c r="Q21" s="31"/>
       <c r="R21" s="31"/>
     </row>
-    <row r="22" spans="1:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="12.6" thickBot="1">
       <c r="B22" s="8"/>
       <c r="C22" s="26" t="s">
         <v>30</v>
@@ -2884,7 +2888,7 @@
       <c r="E22" s="11"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="16.2" thickBot="1">
       <c r="B23" s="27" t="s">
         <v>17</v>
       </c>
@@ -2905,7 +2909,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="35" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" s="35" customFormat="1" ht="16.2" thickBot="1">
       <c r="A24" s="36" t="s">
         <v>29</v>
       </c>
@@ -2943,7 +2947,7 @@
       <c r="Q24" s="31"/>
       <c r="R24" s="31"/>
     </row>
-    <row r="25" spans="1:18" s="35" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="35" customFormat="1" ht="16.2" thickBot="1">
       <c r="A25" s="36"/>
       <c r="B25" s="15" t="s">
         <v>76</v>
@@ -2979,7 +2983,7 @@
       <c r="Q25" s="31"/>
       <c r="R25" s="31"/>
     </row>
-    <row r="26" spans="1:18" s="35" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" s="35" customFormat="1" ht="16.2" thickBot="1">
       <c r="A26" s="36"/>
       <c r="B26" s="15" t="s">
         <v>76</v>
@@ -3015,7 +3019,7 @@
       <c r="Q26" s="31"/>
       <c r="R26" s="31"/>
     </row>
-    <row r="27" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="35" customFormat="1">
       <c r="B27" s="24" t="s">
         <v>78</v>
       </c>
@@ -3042,7 +3046,7 @@
       <c r="Q27" s="31"/>
       <c r="R27" s="31"/>
     </row>
-    <row r="28" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" s="35" customFormat="1">
       <c r="B28" s="24" t="s">
         <v>78</v>
       </c>
@@ -3069,7 +3073,7 @@
       <c r="Q28" s="31"/>
       <c r="R28" s="31"/>
     </row>
-    <row r="29" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" s="35" customFormat="1">
       <c r="B29" s="24" t="s">
         <v>77</v>
       </c>
@@ -3096,7 +3100,7 @@
       <c r="Q29" s="31"/>
       <c r="R29" s="31"/>
     </row>
-    <row r="30" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" s="35" customFormat="1">
       <c r="B30" s="24" t="s">
         <v>77</v>
       </c>
@@ -3123,7 +3127,7 @@
       <c r="Q30" s="31"/>
       <c r="R30" s="31"/>
     </row>
-    <row r="31" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" s="35" customFormat="1">
       <c r="B31" s="24" t="s">
         <v>79</v>
       </c>
@@ -3150,7 +3154,7 @@
       <c r="Q31" s="31"/>
       <c r="R31" s="31"/>
     </row>
-    <row r="32" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:18" s="35" customFormat="1">
       <c r="B32" s="24" t="s">
         <v>79</v>
       </c>
@@ -3177,7 +3181,7 @@
       <c r="Q32" s="31"/>
       <c r="R32" s="31"/>
     </row>
-    <row r="33" spans="2:18" s="35" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:18" s="35" customFormat="1">
       <c r="B33" s="24" t="s">
         <v>80</v>
       </c>
@@ -3204,7 +3208,7 @@
       <c r="Q33" s="31"/>
       <c r="R33" s="31"/>
     </row>
-    <row r="34" spans="2:18" s="35" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:18" s="35" customFormat="1" ht="12.6" thickBot="1">
       <c r="B34" s="24" t="s">
         <v>80</v>
       </c>
@@ -3231,7 +3235,7 @@
       <c r="Q34" s="31"/>
       <c r="R34" s="31"/>
     </row>
-    <row r="35" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:18" ht="24.6" thickBot="1">
       <c r="B35" s="63">
         <v>5</v>
       </c>
@@ -3248,7 +3252,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:18" ht="24.6" thickBot="1">
       <c r="B36" s="63">
         <v>5</v>
       </c>
@@ -3265,7 +3269,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:18" ht="24.6" thickBot="1">
       <c r="B37" s="63">
         <v>6</v>
       </c>
@@ -3282,8 +3286,8 @@
         <v>209</v>
       </c>
     </row>
-    <row r="38" spans="2:18" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:18" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:18" ht="12.6" thickBot="1"/>
+    <row r="39" spans="2:18" ht="12.6" thickBot="1">
       <c r="B39" s="8" t="s">
         <v>16</v>
       </c>
@@ -3294,7 +3298,7 @@
       <c r="E39" s="11"/>
       <c r="F39" s="12"/>
     </row>
-    <row r="40" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" ht="16.2" thickBot="1">
       <c r="B40" s="15" t="s">
         <v>28</v>
       </c>
@@ -3321,7 +3325,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="2:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:18" ht="15.6">
       <c r="B41" s="15" t="s">
         <v>28</v>
       </c>
@@ -3348,7 +3352,7 @@
         <v>1.4659700967420086E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:18" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:18" ht="25.2" thickBot="1">
       <c r="B42" s="15" t="s">
         <v>28</v>
       </c>
@@ -3377,7 +3381,7 @@
         <v>3.7820644719985808E-3</v>
       </c>
     </row>
-    <row r="43" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:18" ht="12.6" thickBot="1">
       <c r="B43" s="8"/>
       <c r="C43" s="26" t="s">
         <v>30</v>
@@ -3386,7 +3390,7 @@
       <c r="E43" s="11"/>
       <c r="F43" s="12"/>
     </row>
-    <row r="44" spans="2:18" ht="13" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:18" ht="12.6" thickBot="1">
       <c r="B44" s="63">
         <v>4</v>
       </c>
@@ -3399,7 +3403,7 @@
       </c>
       <c r="F44" s="28"/>
     </row>
-    <row r="45" spans="2:18" ht="27" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:18" ht="24.6" thickBot="1">
       <c r="B45" s="63" t="s">
         <v>203</v>
       </c>
@@ -3416,7 +3420,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:18" ht="12.6" thickBot="1">
       <c r="B46" s="63" t="s">
         <v>204</v>
       </c>
@@ -3433,7 +3437,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:18" ht="12.6" thickBot="1">
       <c r="B47" s="63">
         <v>6</v>
       </c>
@@ -3454,7 +3458,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:18" ht="14.4">
       <c r="C48" s="39"/>
       <c r="H48" s="31" t="s">
         <v>36</v>
@@ -3472,7 +3476,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="8:12" x14ac:dyDescent="0.15">
+    <row r="49" spans="8:12">
       <c r="H49" s="31" t="s">
         <v>172</v>
       </c>
@@ -3489,7 +3493,7 @@
         <v>3.1157979999996144E-4</v>
       </c>
     </row>
-    <row r="50" spans="8:12" x14ac:dyDescent="0.15">
+    <row r="50" spans="8:12">
       <c r="H50" s="31" t="s">
         <v>173</v>
       </c>
@@ -3506,7 +3510,7 @@
         <v>7.5669383000054324E-4</v>
       </c>
     </row>
-    <row r="51" spans="8:12" x14ac:dyDescent="0.15">
+    <row r="51" spans="8:12">
       <c r="H51" s="31" t="s">
         <v>174</v>
       </c>
@@ -3523,7 +3527,7 @@
         <v>3.5609100000044691E-4</v>
       </c>
     </row>
-    <row r="52" spans="8:12" x14ac:dyDescent="0.15">
+    <row r="52" spans="8:12">
       <c r="H52" s="31" t="s">
         <v>175</v>
       </c>
@@ -3540,7 +3544,7 @@
         <v>4.0060199999913948E-4</v>
       </c>
     </row>
-    <row r="53" spans="8:12" x14ac:dyDescent="0.15">
+    <row r="53" spans="8:12">
       <c r="H53" s="31" t="s">
         <v>176</v>
       </c>
@@ -3563,23 +3567,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F597CC-23D9-EB45-AE40-EDEB80C3B1B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O53"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="6" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>95</v>
       </c>
@@ -3587,7 +3591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>82</v>
       </c>
@@ -3595,7 +3599,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>83</v>
       </c>
@@ -3603,8 +3607,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" ht="16.2" thickBot="1"/>
+    <row r="8" spans="2:9">
       <c r="B8" s="72" t="s">
         <v>86</v>
       </c>
@@ -3618,7 +3622,7 @@
       <c r="H8" s="73"/>
       <c r="I8" s="74"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9">
       <c r="B9" s="76" t="s">
         <v>28</v>
       </c>
@@ -3632,7 +3636,7 @@
       <c r="H9" s="75"/>
       <c r="I9" s="77"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9">
       <c r="B10" s="76"/>
       <c r="C10" s="75" t="s">
         <v>112</v>
@@ -3644,7 +3648,7 @@
       <c r="H10" s="75"/>
       <c r="I10" s="77"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9">
       <c r="B11" s="76"/>
       <c r="C11" s="75" t="s">
         <v>113</v>
@@ -3656,7 +3660,7 @@
       <c r="H11" s="75"/>
       <c r="I11" s="77"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9">
       <c r="B12" s="76"/>
       <c r="C12" s="75"/>
       <c r="D12" s="75"/>
@@ -3666,7 +3670,7 @@
       <c r="H12" s="75"/>
       <c r="I12" s="77"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9">
       <c r="B13" s="76"/>
       <c r="C13" s="75"/>
       <c r="D13" s="75"/>
@@ -3676,7 +3680,7 @@
       <c r="H13" s="75"/>
       <c r="I13" s="77"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9">
       <c r="B14" s="76"/>
       <c r="C14" s="75"/>
       <c r="D14" s="75"/>
@@ -3686,7 +3690,7 @@
       <c r="H14" s="75"/>
       <c r="I14" s="77"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9">
       <c r="B15" s="76"/>
       <c r="C15" s="75"/>
       <c r="D15" s="75"/>
@@ -3696,7 +3700,7 @@
       <c r="H15" s="75"/>
       <c r="I15" s="77"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9">
       <c r="B16" s="76"/>
       <c r="C16" s="75"/>
       <c r="D16" s="75"/>
@@ -3706,7 +3710,7 @@
       <c r="H16" s="75"/>
       <c r="I16" s="77"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15">
       <c r="B17" s="76"/>
       <c r="C17" s="75"/>
       <c r="D17" s="75"/>
@@ -3716,7 +3720,7 @@
       <c r="H17" s="75"/>
       <c r="I17" s="77"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15">
       <c r="B18" s="76"/>
       <c r="C18" s="75"/>
       <c r="D18" s="75"/>
@@ -3726,7 +3730,7 @@
       <c r="H18" s="75"/>
       <c r="I18" s="77"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15">
       <c r="B19" s="76"/>
       <c r="C19" s="75"/>
       <c r="D19" s="75"/>
@@ -3736,7 +3740,7 @@
       <c r="H19" s="75"/>
       <c r="I19" s="77"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15">
       <c r="B20" s="76"/>
       <c r="C20" s="75"/>
       <c r="D20" s="75"/>
@@ -3746,7 +3750,7 @@
       <c r="H20" s="75"/>
       <c r="I20" s="77"/>
     </row>
-    <row r="21" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" ht="16.2" thickBot="1">
       <c r="B21" s="78"/>
       <c r="C21" s="79"/>
       <c r="D21" s="79"/>
@@ -3756,7 +3760,7 @@
       <c r="H21" s="79"/>
       <c r="I21" s="80"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15">
       <c r="M23">
         <f>E29*J24</f>
         <v>12343.166935914553</v>
@@ -3766,7 +3770,7 @@
         <v>296236.00646194926</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15">
       <c r="H24">
         <v>44.94</v>
       </c>
@@ -3782,7 +3786,7 @@
         <v>296236.00646194926</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15">
       <c r="B26" t="s">
         <v>70</v>
       </c>
@@ -3796,7 +3800,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15">
       <c r="D28" t="s">
         <v>121</v>
       </c>
@@ -3808,7 +3812,7 @@
         <v>8.1016485087820469E-5</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15">
       <c r="B29" t="s">
         <v>104</v>
       </c>
@@ -3823,7 +3827,7 @@
         <v>8.0762987324370288E-5</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15">
       <c r="B30" t="s">
         <v>105</v>
       </c>
@@ -3834,7 +3838,7 @@
         <v>1.0013351134846462</v>
       </c>
     </row>
-    <row r="32" spans="2:15" s="87" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" s="87" customFormat="1">
       <c r="B32" s="87" t="s">
         <v>106</v>
       </c>
@@ -3854,7 +3858,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14">
       <c r="B33">
         <v>-10</v>
       </c>
@@ -3871,7 +3875,7 @@
         <v>-123431.66935914553</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14">
       <c r="B34">
         <v>-5</v>
       </c>
@@ -3891,7 +3895,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>107</v>
       </c>
@@ -3919,7 +3923,7 @@
         <v>1.7444805262063983</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14">
       <c r="B36">
         <v>5</v>
       </c>
@@ -3936,7 +3940,7 @@
         <v>61715.834679572763</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14">
       <c r="B37">
         <v>10</v>
       </c>
@@ -3953,7 +3957,7 @@
         <v>123431.66935914553</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14">
       <c r="B38">
         <v>15</v>
       </c>
@@ -3970,7 +3974,7 @@
         <v>185147.5040387183</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14">
       <c r="B39">
         <v>20</v>
       </c>
@@ -3987,7 +3991,7 @@
         <v>246863.33871829105</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14">
       <c r="B40">
         <v>25</v>
       </c>
@@ -4004,7 +4008,7 @@
         <v>308579.17339786387</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14">
       <c r="B41">
         <v>30</v>
       </c>
@@ -4024,7 +4028,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14">
       <c r="B42">
         <v>35</v>
       </c>
@@ -4051,7 +4055,7 @@
         <v>11183</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14">
       <c r="B43">
         <v>40</v>
       </c>
@@ -4074,7 +4078,7 @@
         <v>62000</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14">
       <c r="B44">
         <v>45</v>
       </c>
@@ -4102,7 +4106,7 @@
         <v>73183</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14">
       <c r="B45">
         <v>48.5</v>
       </c>
@@ -4119,7 +4123,7 @@
         <v>598643.59639185574</v>
       </c>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:8">
       <c r="C52" t="s">
         <v>125</v>
       </c>
@@ -4131,7 +4135,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:8">
       <c r="H53">
         <f>5/443000</f>
         <v>1.128668171557562E-5</v>
@@ -4144,30 +4148,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856B0310-C035-6C4C-A5AB-B339976BEC09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U60"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="K29" sqref="K29:O35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.296875" customWidth="1"/>
     <col min="12" max="12" width="20.5" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.796875" customWidth="1"/>
+    <col min="15" max="15" width="17.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21">
       <c r="B2" t="s">
         <v>95</v>
       </c>
@@ -4175,7 +4179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21">
       <c r="B3" t="s">
         <v>82</v>
       </c>
@@ -4183,12 +4187,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:21">
       <c r="D4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:21">
       <c r="B5" t="s">
         <v>83</v>
       </c>
@@ -4196,8 +4200,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:21" ht="16.2" thickBot="1"/>
+    <row r="10" spans="2:21">
       <c r="B10" s="67" t="s">
         <v>81</v>
       </c>
@@ -4224,7 +4228,7 @@
       <c r="T10" s="73"/>
       <c r="U10" s="74"/>
     </row>
-    <row r="11" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" ht="16.2" thickBot="1">
       <c r="B11" s="69" t="s">
         <v>75</v>
       </c>
@@ -4251,7 +4255,7 @@
       <c r="T11" s="75"/>
       <c r="U11" s="77"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:21">
       <c r="B12" s="70"/>
       <c r="N12" s="76"/>
       <c r="O12" s="75"/>
@@ -4262,7 +4266,7 @@
       <c r="T12" s="75"/>
       <c r="U12" s="77"/>
     </row>
-    <row r="13" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" ht="16.2" thickBot="1">
       <c r="B13" s="71"/>
       <c r="N13" s="76"/>
       <c r="O13" s="75"/>
@@ -4273,7 +4277,7 @@
       <c r="T13" s="75"/>
       <c r="U13" s="77"/>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:21">
       <c r="B14" s="67"/>
       <c r="C14" s="181" t="s">
         <v>153</v>
@@ -4293,7 +4297,7 @@
       <c r="R14" s="75"/>
       <c r="S14" s="77"/>
     </row>
-    <row r="15" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" ht="16.2" thickBot="1">
       <c r="B15" s="68" t="s">
         <v>76</v>
       </c>
@@ -4321,7 +4325,7 @@
       <c r="R15" s="75"/>
       <c r="S15" s="77"/>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:21">
       <c r="B16" s="68"/>
       <c r="C16" s="94">
         <v>1</v>
@@ -4349,7 +4353,7 @@
       <c r="R16" s="75"/>
       <c r="S16" s="77"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:19">
       <c r="B17" s="68"/>
       <c r="C17" s="202">
         <v>2</v>
@@ -4371,7 +4375,7 @@
       <c r="R17" s="75"/>
       <c r="S17" s="77"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:19">
       <c r="B18" s="68"/>
       <c r="C18" s="202">
         <v>3</v>
@@ -4393,7 +4397,7 @@
       <c r="R18" s="75"/>
       <c r="S18" s="77"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:19">
       <c r="B19" s="68"/>
       <c r="C19" s="202">
         <v>4</v>
@@ -4415,7 +4419,7 @@
       <c r="R19" s="75"/>
       <c r="S19" s="77"/>
     </row>
-    <row r="20" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" ht="16.2" thickBot="1">
       <c r="B20" s="69"/>
       <c r="C20" s="48">
         <v>5</v>
@@ -4437,7 +4441,7 @@
       <c r="R20" s="75"/>
       <c r="S20" s="77"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:19">
       <c r="B21" s="70"/>
       <c r="C21" s="203"/>
       <c r="D21" s="99"/>
@@ -4453,7 +4457,7 @@
       <c r="R21" s="75"/>
       <c r="S21" s="77"/>
     </row>
-    <row r="22" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" ht="16.2" thickBot="1">
       <c r="B22" s="71"/>
       <c r="C22" s="203"/>
       <c r="D22" s="99"/>
@@ -4469,7 +4473,7 @@
       <c r="R22" s="75"/>
       <c r="S22" s="77"/>
     </row>
-    <row r="23" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" ht="16.2" thickBot="1">
       <c r="B23" s="67"/>
       <c r="C23" s="181" t="s">
         <v>154</v>
@@ -4489,7 +4493,7 @@
       <c r="R23" s="79"/>
       <c r="S23" s="80"/>
     </row>
-    <row r="24" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" ht="16.2" thickBot="1">
       <c r="B24" s="68" t="s">
         <v>78</v>
       </c>
@@ -4509,7 +4513,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:19">
       <c r="B25" s="68"/>
       <c r="C25" s="94">
         <v>1</v>
@@ -4529,7 +4533,7 @@
         <v>7.5669383000054324E-4</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:19">
       <c r="B26" s="68"/>
       <c r="C26" s="202">
         <v>2</v>
@@ -4543,7 +4547,7 @@
       <c r="F26" s="99"/>
       <c r="G26" s="201"/>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:19">
       <c r="B27" s="68"/>
       <c r="C27" s="202">
         <v>3</v>
@@ -4557,7 +4561,7 @@
       <c r="F27" s="99"/>
       <c r="G27" s="201"/>
     </row>
-    <row r="28" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" ht="16.2" thickBot="1">
       <c r="B28" s="68"/>
       <c r="C28" s="202">
         <v>4</v>
@@ -4571,7 +4575,7 @@
       <c r="F28" s="99"/>
       <c r="G28" s="201"/>
     </row>
-    <row r="29" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" ht="16.2" thickBot="1">
       <c r="B29" s="69"/>
       <c r="C29" s="48">
         <v>5</v>
@@ -4594,7 +4598,7 @@
       </c>
       <c r="O29" s="220"/>
     </row>
-    <row r="30" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" ht="16.2" thickBot="1">
       <c r="B30" s="70"/>
       <c r="C30" s="203"/>
       <c r="D30" s="99"/>
@@ -4617,7 +4621,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" ht="16.2" thickBot="1">
       <c r="B31" s="71"/>
       <c r="C31" s="203"/>
       <c r="D31" s="99"/>
@@ -4644,7 +4648,7 @@
         <v>3.1157979999996144E-4</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:19">
       <c r="B32" s="67"/>
       <c r="C32" s="181" t="s">
         <v>155</v>
@@ -4675,7 +4679,7 @@
         <v>7.5669383000054324E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" ht="16.2" thickBot="1">
       <c r="B33" s="68" t="s">
         <v>77</v>
       </c>
@@ -4714,7 +4718,7 @@
         <v>3.5609100000044691E-4</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:15">
       <c r="B34" s="68"/>
       <c r="C34" s="94">
         <v>1</v>
@@ -4753,7 +4757,7 @@
         <v>4.0060199999913948E-4</v>
       </c>
     </row>
-    <row r="35" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" ht="16.2" thickBot="1">
       <c r="B35" s="68"/>
       <c r="C35" s="202">
         <v>2</v>
@@ -4786,7 +4790,7 @@
         <v>3.5609000000391688E-4</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:15">
       <c r="B36" s="68"/>
       <c r="C36" s="202">
         <v>3</v>
@@ -4800,7 +4804,7 @@
       <c r="F36" s="99"/>
       <c r="G36" s="201"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:15">
       <c r="B37" s="68"/>
       <c r="C37" s="202">
         <v>4</v>
@@ -4814,7 +4818,7 @@
       <c r="F37" s="99"/>
       <c r="G37" s="201"/>
     </row>
-    <row r="38" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" ht="16.2" thickBot="1">
       <c r="B38" s="69"/>
       <c r="C38" s="48">
         <v>5</v>
@@ -4828,7 +4832,7 @@
       <c r="F38" s="99"/>
       <c r="G38" s="201"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:15">
       <c r="B39" s="70"/>
       <c r="C39" s="203"/>
       <c r="D39" s="99"/>
@@ -4836,7 +4840,7 @@
       <c r="F39" s="99"/>
       <c r="G39" s="201"/>
     </row>
-    <row r="40" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" ht="16.2" thickBot="1">
       <c r="B40" s="71"/>
       <c r="C40" s="203"/>
       <c r="D40" s="99"/>
@@ -4844,7 +4848,7 @@
       <c r="F40" s="99"/>
       <c r="G40" s="201"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:15">
       <c r="B41" s="67"/>
       <c r="C41" s="181" t="s">
         <v>156</v>
@@ -4856,7 +4860,7 @@
       <c r="F41" s="99"/>
       <c r="G41" s="201"/>
     </row>
-    <row r="42" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" ht="16.2" thickBot="1">
       <c r="B42" s="68" t="s">
         <v>79</v>
       </c>
@@ -4876,7 +4880,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:15">
       <c r="B43" s="68"/>
       <c r="C43" s="94">
         <v>1</v>
@@ -4896,7 +4900,7 @@
         <v>4.0060199999913948E-4</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:15">
       <c r="B44" s="68"/>
       <c r="C44" s="202">
         <v>2</v>
@@ -4910,7 +4914,7 @@
       <c r="F44" s="99"/>
       <c r="G44" s="201"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:15">
       <c r="B45" s="68"/>
       <c r="C45" s="202">
         <v>3</v>
@@ -4924,7 +4928,7 @@
       <c r="F45" s="99"/>
       <c r="G45" s="201"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:15">
       <c r="B46" s="68"/>
       <c r="C46" s="202">
         <v>4</v>
@@ -4938,7 +4942,7 @@
       <c r="F46" s="99"/>
       <c r="G46" s="201"/>
     </row>
-    <row r="47" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" ht="16.2" thickBot="1">
       <c r="B47" s="69"/>
       <c r="C47" s="48">
         <v>5</v>
@@ -4952,7 +4956,7 @@
       <c r="F47" s="99"/>
       <c r="G47" s="201"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:15">
       <c r="B48" s="70"/>
       <c r="C48" s="203"/>
       <c r="D48" s="99"/>
@@ -4960,7 +4964,7 @@
       <c r="F48" s="99"/>
       <c r="G48" s="201"/>
     </row>
-    <row r="49" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" ht="16.2" thickBot="1">
       <c r="B49" s="71"/>
       <c r="C49" s="203"/>
       <c r="D49" s="99"/>
@@ -4968,7 +4972,7 @@
       <c r="F49" s="99"/>
       <c r="G49" s="201"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7">
       <c r="B50" s="67"/>
       <c r="C50" s="181" t="s">
         <v>36</v>
@@ -4980,7 +4984,7 @@
       <c r="F50" s="99"/>
       <c r="G50" s="201"/>
     </row>
-    <row r="51" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" ht="16.2" thickBot="1">
       <c r="B51" s="68" t="s">
         <v>80</v>
       </c>
@@ -5000,7 +5004,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:7">
       <c r="B52" s="68"/>
       <c r="C52" s="94">
         <v>1</v>
@@ -5020,7 +5024,7 @@
         <v>3.5609000000391688E-4</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:7">
       <c r="B53" s="68"/>
       <c r="C53" s="202">
         <v>2</v>
@@ -5034,7 +5038,7 @@
       <c r="F53" s="99"/>
       <c r="G53" s="201"/>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:7">
       <c r="B54" s="68"/>
       <c r="C54" s="202">
         <v>3</v>
@@ -5048,7 +5052,7 @@
       <c r="F54" s="99"/>
       <c r="G54" s="201"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:7">
       <c r="B55" s="68"/>
       <c r="C55" s="202">
         <v>4</v>
@@ -5062,7 +5066,7 @@
       <c r="F55" s="99"/>
       <c r="G55" s="201"/>
     </row>
-    <row r="56" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" ht="16.2" thickBot="1">
       <c r="B56" s="69"/>
       <c r="C56" s="48">
         <v>5</v>
@@ -5076,13 +5080,13 @@
       <c r="F56" s="204"/>
       <c r="G56" s="205"/>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:7">
       <c r="B57" s="70"/>
     </row>
-    <row r="58" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" ht="16.2" thickBot="1">
       <c r="B58" s="71"/>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:7">
       <c r="B59" s="67"/>
       <c r="C59" s="65"/>
       <c r="D59" s="46" t="s">
@@ -5095,7 +5099,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" ht="16.2" thickBot="1">
       <c r="B60" s="69" t="s">
         <v>75</v>
       </c>
@@ -5112,16 +5116,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD3A049-3F74-2A47-9E3D-D1B8F2C53856}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9">
       <c r="B2" s="86" t="s">
         <v>95</v>
       </c>
@@ -5130,7 +5134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>82</v>
       </c>
@@ -5138,18 +5142,18 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9">
       <c r="D4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9">
       <c r="D5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" ht="16.2" thickBot="1"/>
+    <row r="8" spans="2:9">
       <c r="B8" s="72" t="s">
         <v>86</v>
       </c>
@@ -5163,7 +5167,7 @@
       <c r="H8" s="73"/>
       <c r="I8" s="74"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9">
       <c r="B9" s="76">
         <v>4</v>
       </c>
@@ -5175,7 +5179,7 @@
       <c r="H9" s="75"/>
       <c r="I9" s="77"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9">
       <c r="B10" s="76"/>
       <c r="C10" s="75"/>
       <c r="D10" s="75"/>
@@ -5185,7 +5189,7 @@
       <c r="H10" s="75"/>
       <c r="I10" s="77"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9">
       <c r="B11" s="76"/>
       <c r="C11" s="75"/>
       <c r="D11" s="75"/>
@@ -5195,7 +5199,7 @@
       <c r="H11" s="75"/>
       <c r="I11" s="77"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9">
       <c r="B12" s="76"/>
       <c r="C12" s="75"/>
       <c r="D12" s="75"/>
@@ -5205,7 +5209,7 @@
       <c r="H12" s="75"/>
       <c r="I12" s="77"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9">
       <c r="B13" s="76"/>
       <c r="C13" s="75"/>
       <c r="D13" s="75"/>
@@ -5215,7 +5219,7 @@
       <c r="H13" s="75"/>
       <c r="I13" s="77"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9">
       <c r="B14" s="76"/>
       <c r="C14" s="75"/>
       <c r="D14" s="75"/>
@@ -5225,7 +5229,7 @@
       <c r="H14" s="75"/>
       <c r="I14" s="77"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9">
       <c r="B15" s="76"/>
       <c r="C15" s="75"/>
       <c r="D15" s="75"/>
@@ -5235,7 +5239,7 @@
       <c r="H15" s="75"/>
       <c r="I15" s="77"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9">
       <c r="B16" s="76"/>
       <c r="C16" s="75"/>
       <c r="D16" s="75"/>
@@ -5245,7 +5249,7 @@
       <c r="H16" s="75"/>
       <c r="I16" s="77"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9">
       <c r="B17" s="76"/>
       <c r="C17" s="75"/>
       <c r="D17" s="75"/>
@@ -5255,7 +5259,7 @@
       <c r="H17" s="75"/>
       <c r="I17" s="77"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9">
       <c r="B18" s="76"/>
       <c r="C18" s="75"/>
       <c r="D18" s="75"/>
@@ -5265,7 +5269,7 @@
       <c r="H18" s="75"/>
       <c r="I18" s="77"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9">
       <c r="B19" s="76"/>
       <c r="C19" s="75"/>
       <c r="D19" s="75"/>
@@ -5275,7 +5279,7 @@
       <c r="H19" s="75"/>
       <c r="I19" s="77"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9">
       <c r="B20" s="76"/>
       <c r="C20" s="75"/>
       <c r="D20" s="75"/>
@@ -5285,7 +5289,7 @@
       <c r="H20" s="75"/>
       <c r="I20" s="77"/>
     </row>
-    <row r="21" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="16.2" thickBot="1">
       <c r="B21" s="78"/>
       <c r="C21" s="79"/>
       <c r="D21" s="79"/>
@@ -5301,28 +5305,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CEB521-8DC8-0C48-A601-3238D1EFF0A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z125"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10:O10"/>
+    <sheetView topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13.69921875" customWidth="1"/>
+    <col min="12" max="12" width="13.296875" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.796875" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:26">
       <c r="B2" t="s">
         <v>95</v>
       </c>
@@ -5330,7 +5334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:26">
       <c r="B3" t="s">
         <v>82</v>
       </c>
@@ -5341,13 +5345,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="2:26" s="113" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:26" s="113" customFormat="1">
       <c r="E5" s="117" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:26" ht="16.2" thickBot="1"/>
+    <row r="7" spans="2:26" ht="16.2" thickBot="1">
       <c r="B7" t="s">
         <v>108</v>
       </c>
@@ -5391,7 +5395,7 @@
       <c r="Y7" s="73"/>
       <c r="Z7" s="74"/>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:26">
       <c r="C8" s="95" t="s">
         <v>127</v>
       </c>
@@ -5430,7 +5434,7 @@
       <c r="Y8" s="92"/>
       <c r="Z8" s="93"/>
     </row>
-    <row r="9" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:26" ht="16.2" thickBot="1">
       <c r="C9" s="94">
         <v>-5</v>
       </c>
@@ -5471,7 +5475,7 @@
       <c r="Y9" s="75"/>
       <c r="Z9" s="77"/>
     </row>
-    <row r="10" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:26" ht="16.2" thickBot="1">
       <c r="C10" s="68">
         <v>0</v>
       </c>
@@ -5516,7 +5520,7 @@
       <c r="Y10" s="75"/>
       <c r="Z10" s="77"/>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:26">
       <c r="C11" s="68">
         <v>5</v>
       </c>
@@ -5564,7 +5568,7 @@
       <c r="Y11" s="75"/>
       <c r="Z11" s="77"/>
     </row>
-    <row r="12" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:26" ht="16.2" thickBot="1">
       <c r="C12" s="68">
         <v>10</v>
       </c>
@@ -5612,7 +5616,7 @@
       <c r="Y12" s="75"/>
       <c r="Z12" s="77"/>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:26">
       <c r="C13" s="68">
         <v>15</v>
       </c>
@@ -5651,7 +5655,7 @@
       <c r="Y13" s="75"/>
       <c r="Z13" s="77"/>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:26">
       <c r="C14" s="68">
         <v>20</v>
       </c>
@@ -5690,7 +5694,7 @@
       <c r="Y14" s="75"/>
       <c r="Z14" s="77"/>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:26">
       <c r="C15" s="68">
         <v>25</v>
       </c>
@@ -5729,7 +5733,7 @@
       <c r="Y15" s="75"/>
       <c r="Z15" s="77"/>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:26">
       <c r="C16" s="68">
         <v>30</v>
       </c>
@@ -5752,7 +5756,10 @@
       </c>
       <c r="I16" s="98"/>
       <c r="J16" s="98"/>
-      <c r="K16" s="99"/>
+      <c r="K16" s="252">
+        <f>AVERAGE(F12,F14,F16,F18)</f>
+        <v>4.7285708864759357E-3</v>
+      </c>
       <c r="L16" s="99"/>
       <c r="M16" s="99"/>
       <c r="N16" s="99"/>
@@ -5768,7 +5775,7 @@
       <c r="Y16" s="75"/>
       <c r="Z16" s="77"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26">
       <c r="C17" s="68">
         <v>35</v>
       </c>
@@ -5791,7 +5798,10 @@
       </c>
       <c r="I17" s="98"/>
       <c r="J17" s="98"/>
-      <c r="K17" s="99"/>
+      <c r="K17" s="252">
+        <f>AVERAGE(H12,H14,H16,H18)</f>
+        <v>4.6587321742004306E-3</v>
+      </c>
       <c r="L17" s="99"/>
       <c r="M17" s="99"/>
       <c r="N17" s="99"/>
@@ -5807,7 +5817,7 @@
       <c r="Y17" s="75"/>
       <c r="Z17" s="77"/>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:26">
       <c r="C18" s="71">
         <v>40</v>
       </c>
@@ -5845,7 +5855,7 @@
       <c r="Y18" s="75"/>
       <c r="Z18" s="77"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:26">
       <c r="C19" s="71">
         <v>45</v>
       </c>
@@ -5884,7 +5894,7 @@
       <c r="Y19" s="75"/>
       <c r="Z19" s="77"/>
     </row>
-    <row r="20" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" ht="16.2" thickBot="1">
       <c r="C20" s="69" t="s">
         <v>128</v>
       </c>
@@ -5913,7 +5923,7 @@
       <c r="Y20" s="75"/>
       <c r="Z20" s="77"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26">
       <c r="R21" s="76"/>
       <c r="S21" s="75" t="s">
         <v>131</v>
@@ -5925,7 +5935,7 @@
       <c r="X21" s="75"/>
       <c r="Y21" s="77"/>
     </row>
-    <row r="22" spans="2:26" s="113" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:26" s="113" customFormat="1">
       <c r="B22" s="117"/>
       <c r="D22" s="117"/>
       <c r="E22" s="117" t="s">
@@ -5940,7 +5950,7 @@
       <c r="X22" s="115"/>
       <c r="Y22" s="116"/>
     </row>
-    <row r="23" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26" ht="16.2" thickBot="1">
       <c r="R23" s="78"/>
       <c r="S23" s="79"/>
       <c r="T23" s="79"/>
@@ -5950,12 +5960,12 @@
       <c r="X23" s="79"/>
       <c r="Y23" s="80"/>
     </row>
-    <row r="24" spans="2:26" s="118" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26" s="118" customFormat="1" ht="16.2" thickBot="1">
       <c r="C24" s="118" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="2:26" s="118" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26" s="118" customFormat="1" ht="16.2" thickBot="1">
       <c r="C25" s="119" t="s">
         <v>52</v>
       </c>
@@ -5982,7 +5992,7 @@
       <c r="P25" s="126"/>
       <c r="Q25" s="127"/>
     </row>
-    <row r="26" spans="2:26" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:26" s="118" customFormat="1">
       <c r="C26" s="128" t="s">
         <v>127</v>
       </c>
@@ -6021,7 +6031,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="2:26" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:26" s="118" customFormat="1">
       <c r="C27" s="136">
         <v>-5</v>
       </c>
@@ -6072,7 +6082,7 @@
         <v>2.8048311745862975E-3</v>
       </c>
     </row>
-    <row r="28" spans="2:26" s="118" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:26" s="118" customFormat="1" ht="46.8">
       <c r="C28" s="142">
         <v>0</v>
       </c>
@@ -6116,7 +6126,7 @@
       </c>
       <c r="Q28" s="141"/>
     </row>
-    <row r="29" spans="2:26" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:26" s="118" customFormat="1">
       <c r="C29" s="142">
         <v>5</v>
       </c>
@@ -6167,7 +6177,7 @@
         <v>8.0006476763472278E-4</v>
       </c>
     </row>
-    <row r="30" spans="2:26" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:26" s="118" customFormat="1">
       <c r="C30" s="142">
         <v>10</v>
       </c>
@@ -6218,7 +6228,7 @@
         <v>-1.7062970232828434E-4</v>
       </c>
     </row>
-    <row r="31" spans="2:26" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:26" s="118" customFormat="1">
       <c r="C31" s="142">
         <v>15</v>
       </c>
@@ -6236,7 +6246,7 @@
       <c r="P31" s="140"/>
       <c r="Q31" s="141"/>
     </row>
-    <row r="32" spans="2:26" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:26" s="118" customFormat="1">
       <c r="C32" s="142">
         <v>20</v>
       </c>
@@ -6254,7 +6264,7 @@
       <c r="P32" s="140"/>
       <c r="Q32" s="141"/>
     </row>
-    <row r="33" spans="3:17" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:17" s="118" customFormat="1">
       <c r="C33" s="142">
         <v>25</v>
       </c>
@@ -6272,7 +6282,7 @@
       <c r="P33" s="140"/>
       <c r="Q33" s="141"/>
     </row>
-    <row r="34" spans="3:17" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:17" s="118" customFormat="1">
       <c r="C34" s="142">
         <v>30</v>
       </c>
@@ -6290,7 +6300,7 @@
       <c r="P34" s="140"/>
       <c r="Q34" s="141"/>
     </row>
-    <row r="35" spans="3:17" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:17" s="118" customFormat="1">
       <c r="C35" s="142">
         <v>35</v>
       </c>
@@ -6341,7 +6351,7 @@
         <v>1.0036414201515242E-2</v>
       </c>
     </row>
-    <row r="36" spans="3:17" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:17" s="118" customFormat="1">
       <c r="C36" s="147">
         <v>40</v>
       </c>
@@ -6359,7 +6369,7 @@
       <c r="P36" s="140"/>
       <c r="Q36" s="141"/>
     </row>
-    <row r="37" spans="3:17" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:17" s="118" customFormat="1">
       <c r="C37" s="147">
         <v>45</v>
       </c>
@@ -6410,7 +6420,7 @@
         <v>5.8317037835706742E-3</v>
       </c>
     </row>
-    <row r="38" spans="3:17" s="118" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:17" s="118" customFormat="1" ht="16.2" thickBot="1">
       <c r="C38" s="149" t="s">
         <v>128</v>
       </c>
@@ -6428,7 +6438,7 @@
       <c r="P38" s="140"/>
       <c r="Q38" s="141"/>
     </row>
-    <row r="39" spans="3:17" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:17" s="118" customFormat="1">
       <c r="F39" s="139"/>
       <c r="G39" s="140" t="s">
         <v>140</v>
@@ -6451,7 +6461,7 @@
       <c r="P39" s="140"/>
       <c r="Q39" s="141"/>
     </row>
-    <row r="40" spans="3:17" s="118" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:17" s="118" customFormat="1" ht="16.2" thickBot="1">
       <c r="F40" s="151"/>
       <c r="G40" s="152" t="s">
         <v>137</v>
@@ -6474,12 +6484,12 @@
       <c r="P40" s="152"/>
       <c r="Q40" s="153"/>
     </row>
-    <row r="46" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:17" ht="16.2" thickBot="1">
       <c r="C46" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="47" spans="3:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:17" ht="16.2" thickBot="1">
       <c r="C47" s="85" t="s">
         <v>52</v>
       </c>
@@ -6499,7 +6509,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:17">
       <c r="C48" s="95" t="s">
         <v>127</v>
       </c>
@@ -6511,7 +6521,7 @@
       <c r="G48" s="96"/>
       <c r="H48" s="97"/>
     </row>
-    <row r="49" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:15" ht="16.2" thickBot="1">
       <c r="C49" s="94">
         <v>-5</v>
       </c>
@@ -6533,7 +6543,7 @@
         <v>2.6320620675006623E-3</v>
       </c>
     </row>
-    <row r="50" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:15" ht="16.2" thickBot="1">
       <c r="C50" s="68">
         <v>0</v>
       </c>
@@ -6565,7 +6575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:15">
       <c r="C51" s="68">
         <v>5</v>
       </c>
@@ -6600,7 +6610,7 @@
         <v>1.4834046925780164E-2</v>
       </c>
     </row>
-    <row r="52" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:15" ht="16.2" thickBot="1">
       <c r="C52" s="68">
         <v>10</v>
       </c>
@@ -6635,7 +6645,7 @@
         <v>3.8084209800004487E-3</v>
       </c>
     </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:15">
       <c r="C53" s="68">
         <v>15</v>
       </c>
@@ -6651,7 +6661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:15">
       <c r="C54" s="68">
         <v>20</v>
       </c>
@@ -6667,7 +6677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:15">
       <c r="C55" s="68">
         <v>25</v>
       </c>
@@ -6683,7 +6693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:15">
       <c r="C56" s="68">
         <v>30</v>
       </c>
@@ -6699,7 +6709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:15">
       <c r="C57" s="68">
         <v>35</v>
       </c>
@@ -6722,7 +6732,7 @@
       </c>
       <c r="K57" s="106"/>
     </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:15">
       <c r="C58" s="71">
         <v>40</v>
       </c>
@@ -6738,7 +6748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:15">
       <c r="C59" s="71">
         <v>45</v>
       </c>
@@ -6761,7 +6771,7 @@
       </c>
       <c r="J59" s="105"/>
     </row>
-    <row r="60" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:15" ht="16.2" thickBot="1">
       <c r="C60" s="69" t="s">
         <v>128</v>
       </c>
@@ -6780,7 +6790,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:15">
       <c r="L61" t="s">
         <v>151</v>
       </c>
@@ -6789,7 +6799,7 @@
         <v>0.99954895683835387</v>
       </c>
     </row>
-    <row r="62" spans="3:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:15">
       <c r="L62" t="s">
         <v>152</v>
       </c>
@@ -6798,7 +6808,7 @@
         <v>1.0001512578738871</v>
       </c>
     </row>
-    <row r="68" spans="2:25" s="113" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:25" s="113" customFormat="1">
       <c r="B68" s="117"/>
       <c r="D68" s="117"/>
       <c r="E68" s="117" t="s">
@@ -6813,8 +6823,8 @@
       <c r="X68" s="115"/>
       <c r="Y68" s="116"/>
     </row>
-    <row r="70" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:25" ht="16.2" thickBot="1"/>
+    <row r="71" spans="2:25" ht="16.2" thickBot="1">
       <c r="B71" s="85" t="s">
         <v>52</v>
       </c>
@@ -6842,7 +6852,7 @@
       <c r="N71" s="102"/>
       <c r="O71" s="102"/>
     </row>
-    <row r="72" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:25">
       <c r="B72" s="95" t="s">
         <v>127</v>
       </c>
@@ -6860,7 +6870,7 @@
       <c r="N72" s="100"/>
       <c r="O72" s="100"/>
     </row>
-    <row r="73" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:25" ht="16.2" thickBot="1">
       <c r="B73" s="94">
         <v>-5</v>
       </c>
@@ -6890,7 +6900,7 @@
       <c r="N73" s="104"/>
       <c r="O73" s="104"/>
     </row>
-    <row r="74" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:25" ht="16.2" thickBot="1">
       <c r="B74" s="68">
         <v>0</v>
       </c>
@@ -6918,7 +6928,7 @@
       </c>
       <c r="O74" s="99"/>
     </row>
-    <row r="75" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:25">
       <c r="B75" s="68">
         <v>5</v>
       </c>
@@ -6957,7 +6967,7 @@
       </c>
       <c r="O75" s="99"/>
     </row>
-    <row r="76" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:25" ht="16.2" thickBot="1">
       <c r="B76" s="68">
         <v>10</v>
       </c>
@@ -6996,7 +7006,7 @@
       </c>
       <c r="O76" s="99"/>
     </row>
-    <row r="77" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:25">
       <c r="B77" s="68"/>
       <c r="C77" s="161">
         <v>14.989699999999999</v>
@@ -7024,7 +7034,7 @@
       <c r="N77" s="99"/>
       <c r="O77" s="99"/>
     </row>
-    <row r="78" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:25">
       <c r="B78" s="68"/>
       <c r="C78" s="162">
         <v>19.995100000000001</v>
@@ -7052,7 +7062,7 @@
       <c r="N78" s="99"/>
       <c r="O78" s="99"/>
     </row>
-    <row r="79" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:25">
       <c r="B79" s="68"/>
       <c r="C79" s="161">
         <v>24.9998</v>
@@ -7080,7 +7090,7 @@
       <c r="N79" s="99"/>
       <c r="O79" s="99"/>
     </row>
-    <row r="80" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:25">
       <c r="B80" s="68"/>
       <c r="C80" s="161">
         <v>29.996500000000001</v>
@@ -7108,7 +7118,7 @@
       <c r="N80" s="99"/>
       <c r="O80" s="99"/>
     </row>
-    <row r="81" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:25">
       <c r="B81" s="68">
         <v>35</v>
       </c>
@@ -7138,7 +7148,7 @@
       <c r="N81" s="99"/>
       <c r="O81" s="99"/>
     </row>
-    <row r="82" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:25">
       <c r="B82" s="71"/>
       <c r="C82" s="163">
         <v>40.009500000000003</v>
@@ -7165,7 +7175,7 @@
       <c r="N82" s="99"/>
       <c r="O82" s="99"/>
     </row>
-    <row r="83" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:25">
       <c r="B83" s="71">
         <v>45</v>
       </c>
@@ -7195,7 +7205,7 @@
       <c r="N83" s="99"/>
       <c r="O83" s="99"/>
     </row>
-    <row r="84" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:25" ht="16.2" thickBot="1">
       <c r="B84" s="69" t="s">
         <v>128</v>
       </c>
@@ -7213,7 +7223,7 @@
       <c r="N84" s="99"/>
       <c r="O84" s="99"/>
     </row>
-    <row r="87" spans="2:25" s="113" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:25" s="113" customFormat="1">
       <c r="B87" s="117"/>
       <c r="D87" s="117"/>
       <c r="E87" s="117" t="s">
@@ -7228,8 +7238,8 @@
       <c r="X87" s="115"/>
       <c r="Y87" s="116"/>
     </row>
-    <row r="89" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:25" ht="16.2" thickBot="1"/>
+    <row r="90" spans="2:25" ht="16.2" thickBot="1">
       <c r="B90" s="85" t="s">
         <v>52</v>
       </c>
@@ -7257,7 +7267,7 @@
       <c r="N90" s="102"/>
       <c r="O90" s="102"/>
     </row>
-    <row r="91" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:25">
       <c r="B91" s="95" t="s">
         <v>127</v>
       </c>
@@ -7275,7 +7285,7 @@
       <c r="N91" s="100"/>
       <c r="O91" s="100"/>
     </row>
-    <row r="92" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:25" ht="16.2" thickBot="1">
       <c r="B92" s="94">
         <v>-5</v>
       </c>
@@ -7305,7 +7315,7 @@
       <c r="N92" s="104"/>
       <c r="O92" s="104"/>
     </row>
-    <row r="93" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:25" ht="16.2" thickBot="1">
       <c r="B93" s="68"/>
       <c r="C93" s="161"/>
       <c r="D93" s="159"/>
@@ -7327,7 +7337,7 @@
       </c>
       <c r="O93" s="99"/>
     </row>
-    <row r="94" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:25">
       <c r="B94" s="68">
         <v>5</v>
       </c>
@@ -7366,7 +7376,7 @@
       </c>
       <c r="O94" s="99"/>
     </row>
-    <row r="95" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:25" ht="16.2" thickBot="1">
       <c r="B95" s="68">
         <v>10</v>
       </c>
@@ -7405,7 +7415,7 @@
       </c>
       <c r="O95" s="99"/>
     </row>
-    <row r="96" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:25">
       <c r="B96" s="68"/>
       <c r="C96" s="161"/>
       <c r="D96" s="159"/>
@@ -7421,7 +7431,7 @@
       <c r="N96" s="99"/>
       <c r="O96" s="99"/>
     </row>
-    <row r="97" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:25">
       <c r="B97" s="68"/>
       <c r="C97" s="162"/>
       <c r="D97" s="159"/>
@@ -7437,7 +7447,7 @@
       <c r="N97" s="99"/>
       <c r="O97" s="99"/>
     </row>
-    <row r="98" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:25">
       <c r="B98" s="68"/>
       <c r="C98" s="161"/>
       <c r="D98" s="159"/>
@@ -7453,7 +7463,7 @@
       <c r="N98" s="99"/>
       <c r="O98" s="99"/>
     </row>
-    <row r="99" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:25">
       <c r="B99" s="68"/>
       <c r="C99" s="161"/>
       <c r="D99" s="161"/>
@@ -7469,7 +7479,7 @@
       <c r="N99" s="99"/>
       <c r="O99" s="99"/>
     </row>
-    <row r="100" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:25">
       <c r="B100" s="68">
         <v>35</v>
       </c>
@@ -7499,7 +7509,7 @@
       <c r="N100" s="99"/>
       <c r="O100" s="99"/>
     </row>
-    <row r="101" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:25">
       <c r="B101" s="71"/>
       <c r="C101" s="163"/>
       <c r="D101" s="163"/>
@@ -7514,7 +7524,7 @@
       <c r="N101" s="99"/>
       <c r="O101" s="99"/>
     </row>
-    <row r="102" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:25">
       <c r="B102" s="71">
         <v>45</v>
       </c>
@@ -7544,7 +7554,7 @@
       <c r="N102" s="99"/>
       <c r="O102" s="99"/>
     </row>
-    <row r="103" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:25" ht="16.2" thickBot="1">
       <c r="B103" s="69" t="s">
         <v>128</v>
       </c>
@@ -7562,7 +7572,7 @@
       <c r="N103" s="99"/>
       <c r="O103" s="99"/>
     </row>
-    <row r="109" spans="2:25" s="113" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:25" s="113" customFormat="1">
       <c r="B109" s="117"/>
       <c r="D109" s="117"/>
       <c r="E109" s="117" t="s">
@@ -7577,8 +7587,8 @@
       <c r="X109" s="115"/>
       <c r="Y109" s="116"/>
     </row>
-    <row r="111" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:25" ht="16.2" thickBot="1"/>
+    <row r="112" spans="2:25" ht="16.2" thickBot="1">
       <c r="B112" s="85" t="s">
         <v>52</v>
       </c>
@@ -7606,7 +7616,7 @@
       <c r="N112" s="102"/>
       <c r="O112" s="102"/>
     </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:15">
       <c r="B113" s="95" t="s">
         <v>127</v>
       </c>
@@ -7624,7 +7634,7 @@
       <c r="N113" s="100"/>
       <c r="O113" s="100"/>
     </row>
-    <row r="114" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:15" ht="16.2" thickBot="1">
       <c r="B114" s="94">
         <v>-5</v>
       </c>
@@ -7635,14 +7645,14 @@
         <v>-5.0163597009674197</v>
       </c>
       <c r="E114" s="160">
-        <f t="shared" ref="E114:E124" si="8">ABS(C114-D114)</f>
+        <f t="shared" ref="E114" si="8">ABS(C114-D114)</f>
         <v>1.4659700967420086E-2</v>
       </c>
       <c r="F114" s="159">
         <v>-5.0039296815569996</v>
       </c>
       <c r="G114" s="164">
-        <f t="shared" ref="G114:G124" si="9">ABS(C114-F114)</f>
+        <f t="shared" ref="G114" si="9">ABS(C114-F114)</f>
         <v>2.229681556999985E-3</v>
       </c>
       <c r="H114" s="98"/>
@@ -7654,7 +7664,7 @@
       <c r="N114" s="104"/>
       <c r="O114" s="104"/>
     </row>
-    <row r="115" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:15" ht="16.2" thickBot="1">
       <c r="B115" s="226">
         <v>0</v>
       </c>
@@ -7688,7 +7698,7 @@
       </c>
       <c r="O115" s="99"/>
     </row>
-    <row r="116" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:15">
       <c r="B116" s="68">
         <v>5</v>
       </c>
@@ -7699,14 +7709,14 @@
         <v>4.9833796713167704</v>
       </c>
       <c r="E116" s="160">
-        <f t="shared" ref="E116:E125" si="10">ABS(C116-D116)</f>
+        <f t="shared" ref="E116:E117" si="10">ABS(C116-D116)</f>
         <v>1.0879671316770256E-2</v>
       </c>
       <c r="F116" s="159">
         <v>4.9736924075495903</v>
       </c>
       <c r="G116" s="164">
-        <f t="shared" ref="G116:G125" si="11">ABS(C116-F116)</f>
+        <f t="shared" ref="G116:G117" si="11">ABS(C116-F116)</f>
         <v>1.1924075495901576E-3</v>
       </c>
       <c r="H116" s="98"/>
@@ -7727,7 +7737,7 @@
       </c>
       <c r="O116" s="99"/>
     </row>
-    <row r="117" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:15" ht="16.2" thickBot="1">
       <c r="B117" s="68">
         <v>10</v>
       </c>
@@ -7766,7 +7776,7 @@
       </c>
       <c r="O117" s="99"/>
     </row>
-    <row r="118" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:15">
       <c r="B118" s="68"/>
       <c r="C118" s="161"/>
       <c r="D118" s="159"/>
@@ -7782,7 +7792,7 @@
       <c r="N118" s="99"/>
       <c r="O118" s="99"/>
     </row>
-    <row r="119" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:15">
       <c r="B119" s="68"/>
       <c r="C119" s="162"/>
       <c r="D119" s="159"/>
@@ -7798,7 +7808,7 @@
       <c r="N119" s="99"/>
       <c r="O119" s="99"/>
     </row>
-    <row r="120" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:15">
       <c r="B120" s="68"/>
       <c r="C120" s="161"/>
       <c r="D120" s="159"/>
@@ -7814,7 +7824,7 @@
       <c r="N120" s="99"/>
       <c r="O120" s="99"/>
     </row>
-    <row r="121" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:15">
       <c r="B121" s="68"/>
       <c r="C121" s="161"/>
       <c r="D121" s="161"/>
@@ -7830,7 +7840,7 @@
       <c r="N121" s="99"/>
       <c r="O121" s="99"/>
     </row>
-    <row r="122" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:15">
       <c r="B122" s="68">
         <v>35</v>
       </c>
@@ -7841,14 +7851,14 @@
         <v>34.982637090717901</v>
       </c>
       <c r="E122" s="160">
-        <f t="shared" ref="E122:E125" si="12">ABS(C122-D122)</f>
+        <f t="shared" ref="E122" si="12">ABS(C122-D122)</f>
         <v>2.5370907179009805E-3</v>
       </c>
       <c r="F122" s="161">
         <v>34.976317935528002</v>
       </c>
       <c r="G122" s="164">
-        <f t="shared" ref="G122:G125" si="13">ABS(C122-F122)</f>
+        <f t="shared" ref="G122" si="13">ABS(C122-F122)</f>
         <v>3.7820644719985808E-3</v>
       </c>
       <c r="H122" s="98"/>
@@ -7860,7 +7870,7 @@
       <c r="N122" s="99"/>
       <c r="O122" s="99"/>
     </row>
-    <row r="123" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:15">
       <c r="B123" s="71"/>
       <c r="C123" s="163"/>
       <c r="D123" s="163"/>
@@ -7875,7 +7885,7 @@
       <c r="N123" s="99"/>
       <c r="O123" s="99"/>
     </row>
-    <row r="124" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:15">
       <c r="B124" s="71">
         <v>45</v>
       </c>
@@ -7886,14 +7896,14 @@
         <v>44.982387856876699</v>
       </c>
       <c r="E124" s="160">
-        <f t="shared" ref="E124:E125" si="14">ABS(C124-D124)</f>
+        <f t="shared" ref="E124" si="14">ABS(C124-D124)</f>
         <v>6.6121431232986083E-3</v>
       </c>
       <c r="F124" s="163">
         <v>44.990845211032799</v>
       </c>
       <c r="G124" s="164">
-        <f t="shared" ref="G124:G125" si="15">ABS(C124-F124)</f>
+        <f t="shared" ref="G124" si="15">ABS(C124-F124)</f>
         <v>1.8452110328013305E-3</v>
       </c>
       <c r="H124" s="98"/>
@@ -7905,7 +7915,7 @@
       <c r="N124" s="99"/>
       <c r="O124" s="99"/>
     </row>
-    <row r="125" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:15" ht="16.2" thickBot="1">
       <c r="B125" s="69" t="s">
         <v>128</v>
       </c>
@@ -7929,22 +7939,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F11942-15E9-084A-9037-102332C5B852}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.796875" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.796875" customWidth="1"/>
+    <col min="5" max="5" width="13.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:19">
       <c r="B2" s="89" t="s">
         <v>95</v>
       </c>
@@ -7958,7 +7968,7 @@
       <c r="H2" s="87"/>
       <c r="I2" s="87"/>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:19">
       <c r="B3" s="87" t="s">
         <v>82</v>
       </c>
@@ -7972,7 +7982,7 @@
       <c r="H3" s="87"/>
       <c r="I3" s="87"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:19">
       <c r="B4" s="87"/>
       <c r="C4" s="87"/>
       <c r="D4" s="87" t="s">
@@ -7984,7 +7994,7 @@
       <c r="H4" s="87"/>
       <c r="I4" s="87"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:19">
       <c r="B5" s="87"/>
       <c r="C5" s="87"/>
       <c r="D5" s="87"/>
@@ -7994,7 +8004,7 @@
       <c r="H5" s="87"/>
       <c r="I5" s="87"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19">
       <c r="B6" s="87" t="s">
         <v>161</v>
       </c>
@@ -8018,8 +8028,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" ht="16.2" thickBot="1"/>
+    <row r="9" spans="2:19" ht="16.2" thickBot="1">
       <c r="B9" s="87" t="s">
         <v>52</v>
       </c>
@@ -8042,7 +8052,7 @@
       <c r="R9" s="73"/>
       <c r="S9" s="74"/>
     </row>
-    <row r="10" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" ht="16.2" thickBot="1">
       <c r="B10" s="56" t="s">
         <v>95</v>
       </c>
@@ -8071,7 +8081,7 @@
       <c r="R10" s="75"/>
       <c r="S10" s="77"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:19">
       <c r="B11" s="167">
         <v>1</v>
       </c>
@@ -8099,7 +8109,7 @@
       <c r="R11" s="75"/>
       <c r="S11" s="77"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:19">
       <c r="B12" s="168">
         <v>2</v>
       </c>
@@ -8125,7 +8135,7 @@
       <c r="R12" s="75"/>
       <c r="S12" s="77"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:19">
       <c r="B13" s="168">
         <v>3</v>
       </c>
@@ -8147,7 +8157,7 @@
       <c r="R13" s="75"/>
       <c r="S13" s="77"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:19">
       <c r="B14" s="168">
         <v>4</v>
       </c>
@@ -8159,6 +8169,13 @@
       </c>
       <c r="E14" s="45">
         <v>-5.0109131500000004</v>
+      </c>
+      <c r="G14" s="253">
+        <f>MAX(D41,E41,E53,D53,D65,E65,E77,D77,D89,E89,D101,E101,E113,D113,E125,D125,D137,E137,E149,D149)</f>
+        <v>1.290800000003145E-3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>213</v>
       </c>
       <c r="L14" s="76"/>
       <c r="M14" s="75"/>
@@ -8169,7 +8186,7 @@
       <c r="R14" s="75"/>
       <c r="S14" s="77"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:19">
       <c r="B15" s="168">
         <v>5</v>
       </c>
@@ -8191,7 +8208,7 @@
       <c r="R15" s="75"/>
       <c r="S15" s="77"/>
     </row>
-    <row r="16" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" ht="16.2" thickBot="1">
       <c r="B16" s="169">
         <v>6</v>
       </c>
@@ -8213,7 +8230,7 @@
       <c r="R16" s="75"/>
       <c r="S16" s="77"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:19">
       <c r="B17" s="181" t="s">
         <v>163</v>
       </c>
@@ -8238,7 +8255,7 @@
       <c r="R17" s="75"/>
       <c r="S17" s="77"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:19">
       <c r="B18" s="168" t="s">
         <v>165</v>
       </c>
@@ -8263,7 +8280,7 @@
       <c r="R18" s="75"/>
       <c r="S18" s="77"/>
     </row>
-    <row r="19" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" ht="16.2" thickBot="1">
       <c r="B19" s="169" t="s">
         <v>164</v>
       </c>
@@ -8282,7 +8299,7 @@
       <c r="R19" s="75"/>
       <c r="S19" s="77"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:19">
       <c r="L20" s="76"/>
       <c r="M20" s="75"/>
       <c r="N20" s="75"/>
@@ -8292,7 +8309,7 @@
       <c r="R20" s="75"/>
       <c r="S20" s="77"/>
     </row>
-    <row r="21" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" ht="16.2" thickBot="1">
       <c r="B21" s="87" t="s">
         <v>52</v>
       </c>
@@ -8311,7 +8328,7 @@
       <c r="R21" s="75"/>
       <c r="S21" s="77"/>
     </row>
-    <row r="22" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" ht="16.2" thickBot="1">
       <c r="B22" s="56" t="s">
         <v>95</v>
       </c>
@@ -8333,7 +8350,7 @@
       <c r="R22" s="75"/>
       <c r="S22" s="77"/>
     </row>
-    <row r="23" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" ht="16.2" thickBot="1">
       <c r="B23" s="167">
         <v>1</v>
       </c>
@@ -8355,7 +8372,7 @@
       <c r="R23" s="79"/>
       <c r="S23" s="80"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:19">
       <c r="B24" s="168">
         <v>2</v>
       </c>
@@ -8369,7 +8386,7 @@
         <v>-4.9970701100000001</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:19">
       <c r="B25" s="168">
         <v>3</v>
       </c>
@@ -8383,7 +8400,7 @@
         <v>-4.99684755</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:19">
       <c r="B26" s="168">
         <v>4</v>
       </c>
@@ -8397,7 +8414,7 @@
         <v>-4.9967140099999998</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:19">
       <c r="B27" s="168">
         <v>5</v>
       </c>
@@ -8411,7 +8428,7 @@
         <v>-4.99653597</v>
       </c>
     </row>
-    <row r="28" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" ht="16.2" thickBot="1">
       <c r="B28" s="169">
         <v>6</v>
       </c>
@@ -8425,7 +8442,7 @@
         <v>-4.9964914599999997</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:19">
       <c r="B29" s="181" t="s">
         <v>163</v>
       </c>
@@ -8442,7 +8459,7 @@
         <v>5.7865000000045796E-4</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:19">
       <c r="B30" s="168" t="s">
         <v>165</v>
       </c>
@@ -8459,7 +8476,7 @@
         <v>2.1331544272908644E-4</v>
       </c>
     </row>
-    <row r="31" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" ht="16.2" thickBot="1">
       <c r="B31" s="169" t="s">
         <v>164</v>
       </c>
@@ -8470,7 +8487,7 @@
       <c r="D31" s="44"/>
       <c r="E31" s="42"/>
     </row>
-    <row r="33" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" ht="16.2" thickBot="1">
       <c r="B33" s="87" t="s">
         <v>52</v>
       </c>
@@ -8482,7 +8499,7 @@
       </c>
       <c r="J33" s="87"/>
     </row>
-    <row r="34" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" ht="16.2" thickBot="1">
       <c r="B34" s="56" t="s">
         <v>95</v>
       </c>
@@ -8497,7 +8514,7 @@
       </c>
       <c r="J34" s="88"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10">
       <c r="B35" s="167">
         <v>1</v>
       </c>
@@ -8512,7 +8529,7 @@
       </c>
       <c r="J35" s="87"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10">
       <c r="B36" s="168">
         <v>2</v>
       </c>
@@ -8527,7 +8544,7 @@
       </c>
       <c r="J36" s="87"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10">
       <c r="B37" s="168">
         <v>3</v>
       </c>
@@ -8542,7 +8559,7 @@
       </c>
       <c r="J37" s="87"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10">
       <c r="B38" s="168">
         <v>4</v>
       </c>
@@ -8557,7 +8574,7 @@
       </c>
       <c r="J38" s="87"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10">
       <c r="B39" s="168">
         <v>5</v>
       </c>
@@ -8572,7 +8589,7 @@
       </c>
       <c r="J39" s="87"/>
     </row>
-    <row r="40" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" ht="16.2" thickBot="1">
       <c r="B40" s="169">
         <v>6</v>
       </c>
@@ -8586,7 +8603,7 @@
         <v>-1.08583699E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10">
       <c r="B41" s="181" t="s">
         <v>163</v>
       </c>
@@ -8603,7 +8620,7 @@
         <v>8.4571659999999917E-4</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10">
       <c r="B42" s="168" t="s">
         <v>165</v>
       </c>
@@ -8620,7 +8637,7 @@
         <v>3.1432319015201309E-4</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" ht="16.2" thickBot="1">
       <c r="B43" s="169" t="s">
         <v>164</v>
       </c>
@@ -8631,7 +8648,7 @@
       <c r="D43" s="44"/>
       <c r="E43" s="42"/>
     </row>
-    <row r="45" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" ht="16.2" thickBot="1">
       <c r="B45" s="87" t="s">
         <v>52</v>
       </c>
@@ -8642,7 +8659,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" ht="16.2" thickBot="1">
       <c r="B46" s="56" t="s">
         <v>95</v>
       </c>
@@ -8656,7 +8673,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10">
       <c r="B47" s="167">
         <v>1</v>
       </c>
@@ -8670,7 +8687,7 @@
         <v>7.0797249199999997E-3</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10">
       <c r="B48" s="168">
         <v>2</v>
       </c>
@@ -8684,7 +8701,7 @@
         <v>5.8779170699999996E-3</v>
       </c>
     </row>
-    <row r="49" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:24">
       <c r="B49" s="168">
         <v>3</v>
       </c>
@@ -8698,7 +8715,7 @@
         <v>6.3675424900000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:24">
       <c r="B50" s="168">
         <v>4</v>
       </c>
@@ -8712,7 +8729,7 @@
         <v>6.4120538899999999E-3</v>
       </c>
     </row>
-    <row r="51" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:24">
       <c r="B51" s="168">
         <v>5</v>
       </c>
@@ -8726,7 +8743,7 @@
         <v>6.5900995E-3</v>
       </c>
     </row>
-    <row r="52" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:24" ht="16.2" thickBot="1">
       <c r="B52" s="169">
         <v>6</v>
       </c>
@@ -8740,7 +8757,7 @@
         <v>6.7681451100000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:24">
       <c r="B53" s="181" t="s">
         <v>163</v>
       </c>
@@ -8757,7 +8774,7 @@
         <v>1.2018078500000001E-3</v>
       </c>
     </row>
-    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:24">
       <c r="B54" s="168" t="s">
         <v>165</v>
       </c>
@@ -8774,7 +8791,7 @@
         <v>4.0665658359148019E-4</v>
       </c>
     </row>
-    <row r="55" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:24" ht="16.2" thickBot="1">
       <c r="B55" s="169" t="s">
         <v>164</v>
       </c>
@@ -8785,7 +8802,7 @@
       <c r="D55" s="44"/>
       <c r="E55" s="42"/>
     </row>
-    <row r="57" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:24" ht="16.2" thickBot="1">
       <c r="B57" s="87" t="s">
         <v>52</v>
       </c>
@@ -8796,7 +8813,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:24" ht="16.2" thickBot="1">
       <c r="B58" s="56" t="s">
         <v>95</v>
       </c>
@@ -8815,7 +8832,7 @@
       <c r="W58" s="86"/>
       <c r="X58" s="86"/>
     </row>
-    <row r="59" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:24">
       <c r="B59" s="167">
         <v>1</v>
       </c>
@@ -8834,7 +8851,7 @@
       <c r="W59" s="86"/>
       <c r="X59" s="86"/>
     </row>
-    <row r="60" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:24">
       <c r="B60" s="168">
         <v>2</v>
       </c>
@@ -8853,7 +8870,7 @@
       <c r="W60" s="86"/>
       <c r="X60" s="86"/>
     </row>
-    <row r="61" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:24">
       <c r="B61" s="168">
         <v>3</v>
       </c>
@@ -8872,7 +8889,7 @@
       <c r="W61" s="86"/>
       <c r="X61" s="86"/>
     </row>
-    <row r="62" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:24">
       <c r="B62" s="168">
         <v>4</v>
       </c>
@@ -8891,7 +8908,7 @@
       <c r="W62" s="86"/>
       <c r="X62" s="86"/>
     </row>
-    <row r="63" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:24">
       <c r="B63" s="168">
         <v>5</v>
       </c>
@@ -8910,7 +8927,7 @@
       <c r="W63" s="86"/>
       <c r="X63" s="86"/>
     </row>
-    <row r="64" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:24" ht="16.2" thickBot="1">
       <c r="B64" s="169">
         <v>6</v>
       </c>
@@ -8929,7 +8946,7 @@
       <c r="W64" s="86"/>
       <c r="X64" s="86"/>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:17">
       <c r="B65" s="181" t="s">
         <v>163</v>
       </c>
@@ -8946,7 +8963,7 @@
         <v>1.0682800000001436E-3</v>
       </c>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:17">
       <c r="B66" s="168" t="s">
         <v>165</v>
       </c>
@@ -8963,7 +8980,7 @@
         <v>4.0274203454598444E-4</v>
       </c>
     </row>
-    <row r="67" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:17" ht="16.2" thickBot="1">
       <c r="B67" s="169" t="s">
         <v>164</v>
       </c>
@@ -8974,7 +8991,7 @@
       <c r="D67" s="44"/>
       <c r="E67" s="42"/>
     </row>
-    <row r="69" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:17" ht="16.2" thickBot="1">
       <c r="B69" s="87" t="s">
         <v>52</v>
       </c>
@@ -8985,7 +9002,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:17" ht="16.2" thickBot="1">
       <c r="B70" s="56" t="s">
         <v>95</v>
       </c>
@@ -8999,7 +9016,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:17">
       <c r="B71" s="167">
         <v>1</v>
       </c>
@@ -9013,7 +9030,7 @@
         <v>10.01524586</v>
       </c>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:17">
       <c r="B72" s="168">
         <v>2</v>
       </c>
@@ -9027,7 +9044,7 @@
         <v>10.014355630000001</v>
       </c>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:17">
       <c r="B73" s="168">
         <v>3</v>
       </c>
@@ -9041,7 +9058,7 @@
         <v>10.014667210000001</v>
       </c>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:17">
       <c r="B74" s="168">
         <v>4</v>
       </c>
@@ -9055,7 +9072,7 @@
         <v>10.01484526</v>
       </c>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:17">
       <c r="B75" s="168">
         <v>5</v>
       </c>
@@ -9069,7 +9086,7 @@
         <v>10.015023299999999</v>
       </c>
     </row>
-    <row r="76" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:17" ht="16.2" thickBot="1">
       <c r="B76" s="169">
         <v>6</v>
       </c>
@@ -9083,7 +9100,7 @@
         <v>10.01520135</v>
       </c>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:17">
       <c r="B77" s="181" t="s">
         <v>163</v>
       </c>
@@ -9101,7 +9118,7 @@
       </c>
       <c r="Q77" s="89"/>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:17">
       <c r="B78" s="168" t="s">
         <v>165</v>
       </c>
@@ -9119,7 +9136,7 @@
       </c>
       <c r="Q78" s="89"/>
     </row>
-    <row r="79" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:17" ht="16.2" thickBot="1">
       <c r="B79" s="169" t="s">
         <v>164</v>
       </c>
@@ -9131,10 +9148,10 @@
       <c r="E79" s="42"/>
       <c r="Q79" s="89"/>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:17">
       <c r="Q80" s="89"/>
     </row>
-    <row r="81" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:17" ht="16.2" thickBot="1">
       <c r="B81" s="89" t="s">
         <v>52</v>
       </c>
@@ -9146,7 +9163,7 @@
       </c>
       <c r="Q81" s="89"/>
     </row>
-    <row r="82" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:17" ht="16.2" thickBot="1">
       <c r="B82" s="56" t="s">
         <v>95</v>
       </c>
@@ -9161,7 +9178,7 @@
       </c>
       <c r="Q82" s="89"/>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:17">
       <c r="B83" s="167">
         <v>1</v>
       </c>
@@ -9176,7 +9193,7 @@
       </c>
       <c r="Q83" s="89"/>
     </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:17">
       <c r="B84" s="168">
         <v>2</v>
       </c>
@@ -9191,7 +9208,7 @@
       </c>
       <c r="Q84" s="89"/>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:17">
       <c r="B85" s="168">
         <v>3</v>
       </c>
@@ -9205,7 +9222,7 @@
         <v>19.998441100000001</v>
       </c>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:17">
       <c r="B86" s="168">
         <v>4</v>
       </c>
@@ -9219,7 +9236,7 @@
         <v>19.998263049999998</v>
       </c>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:17">
       <c r="B87" s="168">
         <v>5</v>
       </c>
@@ -9233,7 +9250,7 @@
         <v>19.998040499999998</v>
       </c>
     </row>
-    <row r="88" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:17" ht="16.2" thickBot="1">
       <c r="B88" s="169">
         <v>6</v>
       </c>
@@ -9247,7 +9264,7 @@
         <v>19.997906960000002</v>
       </c>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:17">
       <c r="B89" s="181" t="s">
         <v>163</v>
       </c>
@@ -9264,7 +9281,7 @@
         <v>1.2018099999977494E-3</v>
       </c>
     </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:17">
       <c r="B90" s="168" t="s">
         <v>165</v>
       </c>
@@ -9281,7 +9298,7 @@
         <v>4.3429956286692947E-4</v>
       </c>
     </row>
-    <row r="91" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:17" ht="16.2" thickBot="1">
       <c r="B91" s="169" t="s">
         <v>164</v>
       </c>
@@ -9292,7 +9309,7 @@
       <c r="D91" s="44"/>
       <c r="E91" s="42"/>
     </row>
-    <row r="93" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:17" ht="16.2" thickBot="1">
       <c r="B93" s="89" t="s">
         <v>52</v>
       </c>
@@ -9303,7 +9320,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:17" ht="16.2" thickBot="1">
       <c r="B94" s="56" t="s">
         <v>95</v>
       </c>
@@ -9317,7 +9334,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:17">
       <c r="B95" s="167">
         <v>1</v>
       </c>
@@ -9331,7 +9348,7 @@
         <v>20.012996300000001</v>
       </c>
     </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:17">
       <c r="B96" s="168">
         <v>2</v>
       </c>
@@ -9345,7 +9362,7 @@
         <v>20.013218800000001</v>
       </c>
     </row>
-    <row r="97" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:24">
       <c r="B97" s="168">
         <v>3</v>
       </c>
@@ -9359,7 +9376,7 @@
         <v>20.0133969</v>
       </c>
     </row>
-    <row r="98" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:24">
       <c r="B98" s="168">
         <v>4</v>
       </c>
@@ -9373,7 +9390,7 @@
         <v>20.013574899999998</v>
       </c>
     </row>
-    <row r="99" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:24">
       <c r="B99" s="168">
         <v>5</v>
       </c>
@@ -9387,7 +9404,7 @@
         <v>20.013753000000001</v>
       </c>
     </row>
-    <row r="100" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:24" ht="16.2" thickBot="1">
       <c r="B100" s="169">
         <v>6</v>
       </c>
@@ -9401,7 +9418,7 @@
         <v>20.013040799999999</v>
       </c>
     </row>
-    <row r="101" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:24">
       <c r="B101" s="181" t="s">
         <v>163</v>
       </c>
@@ -9418,7 +9435,7 @@
         <v>7.5670000000016557E-4</v>
       </c>
     </row>
-    <row r="102" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:24">
       <c r="B102" s="168" t="s">
         <v>165</v>
       </c>
@@ -9435,7 +9452,7 @@
         <v>3.0024600191621165E-4</v>
       </c>
     </row>
-    <row r="103" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:24" ht="16.2" thickBot="1">
       <c r="B103" s="169" t="s">
         <v>164</v>
       </c>
@@ -9446,7 +9463,7 @@
       <c r="D103" s="44"/>
       <c r="E103" s="42"/>
     </row>
-    <row r="105" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:24" ht="16.2" thickBot="1">
       <c r="B105" s="89" t="s">
         <v>52</v>
       </c>
@@ -9457,7 +9474,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="106" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:24" ht="16.2" thickBot="1">
       <c r="B106" s="56" t="s">
         <v>95</v>
       </c>
@@ -9479,7 +9496,7 @@
       <c r="W106" s="86"/>
       <c r="X106" s="86"/>
     </row>
-    <row r="107" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:24">
       <c r="B107" s="167">
         <v>1</v>
       </c>
@@ -9501,7 +9518,7 @@
       <c r="W107" s="86"/>
       <c r="X107" s="86"/>
     </row>
-    <row r="108" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:24">
       <c r="B108" s="168">
         <v>2</v>
       </c>
@@ -9523,7 +9540,7 @@
       <c r="W108" s="86"/>
       <c r="X108" s="86"/>
     </row>
-    <row r="109" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:24">
       <c r="B109" s="168">
         <v>3</v>
       </c>
@@ -9545,7 +9562,7 @@
       <c r="W109" s="86"/>
       <c r="X109" s="86"/>
     </row>
-    <row r="110" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:24">
       <c r="B110" s="168">
         <v>4</v>
       </c>
@@ -9567,7 +9584,7 @@
       <c r="W110" s="86"/>
       <c r="X110" s="86"/>
     </row>
-    <row r="111" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:24">
       <c r="B111" s="168">
         <v>5</v>
       </c>
@@ -9589,7 +9606,7 @@
       <c r="W111" s="86"/>
       <c r="X111" s="86"/>
     </row>
-    <row r="112" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:24" ht="16.2" thickBot="1">
       <c r="B112" s="169">
         <v>6</v>
       </c>
@@ -9611,7 +9628,7 @@
       <c r="W112" s="86"/>
       <c r="X112" s="86"/>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:11">
       <c r="B113" s="181" t="s">
         <v>163</v>
       </c>
@@ -9628,7 +9645,7 @@
         <v>5.7864999999779343E-4</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:11">
       <c r="B114" s="168" t="s">
         <v>165</v>
       </c>
@@ -9645,7 +9662,7 @@
         <v>2.1760741556723227E-4</v>
       </c>
     </row>
-    <row r="115" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:11" ht="16.2" thickBot="1">
       <c r="B115" s="169" t="s">
         <v>164</v>
       </c>
@@ -9656,7 +9673,7 @@
       <c r="D115" s="44"/>
       <c r="E115" s="42"/>
     </row>
-    <row r="117" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:11" ht="16.2" thickBot="1">
       <c r="B117" s="89" t="s">
         <v>52</v>
       </c>
@@ -9667,7 +9684,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="118" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:11" ht="16.2" thickBot="1">
       <c r="B118" s="56" t="s">
         <v>95</v>
       </c>
@@ -9681,7 +9698,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:11">
       <c r="B119" s="167">
         <v>1</v>
       </c>
@@ -9695,7 +9712,7 @@
         <v>30.016310699999998</v>
       </c>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:11">
       <c r="B120" s="168">
         <v>2</v>
       </c>
@@ -9709,7 +9726,7 @@
         <v>30.016666799999999</v>
       </c>
     </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:11">
       <c r="B121" s="168">
         <v>3</v>
       </c>
@@ -9723,7 +9740,7 @@
         <v>30.016889299999999</v>
       </c>
     </row>
-    <row r="122" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:11">
       <c r="B122" s="168">
         <v>4</v>
       </c>
@@ -9737,7 +9754,7 @@
         <v>30.017200899999999</v>
       </c>
     </row>
-    <row r="123" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:11">
       <c r="B123" s="168">
         <v>5</v>
       </c>
@@ -9751,7 +9768,7 @@
         <v>30.017378999999998</v>
       </c>
     </row>
-    <row r="124" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:11" ht="16.2" thickBot="1">
       <c r="B124" s="169">
         <v>6</v>
       </c>
@@ -9766,7 +9783,7 @@
       </c>
       <c r="K124" s="89"/>
     </row>
-    <row r="125" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:11">
       <c r="B125" s="181" t="s">
         <v>163</v>
       </c>
@@ -9784,7 +9801,7 @@
       </c>
       <c r="K125" s="89"/>
     </row>
-    <row r="126" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:11">
       <c r="B126" s="168" t="s">
         <v>165</v>
       </c>
@@ -9802,7 +9819,7 @@
       </c>
       <c r="K126" s="89"/>
     </row>
-    <row r="127" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:11" ht="16.2" thickBot="1">
       <c r="B127" s="169" t="s">
         <v>164</v>
       </c>
@@ -9814,10 +9831,10 @@
       <c r="E127" s="42"/>
       <c r="K127" s="89"/>
     </row>
-    <row r="128" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:11">
       <c r="K128" s="89"/>
     </row>
-    <row r="129" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:11" ht="16.2" thickBot="1">
       <c r="B129" s="89" t="s">
         <v>52</v>
       </c>
@@ -9829,7 +9846,7 @@
       </c>
       <c r="K129" s="89"/>
     </row>
-    <row r="130" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:11" ht="16.2" thickBot="1">
       <c r="B130" s="56" t="s">
         <v>95</v>
       </c>
@@ -9844,7 +9861,7 @@
       </c>
       <c r="K130" s="89"/>
     </row>
-    <row r="131" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:11">
       <c r="B131" s="167">
         <v>1</v>
       </c>
@@ -9859,7 +9876,7 @@
       </c>
       <c r="K131" s="89"/>
     </row>
-    <row r="132" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:11">
       <c r="B132" s="168">
         <v>2</v>
       </c>
@@ -9873,7 +9890,7 @@
         <v>40.006672299999998</v>
       </c>
     </row>
-    <row r="133" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:11">
       <c r="B133" s="168">
         <v>3</v>
       </c>
@@ -9887,7 +9904,7 @@
         <v>40.006494199999999</v>
       </c>
     </row>
-    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:11">
       <c r="B134" s="168">
         <v>4</v>
       </c>
@@ -9901,7 +9918,7 @@
         <v>40.006316200000001</v>
       </c>
     </row>
-    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:11">
       <c r="B135" s="168">
         <v>5</v>
       </c>
@@ -9915,7 +9932,7 @@
         <v>40.0060936</v>
       </c>
     </row>
-    <row r="136" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:11" ht="16.2" thickBot="1">
       <c r="B136" s="169">
         <v>6</v>
       </c>
@@ -9929,7 +9946,7 @@
         <v>40.005960100000003</v>
       </c>
     </row>
-    <row r="137" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:11">
       <c r="B137" s="181" t="s">
         <v>163</v>
       </c>
@@ -9946,7 +9963,7 @@
         <v>7.5669999999661286E-4</v>
       </c>
     </row>
-    <row r="138" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:11">
       <c r="B138" s="168" t="s">
         <v>165</v>
       </c>
@@ -9963,7 +9980,7 @@
         <v>3.0407094566738731E-4</v>
       </c>
     </row>
-    <row r="139" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:11" ht="16.2" thickBot="1">
       <c r="B139" s="169" t="s">
         <v>164</v>
       </c>
@@ -9974,7 +9991,7 @@
       <c r="D139" s="44"/>
       <c r="E139" s="42"/>
     </row>
-    <row r="141" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:11" ht="16.2" thickBot="1">
       <c r="B141" s="89" t="s">
         <v>52</v>
       </c>
@@ -9985,7 +10002,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="142" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:11" ht="16.2" thickBot="1">
       <c r="B142" s="56" t="s">
         <v>95</v>
       </c>
@@ -9999,7 +10016,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:11">
       <c r="B143" s="167">
         <v>1</v>
       </c>
@@ -10013,7 +10030,7 @@
         <v>40.019313539999999</v>
       </c>
     </row>
-    <row r="144" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:11">
       <c r="B144" s="168">
         <v>2</v>
       </c>
@@ -10027,7 +10044,7 @@
         <v>40.01949158</v>
       </c>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:5">
       <c r="B145" s="168">
         <v>3</v>
       </c>
@@ -10041,7 +10058,7 @@
         <v>40.019669630000003</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:5">
       <c r="B146" s="168">
         <v>4</v>
       </c>
@@ -10055,7 +10072,7 @@
         <v>40.019847669999997</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:5">
       <c r="B147" s="168">
         <v>5</v>
       </c>
@@ -10069,7 +10086,7 @@
         <v>40.019981209999997</v>
       </c>
     </row>
-    <row r="148" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:5" ht="16.2" thickBot="1">
       <c r="B148" s="169">
         <v>6</v>
       </c>
@@ -10083,7 +10100,7 @@
         <v>40.020159249999999</v>
       </c>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:5">
       <c r="B149" s="181" t="s">
         <v>163</v>
       </c>
@@ -10100,7 +10117,7 @@
         <v>8.4571000000011054E-4</v>
       </c>
     </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:5">
       <c r="B150" s="168" t="s">
         <v>165</v>
       </c>
@@ -10117,7 +10134,7 @@
         <v>3.1432180049466578E-4</v>
       </c>
     </row>
-    <row r="151" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:5" ht="16.2" thickBot="1">
       <c r="B151" s="169" t="s">
         <v>164</v>
       </c>

</xml_diff>